<commit_message>
[MS-OXCRPC]: Update capture code for latest RS
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCRPC/MS-OXCRPC_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCRPC/MS-OXCRPC_RequirementSpecification.xlsx
@@ -8272,9 +8272,6 @@
     <t>[In Client Versions] [Client version "12.00.0000.000"] The client supports topologies that do not have public folders available.</t>
   </si>
   <si>
-    <t>[In Client Versions] [Client version "12.00.0000.000"] For client versions earlier than 12.00.0000.000, the server MUST fail the EcDoConnectEx method call with ecClientVerDisallowed if the EcDoConnectEx method parameter flag 0x00008000 is not passed in the ulFlags parameter.</t>
-  </si>
-  <si>
     <t>[In Client Versions] [Client version "12.00.0000.000"] For client versions earlier than 12.00.0000.000, the server MUST not fail the EcDoConnectEx method call with ecClientVerDisallowed if the EcDoConnectEx method parameter flag 0x00008000 is passed in the ulFlags parameter.</t>
   </si>
   <si>
@@ -8752,9 +8749,6 @@
     <t>[In Appendix B: Product Behavior] Implementation does return the AUX_EXORGINFO block in the rgbAuxOut buffer on the EcDoConnectEx call. (Microsoft Exchange Server 2007 and above follow this behavior.)</t>
   </si>
   <si>
-    <t>[In Appendix B: Product Behavior] Implementation does fail with error code ecRpcFailed (0x80040115) if the value in pcbOut on input is less than 0x00000008. (Microsoft Exchange Server 2010 and above follow this behavior).</t>
-  </si>
-  <si>
     <t>[In Appendix B: Product Behavior] Implementation does fail with ecRpcFormat (0x000004B6) if the output buffer is less than 0x00008007. (Microsoft Exchange Server 2007 follows this behavior).</t>
   </si>
   <si>
@@ -9313,9 +9307,6 @@
     <t>[In Appendix B: Product Behavior] Implementation does fail with error code ecRpcFormat if the request buffer is larger than 0x00008007 bytes in size. &lt;19&gt; Section 3.1.4.2: Exchange 2007 and 2010 will fail with error code ecRpcFormat (0x000004B6) if the request buffer is larger than 0x00008007 bytes in size.</t>
   </si>
   <si>
-    <t>[In Appendix B: Product Behavior] Implementation does fail with the RPC status code of RPC_X_BAD_STUB_DATA (0x000006F7) if the request buffer is larger than 0x00040000 bytes in size. (Microsoft Exchange Server 2013 and above follow this behavior.)</t>
-  </si>
-  <si>
     <t>MS-OXCRPC_R2001</t>
   </si>
   <si>
@@ -9533,6 +9524,15 @@
   </si>
   <si>
     <t>[In EcDoConnectEx Method (Opnum 10)] [ulConMod] The server determines which public folder replica to use when accessing public folder information when more than one replica of a folder exists.</t>
+  </si>
+  <si>
+    <t>[In Client Versions] [Client version "12.00.0000.000"] For client versions earlier than 12.00.0000.000, the server MUST fail the EcDoConnectEx method call with ecClientVerDisallowed when no public folders are configured within the messaging system if the EcDoConnectEx method parameter flag 0x00008000 is not passed in the ulFlags parameter.</t>
+  </si>
+  <si>
+    <t>[In Appendix B: Product Behavior] Implementation does fail with error code ecRpcFailed (0x80040115) if the value in pcbOut on input is less than 0x00000008. (Microsoft Exchange Server 2010 follows this behavior).</t>
+  </si>
+  <si>
+    <t>[In Appendix B: Product Behavior] Implementation does fail with the RPC status code of RPC_X_BAD_STUB_DATA (0x000006F7) if the request buffer is larger than 0x00040000 bytes in size. (Microsoft Exchange Server 2010 Service Pack 2 (SP2) and above follow this behavior.)</t>
   </si>
 </sst>
 </file>
@@ -10717,7 +10717,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>2936</v>
+        <v>2934</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>27</v>
@@ -10727,7 +10727,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="6" t="s">
-        <v>2937</v>
+        <v>2935</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -10741,7 +10741,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>2942</v>
+        <v>2940</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>26</v>
@@ -11050,7 +11050,7 @@
         <v>17</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>2864</v>
+        <v>2862</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="23" customFormat="1" ht="30">
@@ -11352,7 +11352,7 @@
         <v>17</v>
       </c>
       <c r="I32" s="24" t="s">
-        <v>2865</v>
+        <v>2863</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="23" customFormat="1" ht="30">
@@ -11504,7 +11504,7 @@
         <v>17</v>
       </c>
       <c r="I38" s="31" t="s">
-        <v>2866</v>
+        <v>2864</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -11781,7 +11781,7 @@
         <v>17</v>
       </c>
       <c r="I49" s="31" t="s">
-        <v>2867</v>
+        <v>2865</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="30">
@@ -11808,7 +11808,7 @@
         <v>17</v>
       </c>
       <c r="I50" s="31" t="s">
-        <v>2868</v>
+        <v>2866</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="30">
@@ -11835,7 +11835,7 @@
         <v>17</v>
       </c>
       <c r="I51" s="31" t="s">
-        <v>2868</v>
+        <v>2866</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="30">
@@ -11862,7 +11862,7 @@
         <v>17</v>
       </c>
       <c r="I52" s="31" t="s">
-        <v>2868</v>
+        <v>2866</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="30">
@@ -11964,7 +11964,7 @@
         <v>17</v>
       </c>
       <c r="I56" s="31" t="s">
-        <v>2869</v>
+        <v>2867</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="60">
@@ -11991,7 +11991,7 @@
         <v>17</v>
       </c>
       <c r="I57" s="31" t="s">
-        <v>2870</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="30">
@@ -12018,7 +12018,7 @@
         <v>17</v>
       </c>
       <c r="I58" s="31" t="s">
-        <v>2871</v>
+        <v>2869</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="60">
@@ -12045,7 +12045,7 @@
         <v>17</v>
       </c>
       <c r="I59" s="31" t="s">
-        <v>2870</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="60">
@@ -12072,7 +12072,7 @@
         <v>17</v>
       </c>
       <c r="I60" s="31" t="s">
-        <v>2870</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="60">
@@ -12099,7 +12099,7 @@
         <v>17</v>
       </c>
       <c r="I61" s="31" t="s">
-        <v>2870</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="60">
@@ -12126,7 +12126,7 @@
         <v>17</v>
       </c>
       <c r="I62" s="31" t="s">
-        <v>2870</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="45">
@@ -12803,7 +12803,7 @@
         <v>17</v>
       </c>
       <c r="I89" s="31" t="s">
-        <v>2872</v>
+        <v>2870</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="45">
@@ -12830,7 +12830,7 @@
         <v>17</v>
       </c>
       <c r="I90" s="31" t="s">
-        <v>2873</v>
+        <v>2871</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="45">
@@ -12882,7 +12882,7 @@
         <v>17</v>
       </c>
       <c r="I92" s="31" t="s">
-        <v>2874</v>
+        <v>2872</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="45">
@@ -12934,7 +12934,7 @@
         <v>17</v>
       </c>
       <c r="I94" s="31" t="s">
-        <v>2875</v>
+        <v>2873</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="45">
@@ -17545,7 +17545,7 @@
         <v>1493</v>
       </c>
       <c r="C279" s="31" t="s">
-        <v>2943</v>
+        <v>2941</v>
       </c>
       <c r="D279" s="29"/>
       <c r="E279" s="29" t="s">
@@ -17645,7 +17645,7 @@
         <v>1493</v>
       </c>
       <c r="C283" s="31" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
       <c r="D283" s="29"/>
       <c r="E283" s="29" t="s">
@@ -17736,7 +17736,7 @@
         <v>17</v>
       </c>
       <c r="I286" s="31" t="s">
-        <v>2873</v>
+        <v>2871</v>
       </c>
     </row>
     <row r="287" spans="1:9" ht="30">
@@ -17788,7 +17788,7 @@
         <v>17</v>
       </c>
       <c r="I288" s="31" t="s">
-        <v>2873</v>
+        <v>2871</v>
       </c>
     </row>
     <row r="289" spans="1:9" ht="45">
@@ -17949,7 +17949,7 @@
         <v>1496</v>
       </c>
       <c r="C295" s="31" t="s">
-        <v>2945</v>
+        <v>2943</v>
       </c>
       <c r="D295" s="29"/>
       <c r="E295" s="29" t="s">
@@ -17974,7 +17974,7 @@
         <v>1496</v>
       </c>
       <c r="C296" s="31" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="D296" s="29"/>
       <c r="E296" s="29" t="s">
@@ -17990,7 +17990,7 @@
         <v>17</v>
       </c>
       <c r="I296" s="31" t="s">
-        <v>2876</v>
+        <v>2874</v>
       </c>
     </row>
     <row r="297" spans="1:9" ht="45">
@@ -18092,7 +18092,7 @@
         <v>17</v>
       </c>
       <c r="I300" s="31" t="s">
-        <v>2877</v>
+        <v>2875</v>
       </c>
     </row>
     <row r="301" spans="1:9" ht="45">
@@ -19144,7 +19144,7 @@
         <v>17</v>
       </c>
       <c r="I342" s="31" t="s">
-        <v>2878</v>
+        <v>2876</v>
       </c>
     </row>
     <row r="343" spans="1:9" ht="30">
@@ -20005,7 +20005,7 @@
         <v>1504</v>
       </c>
       <c r="C377" s="31" t="s">
-        <v>2947</v>
+        <v>2945</v>
       </c>
       <c r="D377" s="29"/>
       <c r="E377" s="29" t="s">
@@ -20071,7 +20071,7 @@
         <v>17</v>
       </c>
       <c r="I379" s="31" t="s">
-        <v>2879</v>
+        <v>2877</v>
       </c>
     </row>
     <row r="380" spans="1:9" ht="45">
@@ -20223,7 +20223,7 @@
         <v>17</v>
       </c>
       <c r="I385" s="31" t="s">
-        <v>2880</v>
+        <v>2878</v>
       </c>
     </row>
     <row r="386" spans="1:9" ht="30">
@@ -20234,7 +20234,7 @@
         <v>1505</v>
       </c>
       <c r="C386" s="31" t="s">
-        <v>2948</v>
+        <v>2946</v>
       </c>
       <c r="D386" s="29"/>
       <c r="E386" s="29" t="s">
@@ -20259,7 +20259,7 @@
         <v>1505</v>
       </c>
       <c r="C387" s="31" t="s">
-        <v>2949</v>
+        <v>2947</v>
       </c>
       <c r="D387" s="29"/>
       <c r="E387" s="29" t="s">
@@ -20284,7 +20284,7 @@
         <v>1505</v>
       </c>
       <c r="C388" s="31" t="s">
-        <v>2950</v>
+        <v>2948</v>
       </c>
       <c r="D388" s="29"/>
       <c r="E388" s="29" t="s">
@@ -20350,7 +20350,7 @@
         <v>17</v>
       </c>
       <c r="I390" s="31" t="s">
-        <v>2881</v>
+        <v>2879</v>
       </c>
     </row>
     <row r="391" spans="1:9" ht="30">
@@ -20436,7 +20436,7 @@
         <v>1505</v>
       </c>
       <c r="C394" s="31" t="s">
-        <v>2951</v>
+        <v>2949</v>
       </c>
       <c r="D394" s="29"/>
       <c r="E394" s="29" t="s">
@@ -20486,7 +20486,7 @@
         <v>1505</v>
       </c>
       <c r="C396" s="31" t="s">
-        <v>2952</v>
+        <v>2950</v>
       </c>
       <c r="D396" s="29"/>
       <c r="E396" s="29" t="s">
@@ -20552,7 +20552,7 @@
         <v>17</v>
       </c>
       <c r="I398" s="31" t="s">
-        <v>2882</v>
+        <v>2880</v>
       </c>
     </row>
     <row r="399" spans="1:9" ht="30">
@@ -20579,7 +20579,7 @@
         <v>17</v>
       </c>
       <c r="I399" s="31" t="s">
-        <v>2883</v>
+        <v>2881</v>
       </c>
     </row>
     <row r="400" spans="1:9" ht="45">
@@ -20615,7 +20615,7 @@
         <v>1505</v>
       </c>
       <c r="C401" s="31" t="s">
-        <v>2953</v>
+        <v>2951</v>
       </c>
       <c r="D401" s="29"/>
       <c r="E401" s="29" t="s">
@@ -20681,7 +20681,7 @@
         <v>17</v>
       </c>
       <c r="I403" s="31" t="s">
-        <v>2884</v>
+        <v>2882</v>
       </c>
     </row>
     <row r="404" spans="1:9" ht="30">
@@ -20717,7 +20717,7 @@
         <v>1505</v>
       </c>
       <c r="C405" s="31" t="s">
-        <v>2954</v>
+        <v>2952</v>
       </c>
       <c r="D405" s="29"/>
       <c r="E405" s="29" t="s">
@@ -20767,7 +20767,7 @@
         <v>1505</v>
       </c>
       <c r="C407" s="31" t="s">
-        <v>2955</v>
+        <v>2953</v>
       </c>
       <c r="D407" s="29"/>
       <c r="E407" s="29" t="s">
@@ -20817,7 +20817,7 @@
         <v>1505</v>
       </c>
       <c r="C409" s="31" t="s">
-        <v>2956</v>
+        <v>2954</v>
       </c>
       <c r="D409" s="29"/>
       <c r="E409" s="29" t="s">
@@ -20883,7 +20883,7 @@
         <v>17</v>
       </c>
       <c r="I411" s="31" t="s">
-        <v>2885</v>
+        <v>2883</v>
       </c>
     </row>
     <row r="412" spans="1:9" ht="30">
@@ -20910,7 +20910,7 @@
         <v>17</v>
       </c>
       <c r="I412" s="31" t="s">
-        <v>2886</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="413" spans="1:9" ht="30">
@@ -20946,7 +20946,7 @@
         <v>1505</v>
       </c>
       <c r="C414" s="31" t="s">
-        <v>2957</v>
+        <v>2955</v>
       </c>
       <c r="D414" s="29"/>
       <c r="E414" s="29" t="s">
@@ -20996,7 +20996,7 @@
         <v>1505</v>
       </c>
       <c r="C416" s="31" t="s">
-        <v>2958</v>
+        <v>2956</v>
       </c>
       <c r="D416" s="29"/>
       <c r="E416" s="29" t="s">
@@ -21062,7 +21062,7 @@
         <v>17</v>
       </c>
       <c r="I418" s="31" t="s">
-        <v>2887</v>
+        <v>2885</v>
       </c>
     </row>
     <row r="419" spans="1:9" ht="30">
@@ -21239,7 +21239,7 @@
         <v>17</v>
       </c>
       <c r="I425" s="31" t="s">
-        <v>2888</v>
+        <v>2886</v>
       </c>
     </row>
     <row r="426" spans="1:9" ht="45">
@@ -21253,7 +21253,7 @@
         <v>1970</v>
       </c>
       <c r="D426" s="29" t="s">
-        <v>2833</v>
+        <v>2831</v>
       </c>
       <c r="E426" s="29" t="s">
         <v>19</v>
@@ -21627,7 +21627,7 @@
         <v>32</v>
       </c>
       <c r="C441" s="31" t="s">
-        <v>3089</v>
+        <v>3086</v>
       </c>
       <c r="D441" s="29"/>
       <c r="E441" s="29" t="s">
@@ -21652,7 +21652,7 @@
         <v>32</v>
       </c>
       <c r="C442" s="31" t="s">
-        <v>2959</v>
+        <v>2957</v>
       </c>
       <c r="D442" s="29"/>
       <c r="E442" s="29" t="s">
@@ -21927,7 +21927,7 @@
         <v>32</v>
       </c>
       <c r="C453" s="31" t="s">
-        <v>2960</v>
+        <v>2958</v>
       </c>
       <c r="D453" s="29"/>
       <c r="E453" s="29" t="s">
@@ -21943,7 +21943,7 @@
         <v>17</v>
       </c>
       <c r="I453" s="31" t="s">
-        <v>2889</v>
+        <v>2887</v>
       </c>
     </row>
     <row r="454" spans="1:9" ht="45">
@@ -21979,7 +21979,7 @@
         <v>32</v>
       </c>
       <c r="C455" s="31" t="s">
-        <v>2961</v>
+        <v>2959</v>
       </c>
       <c r="D455" s="29"/>
       <c r="E455" s="29" t="s">
@@ -22529,7 +22529,7 @@
         <v>32</v>
       </c>
       <c r="C477" s="31" t="s">
-        <v>2962</v>
+        <v>2960</v>
       </c>
       <c r="D477" s="29"/>
       <c r="E477" s="29" t="s">
@@ -22545,7 +22545,7 @@
         <v>17</v>
       </c>
       <c r="I477" s="31" t="s">
-        <v>2890</v>
+        <v>2888</v>
       </c>
     </row>
     <row r="478" spans="1:9" ht="30">
@@ -22622,7 +22622,7 @@
         <v>17</v>
       </c>
       <c r="I480" s="31" t="s">
-        <v>2891</v>
+        <v>2889</v>
       </c>
     </row>
     <row r="481" spans="1:9" ht="30">
@@ -22636,7 +22636,7 @@
         <v>2020</v>
       </c>
       <c r="D481" s="29" t="s">
-        <v>2834</v>
+        <v>2832</v>
       </c>
       <c r="E481" s="29" t="s">
         <v>19</v>
@@ -22660,7 +22660,7 @@
         <v>32</v>
       </c>
       <c r="C482" s="31" t="s">
-        <v>2963</v>
+        <v>2961</v>
       </c>
       <c r="D482" s="29"/>
       <c r="E482" s="29" t="s">
@@ -22685,7 +22685,7 @@
         <v>32</v>
       </c>
       <c r="C483" s="31" t="s">
-        <v>2964</v>
+        <v>2962</v>
       </c>
       <c r="D483" s="29"/>
       <c r="E483" s="29" t="s">
@@ -22876,7 +22876,7 @@
         <v>17</v>
       </c>
       <c r="I490" s="31" t="s">
-        <v>2892</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="491" spans="1:9" ht="30">
@@ -23187,7 +23187,7 @@
         <v>32</v>
       </c>
       <c r="C503" s="31" t="s">
-        <v>2965</v>
+        <v>2963</v>
       </c>
       <c r="D503" s="29"/>
       <c r="E503" s="29" t="s">
@@ -23203,7 +23203,7 @@
         <v>17</v>
       </c>
       <c r="I503" s="31" t="s">
-        <v>2893</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="504" spans="1:9" ht="30">
@@ -23414,7 +23414,7 @@
         <v>32</v>
       </c>
       <c r="C512" s="31" t="s">
-        <v>2966</v>
+        <v>2964</v>
       </c>
       <c r="D512" s="29"/>
       <c r="E512" s="29" t="s">
@@ -23430,7 +23430,7 @@
         <v>17</v>
       </c>
       <c r="I512" s="31" t="s">
-        <v>2894</v>
+        <v>2892</v>
       </c>
     </row>
     <row r="513" spans="1:9" ht="60">
@@ -23441,7 +23441,7 @@
         <v>32</v>
       </c>
       <c r="C513" s="31" t="s">
-        <v>2967</v>
+        <v>2965</v>
       </c>
       <c r="D513" s="29"/>
       <c r="E513" s="29" t="s">
@@ -23457,7 +23457,7 @@
         <v>17</v>
       </c>
       <c r="I513" s="31" t="s">
-        <v>2895</v>
+        <v>2893</v>
       </c>
     </row>
     <row r="514" spans="1:9" ht="30">
@@ -23509,7 +23509,7 @@
         <v>17</v>
       </c>
       <c r="I515" s="31" t="s">
-        <v>2896</v>
+        <v>2894</v>
       </c>
     </row>
     <row r="516" spans="1:9" ht="30">
@@ -23770,7 +23770,7 @@
         <v>32</v>
       </c>
       <c r="C526" s="31" t="s">
-        <v>2968</v>
+        <v>2966</v>
       </c>
       <c r="D526" s="29"/>
       <c r="E526" s="29" t="s">
@@ -23786,7 +23786,7 @@
         <v>17</v>
       </c>
       <c r="I526" s="31" t="s">
-        <v>2897</v>
+        <v>2895</v>
       </c>
     </row>
     <row r="527" spans="1:9" ht="45">
@@ -24338,7 +24338,7 @@
         <v>17</v>
       </c>
       <c r="I548" s="31" t="s">
-        <v>2898</v>
+        <v>2896</v>
       </c>
     </row>
     <row r="549" spans="1:9" ht="60">
@@ -24415,7 +24415,7 @@
         <v>17</v>
       </c>
       <c r="I551" s="31" t="s">
-        <v>2898</v>
+        <v>2896</v>
       </c>
     </row>
     <row r="552" spans="1:9" ht="30">
@@ -28367,7 +28367,7 @@
         <v>17</v>
       </c>
       <c r="I709" s="31" t="s">
-        <v>2899</v>
+        <v>2897</v>
       </c>
     </row>
     <row r="710" spans="1:9" ht="30">
@@ -28669,7 +28669,7 @@
         <v>17</v>
       </c>
       <c r="I721" s="31" t="s">
-        <v>2868</v>
+        <v>2866</v>
       </c>
     </row>
     <row r="722" spans="1:9" ht="60">
@@ -28846,7 +28846,7 @@
         <v>17</v>
       </c>
       <c r="I728" s="31" t="s">
-        <v>2872</v>
+        <v>2870</v>
       </c>
     </row>
     <row r="729" spans="1:9" ht="60">
@@ -28857,7 +28857,7 @@
         <v>1523</v>
       </c>
       <c r="C729" s="31" t="s">
-        <v>2969</v>
+        <v>2967</v>
       </c>
       <c r="D729" s="29"/>
       <c r="E729" s="29" t="s">
@@ -28873,7 +28873,7 @@
         <v>17</v>
       </c>
       <c r="I729" s="31" t="s">
-        <v>2900</v>
+        <v>2898</v>
       </c>
     </row>
     <row r="730" spans="1:9" ht="45">
@@ -28900,7 +28900,7 @@
         <v>17</v>
       </c>
       <c r="I730" s="31" t="s">
-        <v>2873</v>
+        <v>2871</v>
       </c>
     </row>
     <row r="731" spans="1:9" ht="30">
@@ -28927,7 +28927,7 @@
         <v>17</v>
       </c>
       <c r="I731" s="31" t="s">
-        <v>2873</v>
+        <v>2871</v>
       </c>
     </row>
     <row r="732" spans="1:9" ht="30">
@@ -28988,7 +28988,7 @@
         <v>1523</v>
       </c>
       <c r="C734" s="31" t="s">
-        <v>2970</v>
+        <v>2968</v>
       </c>
       <c r="D734" s="29"/>
       <c r="E734" s="29" t="s">
@@ -29004,7 +29004,7 @@
         <v>17</v>
       </c>
       <c r="I734" s="31" t="s">
-        <v>2875</v>
+        <v>2873</v>
       </c>
     </row>
     <row r="735" spans="1:9" ht="45">
@@ -29081,7 +29081,7 @@
         <v>17</v>
       </c>
       <c r="I737" s="31" t="s">
-        <v>2901</v>
+        <v>2899</v>
       </c>
     </row>
     <row r="738" spans="1:9" ht="30">
@@ -29095,7 +29095,7 @@
         <v>2269</v>
       </c>
       <c r="D738" s="29" t="s">
-        <v>2835</v>
+        <v>2833</v>
       </c>
       <c r="E738" s="29" t="s">
         <v>19</v>
@@ -29122,7 +29122,7 @@
         <v>2270</v>
       </c>
       <c r="D739" s="29" t="s">
-        <v>2835</v>
+        <v>2833</v>
       </c>
       <c r="E739" s="29" t="s">
         <v>19</v>
@@ -29149,7 +29149,7 @@
         <v>2271</v>
       </c>
       <c r="D740" s="29" t="s">
-        <v>2835</v>
+        <v>2833</v>
       </c>
       <c r="E740" s="29" t="s">
         <v>19</v>
@@ -29176,7 +29176,7 @@
         <v>2272</v>
       </c>
       <c r="D741" s="29" t="s">
-        <v>2835</v>
+        <v>2833</v>
       </c>
       <c r="E741" s="29" t="s">
         <v>19</v>
@@ -29203,7 +29203,7 @@
         <v>2273</v>
       </c>
       <c r="D742" s="29" t="s">
-        <v>2835</v>
+        <v>2833</v>
       </c>
       <c r="E742" s="29" t="s">
         <v>19</v>
@@ -29230,7 +29230,7 @@
         <v>2274</v>
       </c>
       <c r="D743" s="29" t="s">
-        <v>2835</v>
+        <v>2833</v>
       </c>
       <c r="E743" s="29" t="s">
         <v>19</v>
@@ -29370,7 +29370,7 @@
         <v>17</v>
       </c>
       <c r="I748" s="31" t="s">
-        <v>2902</v>
+        <v>2900</v>
       </c>
     </row>
     <row r="749" spans="1:9" ht="45">
@@ -30447,7 +30447,7 @@
         <v>17</v>
       </c>
       <c r="I791" s="31" t="s">
-        <v>2903</v>
+        <v>2901</v>
       </c>
     </row>
     <row r="792" spans="1:9" ht="45">
@@ -30683,7 +30683,7 @@
         <v>33</v>
       </c>
       <c r="C801" s="31" t="s">
-        <v>2971</v>
+        <v>2969</v>
       </c>
       <c r="D801" s="29"/>
       <c r="E801" s="29" t="s">
@@ -30699,7 +30699,7 @@
         <v>17</v>
       </c>
       <c r="I801" s="31" t="s">
-        <v>2904</v>
+        <v>2902</v>
       </c>
     </row>
     <row r="802" spans="1:9" ht="30">
@@ -30960,7 +30960,7 @@
         <v>33</v>
       </c>
       <c r="C812" s="31" t="s">
-        <v>2972</v>
+        <v>2970</v>
       </c>
       <c r="D812" s="29"/>
       <c r="E812" s="29" t="s">
@@ -30976,7 +30976,7 @@
         <v>17</v>
       </c>
       <c r="I812" s="31" t="s">
-        <v>2905</v>
+        <v>2903</v>
       </c>
     </row>
     <row r="813" spans="1:9" ht="30">
@@ -31012,7 +31012,7 @@
         <v>33</v>
       </c>
       <c r="C814" s="31" t="s">
-        <v>2973</v>
+        <v>2971</v>
       </c>
       <c r="D814" s="29"/>
       <c r="E814" s="29" t="s">
@@ -31028,7 +31028,7 @@
         <v>17</v>
       </c>
       <c r="I814" s="31" t="s">
-        <v>2906</v>
+        <v>2904</v>
       </c>
     </row>
     <row r="815" spans="1:9">
@@ -31180,7 +31180,7 @@
         <v>17</v>
       </c>
       <c r="I820" s="31" t="s">
-        <v>2907</v>
+        <v>2905</v>
       </c>
     </row>
     <row r="821" spans="1:9" ht="30">
@@ -31194,7 +31194,7 @@
         <v>2349</v>
       </c>
       <c r="D821" s="29" t="s">
-        <v>2836</v>
+        <v>2834</v>
       </c>
       <c r="E821" s="29" t="s">
         <v>19</v>
@@ -31243,7 +31243,7 @@
         <v>33</v>
       </c>
       <c r="C823" s="31" t="s">
-        <v>2974</v>
+        <v>2972</v>
       </c>
       <c r="D823" s="29"/>
       <c r="E823" s="29" t="s">
@@ -31259,7 +31259,7 @@
         <v>17</v>
       </c>
       <c r="I823" s="31" t="s">
-        <v>2908</v>
+        <v>2906</v>
       </c>
     </row>
     <row r="824" spans="1:9" ht="45">
@@ -31570,7 +31570,7 @@
         <v>33</v>
       </c>
       <c r="C836" s="31" t="s">
-        <v>2975</v>
+        <v>2973</v>
       </c>
       <c r="D836" s="29"/>
       <c r="E836" s="29" t="s">
@@ -31586,7 +31586,7 @@
         <v>17</v>
       </c>
       <c r="I836" s="31" t="s">
-        <v>2941</v>
+        <v>2939</v>
       </c>
     </row>
     <row r="837" spans="1:9">
@@ -31622,7 +31622,7 @@
         <v>33</v>
       </c>
       <c r="C838" s="31" t="s">
-        <v>2976</v>
+        <v>2974</v>
       </c>
       <c r="D838" s="29"/>
       <c r="E838" s="29" t="s">
@@ -31638,7 +31638,7 @@
         <v>17</v>
       </c>
       <c r="I838" s="31" t="s">
-        <v>2909</v>
+        <v>2907</v>
       </c>
     </row>
     <row r="839" spans="1:9" ht="30">
@@ -31690,7 +31690,7 @@
         <v>17</v>
       </c>
       <c r="I840" s="31" t="s">
-        <v>2910</v>
+        <v>2908</v>
       </c>
     </row>
     <row r="841" spans="1:9" ht="30">
@@ -31704,7 +31704,7 @@
         <v>2366</v>
       </c>
       <c r="D841" s="29" t="s">
-        <v>2837</v>
+        <v>2835</v>
       </c>
       <c r="E841" s="29" t="s">
         <v>19</v>
@@ -32094,7 +32094,7 @@
         <v>17</v>
       </c>
       <c r="I856" s="31" t="s">
-        <v>2911</v>
+        <v>2909</v>
       </c>
     </row>
     <row r="857" spans="1:9" ht="60">
@@ -32171,7 +32171,7 @@
         <v>17</v>
       </c>
       <c r="I859" s="31" t="s">
-        <v>2911</v>
+        <v>2909</v>
       </c>
     </row>
     <row r="860" spans="1:9" ht="30">
@@ -32423,7 +32423,7 @@
         <v>17</v>
       </c>
       <c r="I869" s="31" t="s">
-        <v>2912</v>
+        <v>2910</v>
       </c>
     </row>
     <row r="870" spans="1:9" ht="45">
@@ -32450,7 +32450,7 @@
         <v>17</v>
       </c>
       <c r="I870" s="31" t="s">
-        <v>2913</v>
+        <v>2911</v>
       </c>
     </row>
     <row r="871" spans="1:9" ht="45">
@@ -33102,7 +33102,7 @@
         <v>17</v>
       </c>
       <c r="I896" s="31" t="s">
-        <v>2914</v>
+        <v>2912</v>
       </c>
     </row>
     <row r="897" spans="1:9" ht="45">
@@ -33154,7 +33154,7 @@
         <v>17</v>
       </c>
       <c r="I898" s="31" t="s">
-        <v>2913</v>
+        <v>2911</v>
       </c>
     </row>
     <row r="899" spans="1:9" ht="30">
@@ -33215,7 +33215,7 @@
         <v>1533</v>
       </c>
       <c r="C901" s="31" t="s">
-        <v>2977</v>
+        <v>2975</v>
       </c>
       <c r="D901" s="29"/>
       <c r="E901" s="29" t="s">
@@ -33306,7 +33306,7 @@
         <v>17</v>
       </c>
       <c r="I904" s="31" t="s">
-        <v>2915</v>
+        <v>2913</v>
       </c>
     </row>
     <row r="905" spans="1:9" ht="60">
@@ -33333,7 +33333,7 @@
         <v>17</v>
       </c>
       <c r="I905" s="31" t="s">
-        <v>2915</v>
+        <v>2913</v>
       </c>
     </row>
     <row r="906" spans="1:9" ht="30">
@@ -33785,7 +33785,7 @@
         <v>17</v>
       </c>
       <c r="I923" s="31" t="s">
-        <v>2916</v>
+        <v>2914</v>
       </c>
     </row>
     <row r="924" spans="1:9" ht="45">
@@ -33796,7 +33796,7 @@
         <v>1536</v>
       </c>
       <c r="C924" s="31" t="s">
-        <v>2978</v>
+        <v>2976</v>
       </c>
       <c r="D924" s="29"/>
       <c r="E924" s="29" t="s">
@@ -33812,7 +33812,7 @@
         <v>17</v>
       </c>
       <c r="I924" s="31" t="s">
-        <v>2917</v>
+        <v>2915</v>
       </c>
     </row>
     <row r="925" spans="1:9" ht="45">
@@ -33989,7 +33989,7 @@
         <v>17</v>
       </c>
       <c r="I931" s="31" t="s">
-        <v>2918</v>
+        <v>2916</v>
       </c>
     </row>
     <row r="932" spans="1:9" ht="30">
@@ -34003,7 +34003,7 @@
         <v>2269</v>
       </c>
       <c r="D932" s="29" t="s">
-        <v>2838</v>
+        <v>2836</v>
       </c>
       <c r="E932" s="29" t="s">
         <v>19</v>
@@ -34030,7 +34030,7 @@
         <v>2270</v>
       </c>
       <c r="D933" s="29" t="s">
-        <v>2838</v>
+        <v>2836</v>
       </c>
       <c r="E933" s="29" t="s">
         <v>19</v>
@@ -34057,7 +34057,7 @@
         <v>2447</v>
       </c>
       <c r="D934" s="29" t="s">
-        <v>2838</v>
+        <v>2836</v>
       </c>
       <c r="E934" s="29" t="s">
         <v>19</v>
@@ -34084,7 +34084,7 @@
         <v>2448</v>
       </c>
       <c r="D935" s="29" t="s">
-        <v>2838</v>
+        <v>2836</v>
       </c>
       <c r="E935" s="29" t="s">
         <v>19</v>
@@ -34111,7 +34111,7 @@
         <v>2449</v>
       </c>
       <c r="D936" s="29" t="s">
-        <v>2838</v>
+        <v>2836</v>
       </c>
       <c r="E936" s="29" t="s">
         <v>19</v>
@@ -34138,7 +34138,7 @@
         <v>2450</v>
       </c>
       <c r="D937" s="29" t="s">
-        <v>2838</v>
+        <v>2836</v>
       </c>
       <c r="E937" s="29" t="s">
         <v>19</v>
@@ -34165,7 +34165,7 @@
         <v>2451</v>
       </c>
       <c r="D938" s="29" t="s">
-        <v>2838</v>
+        <v>2836</v>
       </c>
       <c r="E938" s="29" t="s">
         <v>19</v>
@@ -34192,7 +34192,7 @@
         <v>2452</v>
       </c>
       <c r="D939" s="29" t="s">
-        <v>2838</v>
+        <v>2836</v>
       </c>
       <c r="E939" s="29" t="s">
         <v>19</v>
@@ -34219,7 +34219,7 @@
         <v>2453</v>
       </c>
       <c r="D940" s="29" t="s">
-        <v>2838</v>
+        <v>2836</v>
       </c>
       <c r="E940" s="29" t="s">
         <v>19</v>
@@ -34246,7 +34246,7 @@
         <v>2454</v>
       </c>
       <c r="D941" s="29" t="s">
-        <v>2838</v>
+        <v>2836</v>
       </c>
       <c r="E941" s="29" t="s">
         <v>19</v>
@@ -34273,7 +34273,7 @@
         <v>2455</v>
       </c>
       <c r="D942" s="29" t="s">
-        <v>2838</v>
+        <v>2836</v>
       </c>
       <c r="E942" s="29" t="s">
         <v>19</v>
@@ -34538,7 +34538,7 @@
         <v>17</v>
       </c>
       <c r="I952" s="31" t="s">
-        <v>2919</v>
+        <v>2917</v>
       </c>
     </row>
     <row r="953" spans="1:9" ht="30">
@@ -34974,7 +34974,7 @@
         <v>1539</v>
       </c>
       <c r="C970" s="31" t="s">
-        <v>2979</v>
+        <v>2977</v>
       </c>
       <c r="D970" s="29"/>
       <c r="E970" s="29" t="s">
@@ -34990,7 +34990,7 @@
         <v>17</v>
       </c>
       <c r="I970" s="31" t="s">
-        <v>2920</v>
+        <v>2918</v>
       </c>
     </row>
     <row r="971" spans="1:9" ht="60">
@@ -35017,7 +35017,7 @@
         <v>17</v>
       </c>
       <c r="I971" s="31" t="s">
-        <v>2921</v>
+        <v>2919</v>
       </c>
     </row>
     <row r="972" spans="1:9" ht="30">
@@ -35078,7 +35078,7 @@
         <v>1540</v>
       </c>
       <c r="C974" s="31" t="s">
-        <v>2980</v>
+        <v>2978</v>
       </c>
       <c r="D974" s="29"/>
       <c r="E974" s="29" t="s">
@@ -35094,7 +35094,7 @@
         <v>17</v>
       </c>
       <c r="I974" s="31" t="s">
-        <v>2939</v>
+        <v>2937</v>
       </c>
     </row>
     <row r="975" spans="1:9" ht="30">
@@ -35121,7 +35121,7 @@
         <v>17</v>
       </c>
       <c r="I975" s="31" t="s">
-        <v>2883</v>
+        <v>2881</v>
       </c>
     </row>
     <row r="976" spans="1:9" ht="45">
@@ -35223,7 +35223,7 @@
         <v>17</v>
       </c>
       <c r="I979" s="31" t="s">
-        <v>2922</v>
+        <v>2920</v>
       </c>
     </row>
     <row r="980" spans="1:9" ht="30">
@@ -35325,7 +35325,7 @@
         <v>17</v>
       </c>
       <c r="I983" s="31" t="s">
-        <v>2923</v>
+        <v>2921</v>
       </c>
     </row>
     <row r="984" spans="1:9" ht="30">
@@ -36986,7 +36986,7 @@
         <v>1553</v>
       </c>
       <c r="C1050" s="31" t="s">
-        <v>2981</v>
+        <v>2979</v>
       </c>
       <c r="D1050" s="29"/>
       <c r="E1050" s="29" t="s">
@@ -37061,7 +37061,7 @@
         <v>1554</v>
       </c>
       <c r="C1053" s="31" t="s">
-        <v>2982</v>
+        <v>2980</v>
       </c>
       <c r="D1053" s="29"/>
       <c r="E1053" s="29" t="s">
@@ -37336,7 +37336,7 @@
         <v>1554</v>
       </c>
       <c r="C1064" s="31" t="s">
-        <v>2983</v>
+        <v>2981</v>
       </c>
       <c r="D1064" s="29"/>
       <c r="E1064" s="29" t="s">
@@ -37386,7 +37386,7 @@
         <v>1554</v>
       </c>
       <c r="C1066" s="31" t="s">
-        <v>2984</v>
+        <v>2982</v>
       </c>
       <c r="D1066" s="29"/>
       <c r="E1066" s="29" t="s">
@@ -38011,7 +38011,7 @@
         <v>1554</v>
       </c>
       <c r="C1091" s="31" t="s">
-        <v>2985</v>
+        <v>2983</v>
       </c>
       <c r="D1091" s="29"/>
       <c r="E1091" s="29" t="s">
@@ -38102,7 +38102,7 @@
         <v>17</v>
       </c>
       <c r="I1094" s="31" t="s">
-        <v>2924</v>
+        <v>2922</v>
       </c>
     </row>
     <row r="1095" spans="1:9" ht="30">
@@ -38363,7 +38363,7 @@
         <v>1554</v>
       </c>
       <c r="C1105" s="31" t="s">
-        <v>2986</v>
+        <v>2984</v>
       </c>
       <c r="D1105" s="29"/>
       <c r="E1105" s="29" t="s">
@@ -38504,7 +38504,7 @@
         <v>17</v>
       </c>
       <c r="I1110" s="31" t="s">
-        <v>2898</v>
+        <v>2896</v>
       </c>
     </row>
     <row r="1111" spans="1:9" ht="30">
@@ -38556,7 +38556,7 @@
         <v>17</v>
       </c>
       <c r="I1112" s="31" t="s">
-        <v>2925</v>
+        <v>2923</v>
       </c>
     </row>
     <row r="1113" spans="1:9" ht="45">
@@ -38608,7 +38608,7 @@
         <v>17</v>
       </c>
       <c r="I1114" s="31" t="s">
-        <v>2926</v>
+        <v>2924</v>
       </c>
     </row>
     <row r="1115" spans="1:9" ht="195">
@@ -38635,7 +38635,7 @@
         <v>17</v>
       </c>
       <c r="I1115" s="31" t="s">
-        <v>2927</v>
+        <v>2925</v>
       </c>
     </row>
     <row r="1116" spans="1:9" ht="30">
@@ -38862,7 +38862,7 @@
         <v>17</v>
       </c>
       <c r="I1124" s="31" t="s">
-        <v>2871</v>
+        <v>2869</v>
       </c>
     </row>
     <row r="1125" spans="1:9" ht="30">
@@ -39048,7 +39048,7 @@
         <v>1557</v>
       </c>
       <c r="C1132" s="31" t="s">
-        <v>2987</v>
+        <v>2985</v>
       </c>
       <c r="D1132" s="29"/>
       <c r="E1132" s="29" t="s">
@@ -39448,7 +39448,7 @@
         <v>1557</v>
       </c>
       <c r="C1148" s="31" t="s">
-        <v>2988</v>
+        <v>2986</v>
       </c>
       <c r="D1148" s="29"/>
       <c r="E1148" s="29" t="s">
@@ -39773,7 +39773,7 @@
         <v>1561</v>
       </c>
       <c r="C1161" s="31" t="s">
-        <v>2989</v>
+        <v>2987</v>
       </c>
       <c r="D1161" s="29"/>
       <c r="E1161" s="29" t="s">
@@ -39998,7 +39998,7 @@
         <v>1561</v>
       </c>
       <c r="C1170" s="31" t="s">
-        <v>2990</v>
+        <v>2988</v>
       </c>
       <c r="D1170" s="29"/>
       <c r="E1170" s="29" t="s">
@@ -40015,7 +40015,7 @@
       </c>
       <c r="I1170" s="31"/>
     </row>
-    <row r="1171" spans="1:9" ht="60">
+    <row r="1171" spans="1:9" ht="75">
       <c r="A1171" s="29" t="s">
         <v>1194</v>
       </c>
@@ -40023,10 +40023,10 @@
         <v>1561</v>
       </c>
       <c r="C1171" s="31" t="s">
-        <v>2669</v>
+        <v>3087</v>
       </c>
       <c r="D1171" s="29" t="s">
-        <v>2839</v>
+        <v>2837</v>
       </c>
       <c r="E1171" s="29" t="s">
         <v>19</v>
@@ -40050,10 +40050,10 @@
         <v>1561</v>
       </c>
       <c r="C1172" s="31" t="s">
-        <v>2670</v>
+        <v>2669</v>
       </c>
       <c r="D1172" s="29" t="s">
-        <v>2839</v>
+        <v>2837</v>
       </c>
       <c r="E1172" s="29" t="s">
         <v>19</v>
@@ -40077,7 +40077,7 @@
         <v>1561</v>
       </c>
       <c r="C1173" s="31" t="s">
-        <v>2671</v>
+        <v>2670</v>
       </c>
       <c r="D1173" s="29"/>
       <c r="E1173" s="29" t="s">
@@ -40102,7 +40102,7 @@
         <v>1561</v>
       </c>
       <c r="C1174" s="31" t="s">
-        <v>2672</v>
+        <v>2671</v>
       </c>
       <c r="D1174" s="29"/>
       <c r="E1174" s="29" t="s">
@@ -40118,7 +40118,7 @@
         <v>17</v>
       </c>
       <c r="I1174" s="31" t="s">
-        <v>2928</v>
+        <v>2926</v>
       </c>
     </row>
     <row r="1175" spans="1:9" ht="30">
@@ -40129,7 +40129,7 @@
         <v>1561</v>
       </c>
       <c r="C1175" s="31" t="s">
-        <v>2673</v>
+        <v>2672</v>
       </c>
       <c r="D1175" s="29"/>
       <c r="E1175" s="29" t="s">
@@ -40154,7 +40154,7 @@
         <v>1561</v>
       </c>
       <c r="C1176" s="31" t="s">
-        <v>2674</v>
+        <v>2673</v>
       </c>
       <c r="D1176" s="29"/>
       <c r="E1176" s="29" t="s">
@@ -40179,7 +40179,7 @@
         <v>1561</v>
       </c>
       <c r="C1177" s="31" t="s">
-        <v>2675</v>
+        <v>2674</v>
       </c>
       <c r="D1177" s="29"/>
       <c r="E1177" s="29" t="s">
@@ -40204,7 +40204,7 @@
         <v>1561</v>
       </c>
       <c r="C1178" s="31" t="s">
-        <v>2676</v>
+        <v>2675</v>
       </c>
       <c r="D1178" s="29"/>
       <c r="E1178" s="29" t="s">
@@ -40229,7 +40229,7 @@
         <v>1561</v>
       </c>
       <c r="C1179" s="31" t="s">
-        <v>2677</v>
+        <v>2676</v>
       </c>
       <c r="D1179" s="29"/>
       <c r="E1179" s="29" t="s">
@@ -40254,7 +40254,7 @@
         <v>1561</v>
       </c>
       <c r="C1180" s="31" t="s">
-        <v>2678</v>
+        <v>2677</v>
       </c>
       <c r="D1180" s="29"/>
       <c r="E1180" s="29" t="s">
@@ -40279,7 +40279,7 @@
         <v>1561</v>
       </c>
       <c r="C1181" s="31" t="s">
-        <v>2679</v>
+        <v>2678</v>
       </c>
       <c r="D1181" s="29"/>
       <c r="E1181" s="29" t="s">
@@ -40304,7 +40304,7 @@
         <v>1561</v>
       </c>
       <c r="C1182" s="31" t="s">
-        <v>2680</v>
+        <v>2679</v>
       </c>
       <c r="D1182" s="29"/>
       <c r="E1182" s="29" t="s">
@@ -40329,7 +40329,7 @@
         <v>1561</v>
       </c>
       <c r="C1183" s="31" t="s">
-        <v>2681</v>
+        <v>2680</v>
       </c>
       <c r="D1183" s="29"/>
       <c r="E1183" s="29" t="s">
@@ -40354,7 +40354,7 @@
         <v>1561</v>
       </c>
       <c r="C1184" s="31" t="s">
-        <v>2682</v>
+        <v>2681</v>
       </c>
       <c r="D1184" s="29"/>
       <c r="E1184" s="29" t="s">
@@ -40379,7 +40379,7 @@
         <v>1562</v>
       </c>
       <c r="C1185" s="31" t="s">
-        <v>2683</v>
+        <v>2682</v>
       </c>
       <c r="D1185" s="29"/>
       <c r="E1185" s="29" t="s">
@@ -40404,7 +40404,7 @@
         <v>1563</v>
       </c>
       <c r="C1186" s="31" t="s">
-        <v>2684</v>
+        <v>2683</v>
       </c>
       <c r="D1186" s="29"/>
       <c r="E1186" s="29" t="s">
@@ -40429,7 +40429,7 @@
         <v>1563</v>
       </c>
       <c r="C1187" s="31" t="s">
-        <v>2685</v>
+        <v>2684</v>
       </c>
       <c r="D1187" s="29"/>
       <c r="E1187" s="29" t="s">
@@ -40454,7 +40454,7 @@
         <v>1563</v>
       </c>
       <c r="C1188" s="31" t="s">
-        <v>2686</v>
+        <v>2685</v>
       </c>
       <c r="D1188" s="29"/>
       <c r="E1188" s="29" t="s">
@@ -40479,7 +40479,7 @@
         <v>1563</v>
       </c>
       <c r="C1189" s="31" t="s">
-        <v>2687</v>
+        <v>2686</v>
       </c>
       <c r="D1189" s="29"/>
       <c r="E1189" s="29" t="s">
@@ -40504,7 +40504,7 @@
         <v>1564</v>
       </c>
       <c r="C1190" s="31" t="s">
-        <v>2688</v>
+        <v>2687</v>
       </c>
       <c r="D1190" s="29"/>
       <c r="E1190" s="29" t="s">
@@ -40520,7 +40520,7 @@
         <v>17</v>
       </c>
       <c r="I1190" s="31" t="s">
-        <v>2898</v>
+        <v>2896</v>
       </c>
     </row>
     <row r="1191" spans="1:9" ht="45">
@@ -40531,7 +40531,7 @@
         <v>1564</v>
       </c>
       <c r="C1191" s="31" t="s">
-        <v>2689</v>
+        <v>2688</v>
       </c>
       <c r="D1191" s="29"/>
       <c r="E1191" s="29" t="s">
@@ -40547,7 +40547,7 @@
         <v>17</v>
       </c>
       <c r="I1191" s="31" t="s">
-        <v>2925</v>
+        <v>2923</v>
       </c>
     </row>
     <row r="1192" spans="1:9" ht="45">
@@ -40558,7 +40558,7 @@
         <v>1564</v>
       </c>
       <c r="C1192" s="31" t="s">
-        <v>2690</v>
+        <v>2689</v>
       </c>
       <c r="D1192" s="29"/>
       <c r="E1192" s="29" t="s">
@@ -40583,7 +40583,7 @@
         <v>1565</v>
       </c>
       <c r="C1193" s="31" t="s">
-        <v>2691</v>
+        <v>2690</v>
       </c>
       <c r="D1193" s="29"/>
       <c r="E1193" s="29" t="s">
@@ -40599,7 +40599,7 @@
         <v>17</v>
       </c>
       <c r="I1193" s="31" t="s">
-        <v>2916</v>
+        <v>2914</v>
       </c>
     </row>
     <row r="1194" spans="1:9" ht="60">
@@ -40610,7 +40610,7 @@
         <v>1565</v>
       </c>
       <c r="C1194" s="31" t="s">
-        <v>2692</v>
+        <v>2691</v>
       </c>
       <c r="D1194" s="29"/>
       <c r="E1194" s="29" t="s">
@@ -40626,7 +40626,7 @@
         <v>17</v>
       </c>
       <c r="I1194" s="31" t="s">
-        <v>2916</v>
+        <v>2914</v>
       </c>
     </row>
     <row r="1195" spans="1:9" ht="30">
@@ -40637,7 +40637,7 @@
         <v>1565</v>
       </c>
       <c r="C1195" s="31" t="s">
-        <v>2693</v>
+        <v>2692</v>
       </c>
       <c r="D1195" s="29"/>
       <c r="E1195" s="29" t="s">
@@ -40662,7 +40662,7 @@
         <v>1565</v>
       </c>
       <c r="C1196" s="31" t="s">
-        <v>2694</v>
+        <v>2693</v>
       </c>
       <c r="D1196" s="29"/>
       <c r="E1196" s="29" t="s">
@@ -40712,7 +40712,7 @@
         <v>1565</v>
       </c>
       <c r="C1198" s="31" t="s">
-        <v>2695</v>
+        <v>2694</v>
       </c>
       <c r="D1198" s="29"/>
       <c r="E1198" s="29" t="s">
@@ -40737,7 +40737,7 @@
         <v>1565</v>
       </c>
       <c r="C1199" s="31" t="s">
-        <v>2696</v>
+        <v>2695</v>
       </c>
       <c r="D1199" s="29"/>
       <c r="E1199" s="29" t="s">
@@ -40762,7 +40762,7 @@
         <v>1565</v>
       </c>
       <c r="C1200" s="31" t="s">
-        <v>2697</v>
+        <v>2696</v>
       </c>
       <c r="D1200" s="29"/>
       <c r="E1200" s="29" t="s">
@@ -40787,7 +40787,7 @@
         <v>1565</v>
       </c>
       <c r="C1201" s="31" t="s">
-        <v>2698</v>
+        <v>2697</v>
       </c>
       <c r="D1201" s="29"/>
       <c r="E1201" s="29" t="s">
@@ -40812,7 +40812,7 @@
         <v>1565</v>
       </c>
       <c r="C1202" s="31" t="s">
-        <v>2699</v>
+        <v>2698</v>
       </c>
       <c r="D1202" s="29"/>
       <c r="E1202" s="29" t="s">
@@ -40837,7 +40837,7 @@
         <v>1565</v>
       </c>
       <c r="C1203" s="31" t="s">
-        <v>2700</v>
+        <v>2699</v>
       </c>
       <c r="D1203" s="29"/>
       <c r="E1203" s="29" t="s">
@@ -40862,7 +40862,7 @@
         <v>1565</v>
       </c>
       <c r="C1204" s="31" t="s">
-        <v>2701</v>
+        <v>2700</v>
       </c>
       <c r="D1204" s="29"/>
       <c r="E1204" s="29" t="s">
@@ -40887,7 +40887,7 @@
         <v>1565</v>
       </c>
       <c r="C1205" s="31" t="s">
-        <v>2702</v>
+        <v>2701</v>
       </c>
       <c r="D1205" s="29"/>
       <c r="E1205" s="29" t="s">
@@ -40912,7 +40912,7 @@
         <v>1565</v>
       </c>
       <c r="C1206" s="31" t="s">
-        <v>2703</v>
+        <v>2702</v>
       </c>
       <c r="D1206" s="29"/>
       <c r="E1206" s="29" t="s">
@@ -40937,7 +40937,7 @@
         <v>1565</v>
       </c>
       <c r="C1207" s="31" t="s">
-        <v>2704</v>
+        <v>2703</v>
       </c>
       <c r="D1207" s="29"/>
       <c r="E1207" s="29" t="s">
@@ -40962,7 +40962,7 @@
         <v>1566</v>
       </c>
       <c r="C1208" s="31" t="s">
-        <v>2705</v>
+        <v>2704</v>
       </c>
       <c r="D1208" s="29"/>
       <c r="E1208" s="29" t="s">
@@ -40987,7 +40987,7 @@
         <v>1566</v>
       </c>
       <c r="C1209" s="31" t="s">
-        <v>2706</v>
+        <v>2705</v>
       </c>
       <c r="D1209" s="29"/>
       <c r="E1209" s="29" t="s">
@@ -41012,7 +41012,7 @@
         <v>1566</v>
       </c>
       <c r="C1210" s="31" t="s">
-        <v>2707</v>
+        <v>2706</v>
       </c>
       <c r="D1210" s="29"/>
       <c r="E1210" s="29" t="s">
@@ -41112,7 +41112,7 @@
         <v>1566</v>
       </c>
       <c r="C1214" s="31" t="s">
-        <v>2708</v>
+        <v>2707</v>
       </c>
       <c r="D1214" s="29"/>
       <c r="E1214" s="29" t="s">
@@ -41137,7 +41137,7 @@
         <v>1566</v>
       </c>
       <c r="C1215" s="31" t="s">
-        <v>2709</v>
+        <v>2708</v>
       </c>
       <c r="D1215" s="29"/>
       <c r="E1215" s="29" t="s">
@@ -41162,7 +41162,7 @@
         <v>1566</v>
       </c>
       <c r="C1216" s="31" t="s">
-        <v>2710</v>
+        <v>2709</v>
       </c>
       <c r="D1216" s="29"/>
       <c r="E1216" s="29" t="s">
@@ -41262,7 +41262,7 @@
         <v>1566</v>
       </c>
       <c r="C1220" s="31" t="s">
-        <v>2711</v>
+        <v>2710</v>
       </c>
       <c r="D1220" s="29"/>
       <c r="E1220" s="29" t="s">
@@ -41287,7 +41287,7 @@
         <v>1566</v>
       </c>
       <c r="C1221" s="31" t="s">
-        <v>2712</v>
+        <v>2711</v>
       </c>
       <c r="D1221" s="29"/>
       <c r="E1221" s="29" t="s">
@@ -41312,7 +41312,7 @@
         <v>1566</v>
       </c>
       <c r="C1222" s="31" t="s">
-        <v>2713</v>
+        <v>2712</v>
       </c>
       <c r="D1222" s="29"/>
       <c r="E1222" s="29" t="s">
@@ -41337,7 +41337,7 @@
         <v>1566</v>
       </c>
       <c r="C1223" s="31" t="s">
-        <v>2714</v>
+        <v>2713</v>
       </c>
       <c r="D1223" s="29"/>
       <c r="E1223" s="29" t="s">
@@ -41362,7 +41362,7 @@
         <v>1566</v>
       </c>
       <c r="C1224" s="31" t="s">
-        <v>2715</v>
+        <v>2714</v>
       </c>
       <c r="D1224" s="29"/>
       <c r="E1224" s="29" t="s">
@@ -41387,7 +41387,7 @@
         <v>1566</v>
       </c>
       <c r="C1225" s="31" t="s">
-        <v>2716</v>
+        <v>2715</v>
       </c>
       <c r="D1225" s="29"/>
       <c r="E1225" s="29" t="s">
@@ -41412,7 +41412,7 @@
         <v>1566</v>
       </c>
       <c r="C1226" s="31" t="s">
-        <v>2717</v>
+        <v>2716</v>
       </c>
       <c r="D1226" s="29"/>
       <c r="E1226" s="29" t="s">
@@ -41437,7 +41437,7 @@
         <v>1566</v>
       </c>
       <c r="C1227" s="31" t="s">
-        <v>2718</v>
+        <v>2717</v>
       </c>
       <c r="D1227" s="29"/>
       <c r="E1227" s="29" t="s">
@@ -41462,7 +41462,7 @@
         <v>1566</v>
       </c>
       <c r="C1228" s="31" t="s">
-        <v>2719</v>
+        <v>2718</v>
       </c>
       <c r="D1228" s="29"/>
       <c r="E1228" s="29" t="s">
@@ -41487,7 +41487,7 @@
         <v>1566</v>
       </c>
       <c r="C1229" s="31" t="s">
-        <v>2720</v>
+        <v>2719</v>
       </c>
       <c r="D1229" s="29"/>
       <c r="E1229" s="29" t="s">
@@ -41512,7 +41512,7 @@
         <v>1566</v>
       </c>
       <c r="C1230" s="31" t="s">
-        <v>2721</v>
+        <v>2720</v>
       </c>
       <c r="D1230" s="29"/>
       <c r="E1230" s="29" t="s">
@@ -41537,7 +41537,7 @@
         <v>1566</v>
       </c>
       <c r="C1231" s="31" t="s">
-        <v>2722</v>
+        <v>2721</v>
       </c>
       <c r="D1231" s="29"/>
       <c r="E1231" s="29" t="s">
@@ -41562,7 +41562,7 @@
         <v>1566</v>
       </c>
       <c r="C1232" s="31" t="s">
-        <v>2723</v>
+        <v>2722</v>
       </c>
       <c r="D1232" s="29"/>
       <c r="E1232" s="29" t="s">
@@ -41587,7 +41587,7 @@
         <v>1566</v>
       </c>
       <c r="C1233" s="31" t="s">
-        <v>2724</v>
+        <v>2723</v>
       </c>
       <c r="D1233" s="29"/>
       <c r="E1233" s="29" t="s">
@@ -41612,7 +41612,7 @@
         <v>1566</v>
       </c>
       <c r="C1234" s="31" t="s">
-        <v>2725</v>
+        <v>2724</v>
       </c>
       <c r="D1234" s="29"/>
       <c r="E1234" s="29" t="s">
@@ -41637,7 +41637,7 @@
         <v>1566</v>
       </c>
       <c r="C1235" s="31" t="s">
-        <v>2726</v>
+        <v>2725</v>
       </c>
       <c r="D1235" s="29"/>
       <c r="E1235" s="29" t="s">
@@ -41662,7 +41662,7 @@
         <v>1566</v>
       </c>
       <c r="C1236" s="31" t="s">
-        <v>2727</v>
+        <v>2726</v>
       </c>
       <c r="D1236" s="29"/>
       <c r="E1236" s="29" t="s">
@@ -41687,7 +41687,7 @@
         <v>1566</v>
       </c>
       <c r="C1237" s="31" t="s">
-        <v>2728</v>
+        <v>2727</v>
       </c>
       <c r="D1237" s="29"/>
       <c r="E1237" s="29" t="s">
@@ -41712,7 +41712,7 @@
         <v>1566</v>
       </c>
       <c r="C1238" s="31" t="s">
-        <v>2729</v>
+        <v>2728</v>
       </c>
       <c r="D1238" s="29"/>
       <c r="E1238" s="29" t="s">
@@ -41737,7 +41737,7 @@
         <v>1566</v>
       </c>
       <c r="C1239" s="31" t="s">
-        <v>2730</v>
+        <v>2729</v>
       </c>
       <c r="D1239" s="29"/>
       <c r="E1239" s="29" t="s">
@@ -41762,7 +41762,7 @@
         <v>1566</v>
       </c>
       <c r="C1240" s="31" t="s">
-        <v>2731</v>
+        <v>2730</v>
       </c>
       <c r="D1240" s="29"/>
       <c r="E1240" s="29" t="s">
@@ -41787,7 +41787,7 @@
         <v>1566</v>
       </c>
       <c r="C1241" s="31" t="s">
-        <v>2732</v>
+        <v>2731</v>
       </c>
       <c r="D1241" s="29"/>
       <c r="E1241" s="29" t="s">
@@ -41812,7 +41812,7 @@
         <v>1566</v>
       </c>
       <c r="C1242" s="31" t="s">
-        <v>2733</v>
+        <v>2732</v>
       </c>
       <c r="D1242" s="29"/>
       <c r="E1242" s="29" t="s">
@@ -41837,7 +41837,7 @@
         <v>1566</v>
       </c>
       <c r="C1243" s="31" t="s">
-        <v>2734</v>
+        <v>2733</v>
       </c>
       <c r="D1243" s="29"/>
       <c r="E1243" s="29" t="s">
@@ -41862,7 +41862,7 @@
         <v>1566</v>
       </c>
       <c r="C1244" s="31" t="s">
-        <v>2735</v>
+        <v>2734</v>
       </c>
       <c r="D1244" s="29"/>
       <c r="E1244" s="29" t="s">
@@ -41887,7 +41887,7 @@
         <v>1566</v>
       </c>
       <c r="C1245" s="31" t="s">
-        <v>2736</v>
+        <v>2735</v>
       </c>
       <c r="D1245" s="29"/>
       <c r="E1245" s="29" t="s">
@@ -41912,7 +41912,7 @@
         <v>1566</v>
       </c>
       <c r="C1246" s="31" t="s">
-        <v>2737</v>
+        <v>2736</v>
       </c>
       <c r="D1246" s="29"/>
       <c r="E1246" s="29" t="s">
@@ -41937,7 +41937,7 @@
         <v>1566</v>
       </c>
       <c r="C1247" s="31" t="s">
-        <v>2738</v>
+        <v>2737</v>
       </c>
       <c r="D1247" s="29"/>
       <c r="E1247" s="29" t="s">
@@ -41962,7 +41962,7 @@
         <v>1566</v>
       </c>
       <c r="C1248" s="31" t="s">
-        <v>2739</v>
+        <v>2738</v>
       </c>
       <c r="D1248" s="29"/>
       <c r="E1248" s="29" t="s">
@@ -41987,7 +41987,7 @@
         <v>1566</v>
       </c>
       <c r="C1249" s="31" t="s">
-        <v>2740</v>
+        <v>2739</v>
       </c>
       <c r="D1249" s="29"/>
       <c r="E1249" s="29" t="s">
@@ -42012,7 +42012,7 @@
         <v>1566</v>
       </c>
       <c r="C1250" s="31" t="s">
-        <v>2741</v>
+        <v>2740</v>
       </c>
       <c r="D1250" s="29"/>
       <c r="E1250" s="29" t="s">
@@ -42037,7 +42037,7 @@
         <v>1567</v>
       </c>
       <c r="C1251" s="31" t="s">
-        <v>2742</v>
+        <v>2741</v>
       </c>
       <c r="D1251" s="29"/>
       <c r="E1251" s="29" t="s">
@@ -42062,7 +42062,7 @@
         <v>1567</v>
       </c>
       <c r="C1252" s="31" t="s">
-        <v>2743</v>
+        <v>2742</v>
       </c>
       <c r="D1252" s="29"/>
       <c r="E1252" s="29" t="s">
@@ -42087,7 +42087,7 @@
         <v>1567</v>
       </c>
       <c r="C1253" s="31" t="s">
-        <v>2744</v>
+        <v>2743</v>
       </c>
       <c r="D1253" s="29"/>
       <c r="E1253" s="29" t="s">
@@ -42112,7 +42112,7 @@
         <v>1568</v>
       </c>
       <c r="C1254" s="31" t="s">
-        <v>2745</v>
+        <v>2744</v>
       </c>
       <c r="D1254" s="29"/>
       <c r="E1254" s="29" t="s">
@@ -42137,7 +42137,7 @@
         <v>1568</v>
       </c>
       <c r="C1255" s="31" t="s">
-        <v>2746</v>
+        <v>2745</v>
       </c>
       <c r="D1255" s="29"/>
       <c r="E1255" s="29" t="s">
@@ -42162,7 +42162,7 @@
         <v>1568</v>
       </c>
       <c r="C1256" s="31" t="s">
-        <v>2747</v>
+        <v>2746</v>
       </c>
       <c r="D1256" s="29"/>
       <c r="E1256" s="29" t="s">
@@ -42187,7 +42187,7 @@
         <v>1568</v>
       </c>
       <c r="C1257" s="31" t="s">
-        <v>2748</v>
+        <v>2747</v>
       </c>
       <c r="D1257" s="29"/>
       <c r="E1257" s="29" t="s">
@@ -42212,7 +42212,7 @@
         <v>1569</v>
       </c>
       <c r="C1258" s="31" t="s">
-        <v>2749</v>
+        <v>2748</v>
       </c>
       <c r="D1258" s="29"/>
       <c r="E1258" s="29" t="s">
@@ -42237,7 +42237,7 @@
         <v>1569</v>
       </c>
       <c r="C1259" s="31" t="s">
-        <v>2750</v>
+        <v>2749</v>
       </c>
       <c r="D1259" s="29"/>
       <c r="E1259" s="29" t="s">
@@ -42262,7 +42262,7 @@
         <v>1569</v>
       </c>
       <c r="C1260" s="31" t="s">
-        <v>2751</v>
+        <v>2750</v>
       </c>
       <c r="D1260" s="29"/>
       <c r="E1260" s="29" t="s">
@@ -42287,7 +42287,7 @@
         <v>1569</v>
       </c>
       <c r="C1261" s="31" t="s">
-        <v>2752</v>
+        <v>2751</v>
       </c>
       <c r="D1261" s="29"/>
       <c r="E1261" s="29" t="s">
@@ -42312,7 +42312,7 @@
         <v>1569</v>
       </c>
       <c r="C1262" s="31" t="s">
-        <v>2753</v>
+        <v>2752</v>
       </c>
       <c r="D1262" s="29"/>
       <c r="E1262" s="29" t="s">
@@ -42337,7 +42337,7 @@
         <v>1569</v>
       </c>
       <c r="C1263" s="31" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="D1263" s="29"/>
       <c r="E1263" s="29" t="s">
@@ -42362,7 +42362,7 @@
         <v>1569</v>
       </c>
       <c r="C1264" s="31" t="s">
-        <v>2755</v>
+        <v>2754</v>
       </c>
       <c r="D1264" s="29"/>
       <c r="E1264" s="29" t="s">
@@ -42387,7 +42387,7 @@
         <v>1570</v>
       </c>
       <c r="C1265" s="31" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D1265" s="29"/>
       <c r="E1265" s="29" t="s">
@@ -42412,7 +42412,7 @@
         <v>1570</v>
       </c>
       <c r="C1266" s="31" t="s">
-        <v>2991</v>
+        <v>2989</v>
       </c>
       <c r="D1266" s="29"/>
       <c r="E1266" s="29" t="s">
@@ -42437,7 +42437,7 @@
         <v>1570</v>
       </c>
       <c r="C1267" s="31" t="s">
-        <v>2757</v>
+        <v>2756</v>
       </c>
       <c r="D1267" s="29"/>
       <c r="E1267" s="29" t="s">
@@ -42462,7 +42462,7 @@
         <v>1570</v>
       </c>
       <c r="C1268" s="31" t="s">
-        <v>2758</v>
+        <v>2757</v>
       </c>
       <c r="D1268" s="29"/>
       <c r="E1268" s="29" t="s">
@@ -42487,7 +42487,7 @@
         <v>1571</v>
       </c>
       <c r="C1269" s="31" t="s">
-        <v>2759</v>
+        <v>2758</v>
       </c>
       <c r="D1269" s="29"/>
       <c r="E1269" s="29" t="s">
@@ -42512,7 +42512,7 @@
         <v>1572</v>
       </c>
       <c r="C1270" s="31" t="s">
-        <v>2760</v>
+        <v>2759</v>
       </c>
       <c r="D1270" s="29"/>
       <c r="E1270" s="29" t="s">
@@ -42587,7 +42587,7 @@
         <v>1572</v>
       </c>
       <c r="C1273" s="31" t="s">
-        <v>2761</v>
+        <v>2760</v>
       </c>
       <c r="D1273" s="29"/>
       <c r="E1273" s="29" t="s">
@@ -42612,7 +42612,7 @@
         <v>1572</v>
       </c>
       <c r="C1274" s="31" t="s">
-        <v>2762</v>
+        <v>2761</v>
       </c>
       <c r="D1274" s="29"/>
       <c r="E1274" s="29" t="s">
@@ -42637,7 +42637,7 @@
         <v>1572</v>
       </c>
       <c r="C1275" s="31" t="s">
-        <v>2763</v>
+        <v>2762</v>
       </c>
       <c r="D1275" s="29"/>
       <c r="E1275" s="29" t="s">
@@ -42662,7 +42662,7 @@
         <v>1572</v>
       </c>
       <c r="C1276" s="31" t="s">
-        <v>2764</v>
+        <v>2763</v>
       </c>
       <c r="D1276" s="29"/>
       <c r="E1276" s="29" t="s">
@@ -42687,7 +42687,7 @@
         <v>1572</v>
       </c>
       <c r="C1277" s="31" t="s">
-        <v>2765</v>
+        <v>2764</v>
       </c>
       <c r="D1277" s="29"/>
       <c r="E1277" s="29" t="s">
@@ -42703,7 +42703,7 @@
         <v>17</v>
       </c>
       <c r="I1277" s="31" t="s">
-        <v>2929</v>
+        <v>2927</v>
       </c>
     </row>
     <row r="1278" spans="1:9" ht="30">
@@ -42714,7 +42714,7 @@
         <v>1572</v>
       </c>
       <c r="C1278" s="31" t="s">
-        <v>2766</v>
+        <v>2765</v>
       </c>
       <c r="D1278" s="29"/>
       <c r="E1278" s="29" t="s">
@@ -42739,7 +42739,7 @@
         <v>1572</v>
       </c>
       <c r="C1279" s="31" t="s">
-        <v>2767</v>
+        <v>2766</v>
       </c>
       <c r="D1279" s="29"/>
       <c r="E1279" s="29" t="s">
@@ -42764,7 +42764,7 @@
         <v>1572</v>
       </c>
       <c r="C1280" s="31" t="s">
-        <v>2768</v>
+        <v>2767</v>
       </c>
       <c r="D1280" s="29"/>
       <c r="E1280" s="29" t="s">
@@ -42789,7 +42789,7 @@
         <v>1572</v>
       </c>
       <c r="C1281" s="31" t="s">
-        <v>2769</v>
+        <v>2768</v>
       </c>
       <c r="D1281" s="29"/>
       <c r="E1281" s="29" t="s">
@@ -42814,7 +42814,7 @@
         <v>1572</v>
       </c>
       <c r="C1282" s="31" t="s">
-        <v>2770</v>
+        <v>2769</v>
       </c>
       <c r="D1282" s="29"/>
       <c r="E1282" s="29" t="s">
@@ -42839,7 +42839,7 @@
         <v>1573</v>
       </c>
       <c r="C1283" s="31" t="s">
-        <v>2771</v>
+        <v>2770</v>
       </c>
       <c r="D1283" s="29"/>
       <c r="E1283" s="29" t="s">
@@ -42864,7 +42864,7 @@
         <v>1573</v>
       </c>
       <c r="C1284" s="31" t="s">
-        <v>2772</v>
+        <v>2771</v>
       </c>
       <c r="D1284" s="29"/>
       <c r="E1284" s="29" t="s">
@@ -42889,7 +42889,7 @@
         <v>1573</v>
       </c>
       <c r="C1285" s="31" t="s">
-        <v>2992</v>
+        <v>2990</v>
       </c>
       <c r="D1285" s="29"/>
       <c r="E1285" s="29" t="s">
@@ -42914,7 +42914,7 @@
         <v>1573</v>
       </c>
       <c r="C1286" s="31" t="s">
-        <v>2773</v>
+        <v>2772</v>
       </c>
       <c r="D1286" s="29"/>
       <c r="E1286" s="29" t="s">
@@ -42939,7 +42939,7 @@
         <v>1573</v>
       </c>
       <c r="C1287" s="31" t="s">
-        <v>2774</v>
+        <v>2773</v>
       </c>
       <c r="D1287" s="29"/>
       <c r="E1287" s="29" t="s">
@@ -42989,7 +42989,7 @@
         <v>1573</v>
       </c>
       <c r="C1289" s="31" t="s">
-        <v>2775</v>
+        <v>2774</v>
       </c>
       <c r="D1289" s="29"/>
       <c r="E1289" s="29" t="s">
@@ -43014,7 +43014,7 @@
         <v>1573</v>
       </c>
       <c r="C1290" s="31" t="s">
-        <v>2776</v>
+        <v>2775</v>
       </c>
       <c r="D1290" s="29"/>
       <c r="E1290" s="29" t="s">
@@ -43039,7 +43039,7 @@
         <v>1574</v>
       </c>
       <c r="C1291" s="31" t="s">
-        <v>2777</v>
+        <v>2776</v>
       </c>
       <c r="D1291" s="29"/>
       <c r="E1291" s="29" t="s">
@@ -43064,7 +43064,7 @@
         <v>1574</v>
       </c>
       <c r="C1292" s="31" t="s">
-        <v>2993</v>
+        <v>2991</v>
       </c>
       <c r="D1292" s="29"/>
       <c r="E1292" s="29" t="s">
@@ -43080,7 +43080,7 @@
         <v>17</v>
       </c>
       <c r="I1292" s="31" t="s">
-        <v>2930</v>
+        <v>2928</v>
       </c>
     </row>
     <row r="1293" spans="1:9" ht="45">
@@ -43091,7 +43091,7 @@
         <v>1574</v>
       </c>
       <c r="C1293" s="31" t="s">
-        <v>2778</v>
+        <v>2777</v>
       </c>
       <c r="D1293" s="29"/>
       <c r="E1293" s="29" t="s">
@@ -43107,7 +43107,7 @@
         <v>17</v>
       </c>
       <c r="I1293" s="31" t="s">
-        <v>2931</v>
+        <v>2929</v>
       </c>
     </row>
     <row r="1294" spans="1:9" ht="45">
@@ -43118,7 +43118,7 @@
         <v>1574</v>
       </c>
       <c r="C1294" s="31" t="s">
-        <v>2779</v>
+        <v>2778</v>
       </c>
       <c r="D1294" s="29"/>
       <c r="E1294" s="29" t="s">
@@ -43143,7 +43143,7 @@
         <v>1574</v>
       </c>
       <c r="C1295" s="31" t="s">
-        <v>2780</v>
+        <v>2779</v>
       </c>
       <c r="D1295" s="29"/>
       <c r="E1295" s="29" t="s">
@@ -43168,7 +43168,7 @@
         <v>1575</v>
       </c>
       <c r="C1296" s="31" t="s">
-        <v>2781</v>
+        <v>2780</v>
       </c>
       <c r="D1296" s="29"/>
       <c r="E1296" s="29" t="s">
@@ -43193,7 +43193,7 @@
         <v>1575</v>
       </c>
       <c r="C1297" s="31" t="s">
-        <v>2994</v>
+        <v>2992</v>
       </c>
       <c r="D1297" s="29"/>
       <c r="E1297" s="29" t="s">
@@ -43209,7 +43209,7 @@
         <v>17</v>
       </c>
       <c r="I1297" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1298" spans="1:9" ht="30">
@@ -43220,7 +43220,7 @@
         <v>1575</v>
       </c>
       <c r="C1298" s="31" t="s">
-        <v>2782</v>
+        <v>2781</v>
       </c>
       <c r="D1298" s="29"/>
       <c r="E1298" s="29" t="s">
@@ -43245,7 +43245,7 @@
         <v>1575</v>
       </c>
       <c r="C1299" s="31" t="s">
-        <v>2783</v>
+        <v>2782</v>
       </c>
       <c r="D1299" s="29"/>
       <c r="E1299" s="29" t="s">
@@ -43270,7 +43270,7 @@
         <v>1575</v>
       </c>
       <c r="C1300" s="31" t="s">
-        <v>2784</v>
+        <v>2783</v>
       </c>
       <c r="D1300" s="29"/>
       <c r="E1300" s="29" t="s">
@@ -43286,7 +43286,7 @@
         <v>17</v>
       </c>
       <c r="I1300" s="31" t="s">
-        <v>2933</v>
+        <v>2931</v>
       </c>
     </row>
     <row r="1301" spans="1:9" ht="30">
@@ -43297,7 +43297,7 @@
         <v>1575</v>
       </c>
       <c r="C1301" s="31" t="s">
-        <v>2785</v>
+        <v>2784</v>
       </c>
       <c r="D1301" s="29"/>
       <c r="E1301" s="29" t="s">
@@ -43322,7 +43322,7 @@
         <v>1575</v>
       </c>
       <c r="C1302" s="31" t="s">
-        <v>2786</v>
+        <v>2785</v>
       </c>
       <c r="D1302" s="29"/>
       <c r="E1302" s="29" t="s">
@@ -43347,7 +43347,7 @@
         <v>1575</v>
       </c>
       <c r="C1303" s="31" t="s">
-        <v>2787</v>
+        <v>2786</v>
       </c>
       <c r="D1303" s="29"/>
       <c r="E1303" s="29" t="s">
@@ -43372,7 +43372,7 @@
         <v>1575</v>
       </c>
       <c r="C1304" s="31" t="s">
-        <v>2788</v>
+        <v>2787</v>
       </c>
       <c r="D1304" s="29"/>
       <c r="E1304" s="29" t="s">
@@ -43397,7 +43397,7 @@
         <v>1575</v>
       </c>
       <c r="C1305" s="31" t="s">
-        <v>2789</v>
+        <v>2788</v>
       </c>
       <c r="D1305" s="29"/>
       <c r="E1305" s="29" t="s">
@@ -43422,7 +43422,7 @@
         <v>1575</v>
       </c>
       <c r="C1306" s="31" t="s">
-        <v>2790</v>
+        <v>2789</v>
       </c>
       <c r="D1306" s="29"/>
       <c r="E1306" s="29" t="s">
@@ -43447,7 +43447,7 @@
         <v>1575</v>
       </c>
       <c r="C1307" s="31" t="s">
-        <v>2791</v>
+        <v>2790</v>
       </c>
       <c r="D1307" s="29"/>
       <c r="E1307" s="29" t="s">
@@ -43472,7 +43472,7 @@
         <v>1575</v>
       </c>
       <c r="C1308" s="31" t="s">
-        <v>2792</v>
+        <v>2791</v>
       </c>
       <c r="D1308" s="29"/>
       <c r="E1308" s="29" t="s">
@@ -43497,7 +43497,7 @@
         <v>1575</v>
       </c>
       <c r="C1309" s="31" t="s">
-        <v>2793</v>
+        <v>2792</v>
       </c>
       <c r="D1309" s="29"/>
       <c r="E1309" s="29" t="s">
@@ -43522,7 +43522,7 @@
         <v>1575</v>
       </c>
       <c r="C1310" s="31" t="s">
-        <v>2794</v>
+        <v>2793</v>
       </c>
       <c r="D1310" s="29"/>
       <c r="E1310" s="29" t="s">
@@ -43547,7 +43547,7 @@
         <v>1575</v>
       </c>
       <c r="C1311" s="31" t="s">
-        <v>2795</v>
+        <v>2794</v>
       </c>
       <c r="D1311" s="29"/>
       <c r="E1311" s="29" t="s">
@@ -43572,7 +43572,7 @@
         <v>1575</v>
       </c>
       <c r="C1312" s="31" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="D1312" s="29"/>
       <c r="E1312" s="29" t="s">
@@ -43597,7 +43597,7 @@
         <v>1575</v>
       </c>
       <c r="C1313" s="31" t="s">
-        <v>2797</v>
+        <v>2796</v>
       </c>
       <c r="D1313" s="29"/>
       <c r="E1313" s="29" t="s">
@@ -43613,7 +43613,7 @@
         <v>17</v>
       </c>
       <c r="I1313" s="31" t="s">
-        <v>2934</v>
+        <v>2932</v>
       </c>
     </row>
     <row r="1314" spans="1:9" ht="60">
@@ -43624,7 +43624,7 @@
         <v>1575</v>
       </c>
       <c r="C1314" s="31" t="s">
-        <v>2798</v>
+        <v>2797</v>
       </c>
       <c r="D1314" s="29"/>
       <c r="E1314" s="29" t="s">
@@ -43649,7 +43649,7 @@
         <v>1575</v>
       </c>
       <c r="C1315" s="31" t="s">
-        <v>2799</v>
+        <v>2798</v>
       </c>
       <c r="D1315" s="29"/>
       <c r="E1315" s="29" t="s">
@@ -43674,7 +43674,7 @@
         <v>1575</v>
       </c>
       <c r="C1316" s="31" t="s">
-        <v>2800</v>
+        <v>2799</v>
       </c>
       <c r="D1316" s="29"/>
       <c r="E1316" s="29" t="s">
@@ -43699,7 +43699,7 @@
         <v>1575</v>
       </c>
       <c r="C1317" s="31" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="D1317" s="29"/>
       <c r="E1317" s="29" t="s">
@@ -43724,7 +43724,7 @@
         <v>1575</v>
       </c>
       <c r="C1318" s="31" t="s">
-        <v>2802</v>
+        <v>2801</v>
       </c>
       <c r="D1318" s="29"/>
       <c r="E1318" s="29" t="s">
@@ -43749,7 +43749,7 @@
         <v>1575</v>
       </c>
       <c r="C1319" s="31" t="s">
-        <v>2995</v>
+        <v>2993</v>
       </c>
       <c r="D1319" s="29"/>
       <c r="E1319" s="29" t="s">
@@ -43774,7 +43774,7 @@
         <v>1575</v>
       </c>
       <c r="C1320" s="31" t="s">
-        <v>2803</v>
+        <v>2802</v>
       </c>
       <c r="D1320" s="29"/>
       <c r="E1320" s="29" t="s">
@@ -43799,7 +43799,7 @@
         <v>1575</v>
       </c>
       <c r="C1321" s="31" t="s">
-        <v>2804</v>
+        <v>2803</v>
       </c>
       <c r="D1321" s="29"/>
       <c r="E1321" s="29" t="s">
@@ -43824,7 +43824,7 @@
         <v>1576</v>
       </c>
       <c r="C1322" s="31" t="s">
-        <v>2805</v>
+        <v>2804</v>
       </c>
       <c r="D1322" s="29"/>
       <c r="E1322" s="29" t="s">
@@ -43899,7 +43899,7 @@
         <v>1576</v>
       </c>
       <c r="C1325" s="31" t="s">
-        <v>2806</v>
+        <v>2805</v>
       </c>
       <c r="D1325" s="29"/>
       <c r="E1325" s="29" t="s">
@@ -43924,7 +43924,7 @@
         <v>1576</v>
       </c>
       <c r="C1326" s="31" t="s">
-        <v>2807</v>
+        <v>2806</v>
       </c>
       <c r="D1326" s="29"/>
       <c r="E1326" s="29" t="s">
@@ -43949,7 +43949,7 @@
         <v>1577</v>
       </c>
       <c r="C1327" s="31" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="D1327" s="29"/>
       <c r="E1327" s="29" t="s">
@@ -43974,7 +43974,7 @@
         <v>1578</v>
       </c>
       <c r="C1328" s="31" t="s">
-        <v>2777</v>
+        <v>2776</v>
       </c>
       <c r="D1328" s="29"/>
       <c r="E1328" s="29" t="s">
@@ -43999,7 +43999,7 @@
         <v>1578</v>
       </c>
       <c r="C1329" s="31" t="s">
-        <v>2996</v>
+        <v>2994</v>
       </c>
       <c r="D1329" s="29"/>
       <c r="E1329" s="29" t="s">
@@ -44074,7 +44074,7 @@
         <v>1579</v>
       </c>
       <c r="C1332" s="31" t="s">
-        <v>2809</v>
+        <v>2808</v>
       </c>
       <c r="D1332" s="29"/>
       <c r="E1332" s="29" t="s">
@@ -44099,7 +44099,7 @@
         <v>1579</v>
       </c>
       <c r="C1333" s="31" t="s">
-        <v>2810</v>
+        <v>2809</v>
       </c>
       <c r="D1333" s="29"/>
       <c r="E1333" s="29" t="s">
@@ -44124,10 +44124,10 @@
         <v>1579</v>
       </c>
       <c r="C1334" s="31" t="s">
-        <v>2811</v>
+        <v>2810</v>
       </c>
       <c r="D1334" s="29" t="s">
-        <v>2840</v>
+        <v>2838</v>
       </c>
       <c r="E1334" s="29" t="s">
         <v>22</v>
@@ -44142,7 +44142,7 @@
         <v>21</v>
       </c>
       <c r="I1334" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1335" spans="1:9" ht="30">
@@ -44153,10 +44153,10 @@
         <v>1579</v>
       </c>
       <c r="C1335" s="31" t="s">
-        <v>2997</v>
+        <v>2995</v>
       </c>
       <c r="D1335" s="29" t="s">
-        <v>2840</v>
+        <v>2838</v>
       </c>
       <c r="E1335" s="29" t="s">
         <v>22</v>
@@ -44180,10 +44180,10 @@
         <v>1579</v>
       </c>
       <c r="C1336" s="31" t="s">
-        <v>2812</v>
+        <v>2811</v>
       </c>
       <c r="D1336" s="29" t="s">
-        <v>2840</v>
+        <v>2838</v>
       </c>
       <c r="E1336" s="29" t="s">
         <v>22</v>
@@ -44198,7 +44198,7 @@
         <v>21</v>
       </c>
       <c r="I1336" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1337" spans="1:9" ht="45">
@@ -44209,10 +44209,10 @@
         <v>1579</v>
       </c>
       <c r="C1337" s="31" t="s">
-        <v>2813</v>
+        <v>2812</v>
       </c>
       <c r="D1337" s="29" t="s">
-        <v>2841</v>
+        <v>2839</v>
       </c>
       <c r="E1337" s="29" t="s">
         <v>22</v>
@@ -44227,7 +44227,7 @@
         <v>21</v>
       </c>
       <c r="I1337" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1338" spans="1:9" ht="45">
@@ -44238,10 +44238,10 @@
         <v>1579</v>
       </c>
       <c r="C1338" s="31" t="s">
-        <v>2998</v>
+        <v>2996</v>
       </c>
       <c r="D1338" s="29" t="s">
-        <v>2841</v>
+        <v>2839</v>
       </c>
       <c r="E1338" s="29" t="s">
         <v>22</v>
@@ -44256,7 +44256,7 @@
         <v>21</v>
       </c>
       <c r="I1338" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1339" spans="1:9" ht="60">
@@ -44267,7 +44267,7 @@
         <v>1579</v>
       </c>
       <c r="C1339" s="31" t="s">
-        <v>3021</v>
+        <v>3018</v>
       </c>
       <c r="D1339" s="29"/>
       <c r="E1339" s="29" t="s">
@@ -44292,7 +44292,7 @@
         <v>1579</v>
       </c>
       <c r="C1340" s="31" t="s">
-        <v>2999</v>
+        <v>2997</v>
       </c>
       <c r="D1340" s="29"/>
       <c r="E1340" s="29" t="s">
@@ -44317,7 +44317,7 @@
         <v>1579</v>
       </c>
       <c r="C1341" s="31" t="s">
-        <v>3023</v>
+        <v>3020</v>
       </c>
       <c r="D1341" s="29"/>
       <c r="E1341" s="29" t="s">
@@ -44342,7 +44342,7 @@
         <v>1579</v>
       </c>
       <c r="C1342" s="31" t="s">
-        <v>3022</v>
+        <v>3019</v>
       </c>
       <c r="D1342" s="29"/>
       <c r="E1342" s="29" t="s">
@@ -44367,7 +44367,7 @@
         <v>1579</v>
       </c>
       <c r="C1343" s="31" t="s">
-        <v>3024</v>
+        <v>3021</v>
       </c>
       <c r="D1343" s="29"/>
       <c r="E1343" s="29" t="s">
@@ -44392,10 +44392,10 @@
         <v>1579</v>
       </c>
       <c r="C1344" s="31" t="s">
-        <v>2814</v>
+        <v>2813</v>
       </c>
       <c r="D1344" s="29" t="s">
-        <v>2842</v>
+        <v>2840</v>
       </c>
       <c r="E1344" s="29" t="s">
         <v>22</v>
@@ -44419,10 +44419,10 @@
         <v>7</v>
       </c>
       <c r="C1345" s="31" t="s">
-        <v>3000</v>
+        <v>2998</v>
       </c>
       <c r="D1345" s="29" t="s">
-        <v>2842</v>
+        <v>2840</v>
       </c>
       <c r="E1345" s="29" t="s">
         <v>22</v>
@@ -44446,10 +44446,10 @@
         <v>1579</v>
       </c>
       <c r="C1346" s="31" t="s">
-        <v>2815</v>
+        <v>2814</v>
       </c>
       <c r="D1346" s="29" t="s">
-        <v>2843</v>
+        <v>2841</v>
       </c>
       <c r="E1346" s="29" t="s">
         <v>22</v>
@@ -44464,7 +44464,7 @@
         <v>20</v>
       </c>
       <c r="I1346" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1347" spans="1:9" ht="30">
@@ -44475,7 +44475,7 @@
         <v>1579</v>
       </c>
       <c r="C1347" s="31" t="s">
-        <v>3001</v>
+        <v>2999</v>
       </c>
       <c r="D1347" s="29"/>
       <c r="E1347" s="29" t="s">
@@ -44500,7 +44500,7 @@
         <v>1579</v>
       </c>
       <c r="C1348" s="31" t="s">
-        <v>3025</v>
+        <v>3022</v>
       </c>
       <c r="D1348" s="29"/>
       <c r="E1348" s="29" t="s">
@@ -44525,10 +44525,10 @@
         <v>1579</v>
       </c>
       <c r="C1349" s="31" t="s">
-        <v>2816</v>
+        <v>2815</v>
       </c>
       <c r="D1349" s="29" t="s">
-        <v>2843</v>
+        <v>2841</v>
       </c>
       <c r="E1349" s="29" t="s">
         <v>22</v>
@@ -44543,7 +44543,7 @@
         <v>20</v>
       </c>
       <c r="I1349" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1350" spans="1:9" ht="45">
@@ -44554,10 +44554,10 @@
         <v>1579</v>
       </c>
       <c r="C1350" s="31" t="s">
-        <v>2817</v>
+        <v>2816</v>
       </c>
       <c r="D1350" s="29" t="s">
-        <v>2843</v>
+        <v>2841</v>
       </c>
       <c r="E1350" s="29" t="s">
         <v>22</v>
@@ -44572,7 +44572,7 @@
         <v>20</v>
       </c>
       <c r="I1350" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1351" spans="1:9" ht="45">
@@ -44583,10 +44583,10 @@
         <v>1579</v>
       </c>
       <c r="C1351" s="31" t="s">
-        <v>2818</v>
+        <v>2817</v>
       </c>
       <c r="D1351" s="29" t="s">
-        <v>2843</v>
+        <v>2841</v>
       </c>
       <c r="E1351" s="29" t="s">
         <v>22</v>
@@ -44601,7 +44601,7 @@
         <v>20</v>
       </c>
       <c r="I1351" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1352" spans="1:9" ht="45">
@@ -44612,10 +44612,10 @@
         <v>1579</v>
       </c>
       <c r="C1352" s="31" t="s">
-        <v>2819</v>
+        <v>2818</v>
       </c>
       <c r="D1352" s="29" t="s">
-        <v>2843</v>
+        <v>2841</v>
       </c>
       <c r="E1352" s="29" t="s">
         <v>22</v>
@@ -44639,7 +44639,7 @@
         <v>1579</v>
       </c>
       <c r="C1353" s="31" t="s">
-        <v>3026</v>
+        <v>3023</v>
       </c>
       <c r="D1353" s="29"/>
       <c r="E1353" s="29" t="s">
@@ -44664,10 +44664,10 @@
         <v>1579</v>
       </c>
       <c r="C1354" s="31" t="s">
-        <v>2820</v>
+        <v>2819</v>
       </c>
       <c r="D1354" s="29" t="s">
-        <v>2843</v>
+        <v>2841</v>
       </c>
       <c r="E1354" s="29" t="s">
         <v>22</v>
@@ -44682,7 +44682,7 @@
         <v>20</v>
       </c>
       <c r="I1354" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1355" spans="1:9" ht="45">
@@ -44693,7 +44693,7 @@
         <v>1579</v>
       </c>
       <c r="C1355" s="31" t="s">
-        <v>3027</v>
+        <v>3024</v>
       </c>
       <c r="D1355" s="29"/>
       <c r="E1355" s="29" t="s">
@@ -44718,10 +44718,10 @@
         <v>1579</v>
       </c>
       <c r="C1356" s="31" t="s">
-        <v>2821</v>
+        <v>2820</v>
       </c>
       <c r="D1356" s="29" t="s">
-        <v>2844</v>
+        <v>2842</v>
       </c>
       <c r="E1356" s="29" t="s">
         <v>22</v>
@@ -44736,7 +44736,7 @@
         <v>20</v>
       </c>
       <c r="I1356" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1357" spans="1:9" ht="45">
@@ -44747,10 +44747,10 @@
         <v>1579</v>
       </c>
       <c r="C1357" s="31" t="s">
-        <v>3028</v>
+        <v>3025</v>
       </c>
       <c r="D1357" s="29" t="s">
-        <v>2844</v>
+        <v>2842</v>
       </c>
       <c r="E1357" s="29" t="s">
         <v>22</v>
@@ -44774,10 +44774,10 @@
         <v>1579</v>
       </c>
       <c r="C1358" s="31" t="s">
-        <v>3029</v>
+        <v>3026</v>
       </c>
       <c r="D1358" s="29" t="s">
-        <v>2845</v>
+        <v>2843</v>
       </c>
       <c r="E1358" s="29" t="s">
         <v>22</v>
@@ -44801,10 +44801,10 @@
         <v>1579</v>
       </c>
       <c r="C1359" s="31" t="s">
-        <v>2822</v>
+        <v>2821</v>
       </c>
       <c r="D1359" s="29" t="s">
-        <v>2845</v>
+        <v>2843</v>
       </c>
       <c r="E1359" s="29" t="s">
         <v>22</v>
@@ -44819,7 +44819,7 @@
         <v>20</v>
       </c>
       <c r="I1359" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1360" spans="1:9" ht="60">
@@ -44830,10 +44830,10 @@
         <v>1579</v>
       </c>
       <c r="C1360" s="31" t="s">
-        <v>3002</v>
+        <v>3000</v>
       </c>
       <c r="D1360" s="29" t="s">
-        <v>2845</v>
+        <v>2843</v>
       </c>
       <c r="E1360" s="29" t="s">
         <v>22</v>
@@ -44857,10 +44857,10 @@
         <v>1579</v>
       </c>
       <c r="C1361" s="31" t="s">
-        <v>3030</v>
+        <v>3027</v>
       </c>
       <c r="D1361" s="29" t="s">
-        <v>2845</v>
+        <v>2843</v>
       </c>
       <c r="E1361" s="29" t="s">
         <v>22</v>
@@ -44875,7 +44875,7 @@
         <v>20</v>
       </c>
       <c r="I1361" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1362" spans="1:9" ht="60">
@@ -44886,7 +44886,7 @@
         <v>1579</v>
       </c>
       <c r="C1362" s="31" t="s">
-        <v>3031</v>
+        <v>3028</v>
       </c>
       <c r="D1362" s="29"/>
       <c r="E1362" s="29" t="s">
@@ -44911,10 +44911,10 @@
         <v>1579</v>
       </c>
       <c r="C1363" s="31" t="s">
-        <v>3032</v>
+        <v>3029</v>
       </c>
       <c r="D1363" s="29" t="s">
-        <v>2846</v>
+        <v>2844</v>
       </c>
       <c r="E1363" s="29" t="s">
         <v>22</v>
@@ -44938,10 +44938,10 @@
         <v>1579</v>
       </c>
       <c r="C1364" s="31" t="s">
-        <v>2823</v>
+        <v>2822</v>
       </c>
       <c r="D1364" s="29" t="s">
-        <v>2846</v>
+        <v>2844</v>
       </c>
       <c r="E1364" s="29" t="s">
         <v>22</v>
@@ -44956,7 +44956,7 @@
         <v>20</v>
       </c>
       <c r="I1364" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1365" spans="1:9" ht="45">
@@ -44967,10 +44967,10 @@
         <v>1579</v>
       </c>
       <c r="C1365" s="31" t="s">
-        <v>3033</v>
+        <v>3030</v>
       </c>
       <c r="D1365" s="29" t="s">
-        <v>2847</v>
+        <v>2845</v>
       </c>
       <c r="E1365" s="29" t="s">
         <v>22</v>
@@ -44994,10 +44994,10 @@
         <v>1579</v>
       </c>
       <c r="C1366" s="31" t="s">
-        <v>2824</v>
+        <v>2823</v>
       </c>
       <c r="D1366" s="29" t="s">
-        <v>2847</v>
+        <v>2845</v>
       </c>
       <c r="E1366" s="29" t="s">
         <v>22</v>
@@ -45012,7 +45012,7 @@
         <v>20</v>
       </c>
       <c r="I1366" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1367" spans="1:9" ht="90">
@@ -45023,10 +45023,10 @@
         <v>1579</v>
       </c>
       <c r="C1367" s="31" t="s">
-        <v>3003</v>
+        <v>3001</v>
       </c>
       <c r="D1367" s="29" t="s">
-        <v>2847</v>
+        <v>2845</v>
       </c>
       <c r="E1367" s="29" t="s">
         <v>22</v>
@@ -45041,7 +45041,7 @@
         <v>20</v>
       </c>
       <c r="I1367" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1368" spans="1:9" ht="60">
@@ -45052,10 +45052,10 @@
         <v>1579</v>
       </c>
       <c r="C1368" s="31" t="s">
-        <v>3004</v>
+        <v>3002</v>
       </c>
       <c r="D1368" s="29" t="s">
-        <v>2847</v>
+        <v>2845</v>
       </c>
       <c r="E1368" s="29" t="s">
         <v>22</v>
@@ -45079,10 +45079,10 @@
         <v>1579</v>
       </c>
       <c r="C1369" s="31" t="s">
-        <v>3005</v>
+        <v>3003</v>
       </c>
       <c r="D1369" s="29" t="s">
-        <v>2848</v>
+        <v>2846</v>
       </c>
       <c r="E1369" s="29" t="s">
         <v>22</v>
@@ -45097,7 +45097,7 @@
         <v>20</v>
       </c>
       <c r="I1369" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1370" spans="1:9" ht="45">
@@ -45108,10 +45108,10 @@
         <v>1579</v>
       </c>
       <c r="C1370" s="31" t="s">
-        <v>2825</v>
+        <v>2824</v>
       </c>
       <c r="D1370" s="29" t="s">
-        <v>2848</v>
+        <v>2846</v>
       </c>
       <c r="E1370" s="29" t="s">
         <v>22</v>
@@ -45126,7 +45126,7 @@
         <v>20</v>
       </c>
       <c r="I1370" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1371" spans="1:9" ht="60">
@@ -45137,7 +45137,7 @@
         <v>1579</v>
       </c>
       <c r="C1371" s="31" t="s">
-        <v>3006</v>
+        <v>3004</v>
       </c>
       <c r="D1371" s="29"/>
       <c r="E1371" s="29" t="s">
@@ -45162,10 +45162,10 @@
         <v>1579</v>
       </c>
       <c r="C1372" s="31" t="s">
-        <v>3007</v>
+        <v>3005</v>
       </c>
       <c r="D1372" s="29" t="s">
-        <v>2849</v>
+        <v>2847</v>
       </c>
       <c r="E1372" s="29" t="s">
         <v>22</v>
@@ -45180,7 +45180,7 @@
         <v>20</v>
       </c>
       <c r="I1372" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1373" spans="1:9" ht="45">
@@ -45191,10 +45191,10 @@
         <v>1579</v>
       </c>
       <c r="C1373" s="31" t="s">
-        <v>2826</v>
+        <v>2825</v>
       </c>
       <c r="D1373" s="29" t="s">
-        <v>2849</v>
+        <v>2847</v>
       </c>
       <c r="E1373" s="29" t="s">
         <v>22</v>
@@ -45209,7 +45209,7 @@
         <v>20</v>
       </c>
       <c r="I1373" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1374" spans="1:9" ht="45">
@@ -45220,10 +45220,10 @@
         <v>1579</v>
       </c>
       <c r="C1374" s="31" t="s">
-        <v>3008</v>
+        <v>3006</v>
       </c>
       <c r="D1374" s="29" t="s">
-        <v>2850</v>
+        <v>2848</v>
       </c>
       <c r="E1374" s="29" t="s">
         <v>22</v>
@@ -45238,7 +45238,7 @@
         <v>20</v>
       </c>
       <c r="I1374" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1375" spans="1:9" ht="45">
@@ -45249,7 +45249,7 @@
         <v>1579</v>
       </c>
       <c r="C1375" s="31" t="s">
-        <v>3009</v>
+        <v>3007</v>
       </c>
       <c r="D1375" s="29"/>
       <c r="E1375" s="29" t="s">
@@ -45274,10 +45274,10 @@
         <v>1579</v>
       </c>
       <c r="C1376" s="31" t="s">
-        <v>3010</v>
+        <v>3008</v>
       </c>
       <c r="D1376" s="29" t="s">
-        <v>2850</v>
+        <v>2848</v>
       </c>
       <c r="E1376" s="29" t="s">
         <v>22</v>
@@ -45292,7 +45292,7 @@
         <v>20</v>
       </c>
       <c r="I1376" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1377" spans="1:9" ht="45">
@@ -45303,10 +45303,10 @@
         <v>1579</v>
       </c>
       <c r="C1377" s="31" t="s">
-        <v>3034</v>
+        <v>3031</v>
       </c>
       <c r="D1377" s="29" t="s">
-        <v>2851</v>
+        <v>2849</v>
       </c>
       <c r="E1377" s="29" t="s">
         <v>22</v>
@@ -45321,7 +45321,7 @@
         <v>21</v>
       </c>
       <c r="I1377" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1378" spans="1:9" ht="45">
@@ -45332,10 +45332,10 @@
         <v>1579</v>
       </c>
       <c r="C1378" s="31" t="s">
-        <v>2827</v>
+        <v>2826</v>
       </c>
       <c r="D1378" s="29" t="s">
-        <v>2851</v>
+        <v>2849</v>
       </c>
       <c r="E1378" s="29" t="s">
         <v>22</v>
@@ -45350,7 +45350,7 @@
         <v>21</v>
       </c>
       <c r="I1378" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1379" spans="1:9" ht="45">
@@ -45361,10 +45361,10 @@
         <v>1579</v>
       </c>
       <c r="C1379" s="31" t="s">
-        <v>2828</v>
+        <v>2827</v>
       </c>
       <c r="D1379" s="29" t="s">
-        <v>2852</v>
+        <v>2850</v>
       </c>
       <c r="E1379" s="29" t="s">
         <v>22</v>
@@ -45379,7 +45379,7 @@
         <v>21</v>
       </c>
       <c r="I1379" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1380" spans="1:9" ht="30">
@@ -45390,7 +45390,7 @@
         <v>1579</v>
       </c>
       <c r="C1380" s="31" t="s">
-        <v>3011</v>
+        <v>3009</v>
       </c>
       <c r="D1380" s="29"/>
       <c r="E1380" s="29" t="s">
@@ -45415,7 +45415,7 @@
         <v>1579</v>
       </c>
       <c r="C1381" s="31" t="s">
-        <v>3012</v>
+        <v>3010</v>
       </c>
       <c r="D1381" s="29"/>
       <c r="E1381" s="29" t="s">
@@ -45440,10 +45440,10 @@
         <v>1579</v>
       </c>
       <c r="C1382" s="31" t="s">
-        <v>3014</v>
+        <v>3012</v>
       </c>
       <c r="D1382" s="29" t="s">
-        <v>2853</v>
+        <v>2851</v>
       </c>
       <c r="E1382" s="29" t="s">
         <v>22</v>
@@ -45458,7 +45458,7 @@
         <v>21</v>
       </c>
       <c r="I1382" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1383" spans="1:9" ht="45">
@@ -45469,10 +45469,10 @@
         <v>1579</v>
       </c>
       <c r="C1383" s="31" t="s">
-        <v>3013</v>
+        <v>3011</v>
       </c>
       <c r="D1383" s="29" t="s">
-        <v>2853</v>
+        <v>2851</v>
       </c>
       <c r="E1383" s="29" t="s">
         <v>22</v>
@@ -45487,7 +45487,7 @@
         <v>21</v>
       </c>
       <c r="I1383" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1384" spans="1:9" ht="60">
@@ -45498,10 +45498,10 @@
         <v>1579</v>
       </c>
       <c r="C1384" s="31" t="s">
-        <v>3015</v>
+        <v>3013</v>
       </c>
       <c r="D1384" s="29" t="s">
-        <v>2854</v>
+        <v>2852</v>
       </c>
       <c r="E1384" s="29" t="s">
         <v>22</v>
@@ -45516,21 +45516,21 @@
         <v>20</v>
       </c>
       <c r="I1384" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1385" spans="1:9" ht="75">
       <c r="A1385" s="29" t="s">
-        <v>3017</v>
+        <v>3014</v>
       </c>
       <c r="B1385" s="33">
         <v>7</v>
       </c>
       <c r="C1385" s="31" t="s">
-        <v>3018</v>
+        <v>3015</v>
       </c>
       <c r="D1385" s="29" t="s">
-        <v>2854</v>
+        <v>2852</v>
       </c>
       <c r="E1385" s="29" t="s">
         <v>22</v>
@@ -45545,10 +45545,10 @@
         <v>20</v>
       </c>
       <c r="I1385" s="31" t="s">
-        <v>2935</v>
-      </c>
-    </row>
-    <row r="1386" spans="1:9" ht="45">
+        <v>2933</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:9" ht="60">
       <c r="A1386" s="29" t="s">
         <v>1408</v>
       </c>
@@ -45556,10 +45556,10 @@
         <v>1579</v>
       </c>
       <c r="C1386" s="31" t="s">
-        <v>3016</v>
+        <v>3089</v>
       </c>
       <c r="D1386" s="29" t="s">
-        <v>2854</v>
+        <v>2852</v>
       </c>
       <c r="E1386" s="29" t="s">
         <v>22</v>
@@ -45574,7 +45574,7 @@
         <v>20</v>
       </c>
       <c r="I1386" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1387" spans="1:9" ht="60">
@@ -45585,10 +45585,10 @@
         <v>1579</v>
       </c>
       <c r="C1387" s="31" t="s">
-        <v>3019</v>
+        <v>3016</v>
       </c>
       <c r="D1387" s="29" t="s">
-        <v>2855</v>
+        <v>2853</v>
       </c>
       <c r="E1387" s="29" t="s">
         <v>22</v>
@@ -45603,7 +45603,7 @@
         <v>20</v>
       </c>
       <c r="I1387" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1388" spans="1:9" ht="45">
@@ -45614,10 +45614,10 @@
         <v>1579</v>
       </c>
       <c r="C1388" s="31" t="s">
-        <v>2940</v>
+        <v>2938</v>
       </c>
       <c r="D1388" s="29" t="s">
-        <v>2855</v>
+        <v>2853</v>
       </c>
       <c r="E1388" s="29" t="s">
         <v>22</v>
@@ -45632,7 +45632,7 @@
         <v>20</v>
       </c>
       <c r="I1388" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1389" spans="1:9" ht="45">
@@ -45643,10 +45643,10 @@
         <v>1579</v>
       </c>
       <c r="C1389" s="31" t="s">
-        <v>3020</v>
+        <v>3017</v>
       </c>
       <c r="D1389" s="29" t="s">
-        <v>2855</v>
+        <v>2853</v>
       </c>
       <c r="E1389" s="29" t="s">
         <v>22</v>
@@ -45670,10 +45670,10 @@
         <v>1579</v>
       </c>
       <c r="C1390" s="31" t="s">
-        <v>2829</v>
+        <v>3088</v>
       </c>
       <c r="D1390" s="29" t="s">
-        <v>2856</v>
+        <v>2854</v>
       </c>
       <c r="E1390" s="29" t="s">
         <v>22</v>
@@ -45688,7 +45688,7 @@
         <v>20</v>
       </c>
       <c r="I1390" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1391" spans="1:9" ht="45">
@@ -45699,10 +45699,10 @@
         <v>1579</v>
       </c>
       <c r="C1391" s="31" t="s">
-        <v>2830</v>
+        <v>2828</v>
       </c>
       <c r="D1391" s="29" t="s">
-        <v>2856</v>
+        <v>2854</v>
       </c>
       <c r="E1391" s="29" t="s">
         <v>22</v>
@@ -45717,21 +45717,21 @@
         <v>20</v>
       </c>
       <c r="I1391" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1392" spans="1:9" ht="45">
       <c r="A1392" s="29" t="s">
-        <v>3035</v>
+        <v>3032</v>
       </c>
       <c r="B1392" s="33">
         <v>7</v>
       </c>
       <c r="C1392" s="31" t="s">
-        <v>3036</v>
+        <v>3033</v>
       </c>
       <c r="D1392" s="29" t="s">
-        <v>2856</v>
+        <v>2854</v>
       </c>
       <c r="E1392" s="29" t="s">
         <v>22</v>
@@ -45746,7 +45746,7 @@
         <v>20</v>
       </c>
       <c r="I1392" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1393" spans="1:9" ht="45">
@@ -45757,10 +45757,10 @@
         <v>1579</v>
       </c>
       <c r="C1393" s="31" t="s">
-        <v>3037</v>
+        <v>3034</v>
       </c>
       <c r="D1393" s="29" t="s">
-        <v>2857</v>
+        <v>2855</v>
       </c>
       <c r="E1393" s="29" t="s">
         <v>22</v>
@@ -45775,7 +45775,7 @@
         <v>20</v>
       </c>
       <c r="I1393" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1394" spans="1:9" ht="45">
@@ -45786,10 +45786,10 @@
         <v>1579</v>
       </c>
       <c r="C1394" s="31" t="s">
-        <v>3038</v>
+        <v>3035</v>
       </c>
       <c r="D1394" s="29" t="s">
-        <v>2857</v>
+        <v>2855</v>
       </c>
       <c r="E1394" s="29" t="s">
         <v>22</v>
@@ -45804,7 +45804,7 @@
         <v>20</v>
       </c>
       <c r="I1394" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1395" spans="1:9" ht="45">
@@ -45815,10 +45815,10 @@
         <v>1579</v>
       </c>
       <c r="C1395" s="31" t="s">
-        <v>3039</v>
+        <v>3036</v>
       </c>
       <c r="D1395" s="29" t="s">
-        <v>2857</v>
+        <v>2855</v>
       </c>
       <c r="E1395" s="29" t="s">
         <v>22</v>
@@ -45833,7 +45833,7 @@
         <v>20</v>
       </c>
       <c r="I1395" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1396" spans="1:9" ht="45">
@@ -45844,10 +45844,10 @@
         <v>1579</v>
       </c>
       <c r="C1396" s="31" t="s">
-        <v>3040</v>
+        <v>3037</v>
       </c>
       <c r="D1396" s="29" t="s">
-        <v>2858</v>
+        <v>2856</v>
       </c>
       <c r="E1396" s="29" t="s">
         <v>22</v>
@@ -45862,7 +45862,7 @@
         <v>21</v>
       </c>
       <c r="I1396" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1397" spans="1:9" ht="45">
@@ -45873,10 +45873,10 @@
         <v>1579</v>
       </c>
       <c r="C1397" s="31" t="s">
-        <v>3041</v>
+        <v>3038</v>
       </c>
       <c r="D1397" s="29" t="s">
-        <v>2858</v>
+        <v>2856</v>
       </c>
       <c r="E1397" s="29" t="s">
         <v>22</v>
@@ -45891,7 +45891,7 @@
         <v>21</v>
       </c>
       <c r="I1397" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1398" spans="1:9" ht="45">
@@ -45902,10 +45902,10 @@
         <v>1579</v>
       </c>
       <c r="C1398" s="31" t="s">
-        <v>2831</v>
+        <v>2829</v>
       </c>
       <c r="D1398" s="29" t="s">
-        <v>2859</v>
+        <v>2857</v>
       </c>
       <c r="E1398" s="29" t="s">
         <v>22</v>
@@ -45920,7 +45920,7 @@
         <v>20</v>
       </c>
       <c r="I1398" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1399" spans="1:9" ht="45">
@@ -45931,10 +45931,10 @@
         <v>1579</v>
       </c>
       <c r="C1399" s="31" t="s">
-        <v>3042</v>
+        <v>3039</v>
       </c>
       <c r="D1399" s="29" t="s">
-        <v>2859</v>
+        <v>2857</v>
       </c>
       <c r="E1399" s="29" t="s">
         <v>22</v>
@@ -45949,7 +45949,7 @@
         <v>20</v>
       </c>
       <c r="I1399" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1400" spans="1:9" ht="60">
@@ -45960,10 +45960,10 @@
         <v>1579</v>
       </c>
       <c r="C1400" s="31" t="s">
-        <v>3043</v>
+        <v>3040</v>
       </c>
       <c r="D1400" s="29" t="s">
-        <v>2860</v>
+        <v>2858</v>
       </c>
       <c r="E1400" s="29" t="s">
         <v>22</v>
@@ -45978,7 +45978,7 @@
         <v>20</v>
       </c>
       <c r="I1400" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1401" spans="1:9" ht="45">
@@ -45989,10 +45989,10 @@
         <v>1579</v>
       </c>
       <c r="C1401" s="31" t="s">
-        <v>2832</v>
+        <v>2830</v>
       </c>
       <c r="D1401" s="29" t="s">
-        <v>2860</v>
+        <v>2858</v>
       </c>
       <c r="E1401" s="29" t="s">
         <v>22</v>
@@ -46007,7 +46007,7 @@
         <v>20</v>
       </c>
       <c r="I1401" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1402" spans="1:9" ht="45">
@@ -46018,10 +46018,10 @@
         <v>1579</v>
       </c>
       <c r="C1402" s="31" t="s">
-        <v>3044</v>
+        <v>3041</v>
       </c>
       <c r="D1402" s="29" t="s">
-        <v>2861</v>
+        <v>2859</v>
       </c>
       <c r="E1402" s="29" t="s">
         <v>22</v>
@@ -46036,7 +46036,7 @@
         <v>17</v>
       </c>
       <c r="I1402" s="31" t="s">
-        <v>2938</v>
+        <v>2936</v>
       </c>
     </row>
     <row r="1403" spans="1:9" ht="45">
@@ -46047,10 +46047,10 @@
         <v>1579</v>
       </c>
       <c r="C1403" s="31" t="s">
-        <v>3045</v>
+        <v>3042</v>
       </c>
       <c r="D1403" s="29" t="s">
-        <v>2861</v>
+        <v>2859</v>
       </c>
       <c r="E1403" s="29" t="s">
         <v>22</v>
@@ -46074,10 +46074,10 @@
         <v>1579</v>
       </c>
       <c r="C1404" s="31" t="s">
-        <v>3046</v>
+        <v>3043</v>
       </c>
       <c r="D1404" s="29" t="s">
-        <v>2861</v>
+        <v>2859</v>
       </c>
       <c r="E1404" s="29" t="s">
         <v>22</v>
@@ -46092,7 +46092,7 @@
         <v>20</v>
       </c>
       <c r="I1404" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1405" spans="1:9" ht="60">
@@ -46103,10 +46103,10 @@
         <v>1579</v>
       </c>
       <c r="C1405" s="31" t="s">
-        <v>3047</v>
+        <v>3044</v>
       </c>
       <c r="D1405" s="29" t="s">
-        <v>2861</v>
+        <v>2859</v>
       </c>
       <c r="E1405" s="29" t="s">
         <v>22</v>
@@ -46121,7 +46121,7 @@
         <v>20</v>
       </c>
       <c r="I1405" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1406" spans="1:9" ht="45">
@@ -46132,7 +46132,7 @@
         <v>1579</v>
       </c>
       <c r="C1406" s="31" t="s">
-        <v>3048</v>
+        <v>3045</v>
       </c>
       <c r="D1406" s="29"/>
       <c r="E1406" s="29" t="s">
@@ -46157,7 +46157,7 @@
         <v>1579</v>
       </c>
       <c r="C1407" s="31" t="s">
-        <v>3049</v>
+        <v>3046</v>
       </c>
       <c r="D1407" s="29"/>
       <c r="E1407" s="29" t="s">
@@ -46182,7 +46182,7 @@
         <v>1579</v>
       </c>
       <c r="C1408" s="31" t="s">
-        <v>3050</v>
+        <v>3047</v>
       </c>
       <c r="D1408" s="29"/>
       <c r="E1408" s="29" t="s">
@@ -46207,7 +46207,7 @@
         <v>1579</v>
       </c>
       <c r="C1409" s="31" t="s">
-        <v>3051</v>
+        <v>3048</v>
       </c>
       <c r="D1409" s="29"/>
       <c r="E1409" s="29" t="s">
@@ -46232,7 +46232,7 @@
         <v>1579</v>
       </c>
       <c r="C1410" s="31" t="s">
-        <v>3052</v>
+        <v>3049</v>
       </c>
       <c r="D1410" s="29"/>
       <c r="E1410" s="29" t="s">
@@ -46257,7 +46257,7 @@
         <v>1579</v>
       </c>
       <c r="C1411" s="31" t="s">
-        <v>3053</v>
+        <v>3050</v>
       </c>
       <c r="D1411" s="29"/>
       <c r="E1411" s="29" t="s">
@@ -46282,7 +46282,7 @@
         <v>1579</v>
       </c>
       <c r="C1412" s="31" t="s">
-        <v>3054</v>
+        <v>3051</v>
       </c>
       <c r="D1412" s="29"/>
       <c r="E1412" s="29" t="s">
@@ -46307,7 +46307,7 @@
         <v>1579</v>
       </c>
       <c r="C1413" s="31" t="s">
-        <v>3055</v>
+        <v>3052</v>
       </c>
       <c r="D1413" s="29"/>
       <c r="E1413" s="29" t="s">
@@ -46332,7 +46332,7 @@
         <v>1579</v>
       </c>
       <c r="C1414" s="31" t="s">
-        <v>3056</v>
+        <v>3053</v>
       </c>
       <c r="D1414" s="29"/>
       <c r="E1414" s="29" t="s">
@@ -46357,7 +46357,7 @@
         <v>1579</v>
       </c>
       <c r="C1415" s="31" t="s">
-        <v>3057</v>
+        <v>3054</v>
       </c>
       <c r="D1415" s="29"/>
       <c r="E1415" s="29" t="s">
@@ -46382,7 +46382,7 @@
         <v>1579</v>
       </c>
       <c r="C1416" s="31" t="s">
-        <v>3058</v>
+        <v>3055</v>
       </c>
       <c r="D1416" s="29"/>
       <c r="E1416" s="29" t="s">
@@ -46407,7 +46407,7 @@
         <v>1579</v>
       </c>
       <c r="C1417" s="31" t="s">
-        <v>3059</v>
+        <v>3056</v>
       </c>
       <c r="D1417" s="29"/>
       <c r="E1417" s="29" t="s">
@@ -46432,7 +46432,7 @@
         <v>1579</v>
       </c>
       <c r="C1418" s="31" t="s">
-        <v>3060</v>
+        <v>3057</v>
       </c>
       <c r="D1418" s="29"/>
       <c r="E1418" s="29" t="s">
@@ -46457,7 +46457,7 @@
         <v>1579</v>
       </c>
       <c r="C1419" s="31" t="s">
-        <v>3063</v>
+        <v>3060</v>
       </c>
       <c r="D1419" s="29"/>
       <c r="E1419" s="29" t="s">
@@ -46482,7 +46482,7 @@
         <v>1579</v>
       </c>
       <c r="C1420" s="31" t="s">
-        <v>3061</v>
+        <v>3058</v>
       </c>
       <c r="D1420" s="29"/>
       <c r="E1420" s="29" t="s">
@@ -46507,7 +46507,7 @@
         <v>1579</v>
       </c>
       <c r="C1421" s="31" t="s">
-        <v>3062</v>
+        <v>3059</v>
       </c>
       <c r="D1421" s="29"/>
       <c r="E1421" s="29" t="s">
@@ -46532,7 +46532,7 @@
         <v>1579</v>
       </c>
       <c r="C1422" s="31" t="s">
-        <v>3064</v>
+        <v>3061</v>
       </c>
       <c r="D1422" s="29"/>
       <c r="E1422" s="29" t="s">
@@ -46557,7 +46557,7 @@
         <v>1579</v>
       </c>
       <c r="C1423" s="31" t="s">
-        <v>3065</v>
+        <v>3062</v>
       </c>
       <c r="D1423" s="29"/>
       <c r="E1423" s="29" t="s">
@@ -46582,7 +46582,7 @@
         <v>1579</v>
       </c>
       <c r="C1424" s="31" t="s">
-        <v>3066</v>
+        <v>3063</v>
       </c>
       <c r="D1424" s="29"/>
       <c r="E1424" s="29" t="s">
@@ -46607,7 +46607,7 @@
         <v>1579</v>
       </c>
       <c r="C1425" s="31" t="s">
-        <v>3067</v>
+        <v>3064</v>
       </c>
       <c r="D1425" s="29"/>
       <c r="E1425" s="29" t="s">
@@ -46632,7 +46632,7 @@
         <v>1579</v>
       </c>
       <c r="C1426" s="31" t="s">
-        <v>3068</v>
+        <v>3065</v>
       </c>
       <c r="D1426" s="29"/>
       <c r="E1426" s="29" t="s">
@@ -46657,7 +46657,7 @@
         <v>1579</v>
       </c>
       <c r="C1427" s="31" t="s">
-        <v>3069</v>
+        <v>3066</v>
       </c>
       <c r="D1427" s="29"/>
       <c r="E1427" s="29" t="s">
@@ -46682,7 +46682,7 @@
         <v>1579</v>
       </c>
       <c r="C1428" s="31" t="s">
-        <v>3070</v>
+        <v>3067</v>
       </c>
       <c r="D1428" s="29"/>
       <c r="E1428" s="29" t="s">
@@ -46707,7 +46707,7 @@
         <v>1579</v>
       </c>
       <c r="C1429" s="31" t="s">
-        <v>3071</v>
+        <v>3068</v>
       </c>
       <c r="D1429" s="29"/>
       <c r="E1429" s="29" t="s">
@@ -46732,7 +46732,7 @@
         <v>1579</v>
       </c>
       <c r="C1430" s="31" t="s">
-        <v>3072</v>
+        <v>3069</v>
       </c>
       <c r="D1430" s="29"/>
       <c r="E1430" s="29" t="s">
@@ -46757,7 +46757,7 @@
         <v>1579</v>
       </c>
       <c r="C1431" s="31" t="s">
-        <v>3073</v>
+        <v>3070</v>
       </c>
       <c r="D1431" s="29"/>
       <c r="E1431" s="29" t="s">
@@ -46782,7 +46782,7 @@
         <v>1579</v>
       </c>
       <c r="C1432" s="31" t="s">
-        <v>3074</v>
+        <v>3071</v>
       </c>
       <c r="D1432" s="29"/>
       <c r="E1432" s="29" t="s">
@@ -46807,7 +46807,7 @@
         <v>1579</v>
       </c>
       <c r="C1433" s="31" t="s">
-        <v>3075</v>
+        <v>3072</v>
       </c>
       <c r="D1433" s="29"/>
       <c r="E1433" s="29" t="s">
@@ -46832,7 +46832,7 @@
         <v>1579</v>
       </c>
       <c r="C1434" s="31" t="s">
-        <v>3076</v>
+        <v>3073</v>
       </c>
       <c r="D1434" s="29"/>
       <c r="E1434" s="29" t="s">
@@ -46857,7 +46857,7 @@
         <v>1579</v>
       </c>
       <c r="C1435" s="31" t="s">
-        <v>3077</v>
+        <v>3074</v>
       </c>
       <c r="D1435" s="29"/>
       <c r="E1435" s="29" t="s">
@@ -46882,7 +46882,7 @@
         <v>1579</v>
       </c>
       <c r="C1436" s="31" t="s">
-        <v>3078</v>
+        <v>3075</v>
       </c>
       <c r="D1436" s="29"/>
       <c r="E1436" s="29" t="s">
@@ -46907,7 +46907,7 @@
         <v>1579</v>
       </c>
       <c r="C1437" s="31" t="s">
-        <v>3079</v>
+        <v>3076</v>
       </c>
       <c r="D1437" s="29"/>
       <c r="E1437" s="29" t="s">
@@ -46932,7 +46932,7 @@
         <v>1579</v>
       </c>
       <c r="C1438" s="31" t="s">
-        <v>3080</v>
+        <v>3077</v>
       </c>
       <c r="D1438" s="29"/>
       <c r="E1438" s="29" t="s">
@@ -46957,7 +46957,7 @@
         <v>1579</v>
       </c>
       <c r="C1439" s="31" t="s">
-        <v>3081</v>
+        <v>3078</v>
       </c>
       <c r="D1439" s="29"/>
       <c r="E1439" s="29" t="s">
@@ -46982,7 +46982,7 @@
         <v>1579</v>
       </c>
       <c r="C1440" s="31" t="s">
-        <v>3082</v>
+        <v>3079</v>
       </c>
       <c r="D1440" s="29"/>
       <c r="E1440" s="29" t="s">
@@ -47007,10 +47007,10 @@
         <v>1579</v>
       </c>
       <c r="C1441" s="31" t="s">
-        <v>3083</v>
+        <v>3080</v>
       </c>
       <c r="D1441" s="29" t="s">
-        <v>2862</v>
+        <v>2860</v>
       </c>
       <c r="E1441" s="29" t="s">
         <v>22</v>
@@ -47025,7 +47025,7 @@
         <v>20</v>
       </c>
       <c r="I1441" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1442" spans="1:9" ht="60">
@@ -47036,10 +47036,10 @@
         <v>1579</v>
       </c>
       <c r="C1442" s="31" t="s">
-        <v>3088</v>
+        <v>3085</v>
       </c>
       <c r="D1442" s="29" t="s">
-        <v>2863</v>
+        <v>2861</v>
       </c>
       <c r="E1442" s="29" t="s">
         <v>22</v>
@@ -47054,7 +47054,7 @@
         <v>20</v>
       </c>
       <c r="I1442" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1443" spans="1:9" ht="60">
@@ -47065,10 +47065,10 @@
         <v>1579</v>
       </c>
       <c r="C1443" s="31" t="s">
-        <v>3084</v>
+        <v>3081</v>
       </c>
       <c r="D1443" s="29" t="s">
-        <v>2863</v>
+        <v>2861</v>
       </c>
       <c r="E1443" s="29" t="s">
         <v>22</v>
@@ -47083,7 +47083,7 @@
         <v>20</v>
       </c>
       <c r="I1443" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1444" spans="1:9" ht="45">
@@ -47094,7 +47094,7 @@
         <v>1579</v>
       </c>
       <c r="C1444" s="31" t="s">
-        <v>3085</v>
+        <v>3082</v>
       </c>
       <c r="D1444" s="29"/>
       <c r="E1444" s="29" t="s">
@@ -47110,7 +47110,7 @@
         <v>20</v>
       </c>
       <c r="I1444" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1445" spans="1:9" ht="30">
@@ -47121,7 +47121,7 @@
         <v>1579</v>
       </c>
       <c r="C1445" s="31" t="s">
-        <v>3086</v>
+        <v>3083</v>
       </c>
       <c r="D1445" s="29"/>
       <c r="E1445" s="29" t="s">
@@ -47146,7 +47146,7 @@
         <v>1579</v>
       </c>
       <c r="C1446" s="31" t="s">
-        <v>3087</v>
+        <v>3084</v>
       </c>
       <c r="D1446" s="29"/>
       <c r="E1446" s="29" t="s">
@@ -47251,6 +47251,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -47299,37 +47314,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -47343,10 +47328,25 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MS-OXCROPS]: Update as blocked TDI. Format RS.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCRPC/MS-OXCRPC_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCRPC/MS-OXCRPC_RequirementSpecification.xlsx
@@ -9539,16 +9539,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="177" formatCode="0.0.0"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="0.0.0"/>
   </numFmts>
   <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -9744,13 +9744,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -9783,7 +9783,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -9851,367 +9851,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="99">
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
+  <dxfs count="27">
     <dxf>
       <font>
         <b val="0"/>
@@ -10723,34 +10363,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I1446" tableType="xml" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I1446" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
   <autoFilter ref="A19:I1446"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="88">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="87">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="86">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="85">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="84">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="83">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="82">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="81">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="80">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -10759,12 +10399,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="79" dataDxfId="77" headerRowBorderDxfId="78" tableBorderDxfId="76" totalsRowBorderDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="74"/>
-    <tableColumn id="2" name="Test" dataDxfId="73"/>
-    <tableColumn id="3" name="Description" dataDxfId="72"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11064,15 +10704,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.375" style="11" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
     <col min="10" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
@@ -11387,7 +11027,7 @@
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:12" s="23" customFormat="1" ht="45">
+    <row r="20" spans="1:12" s="23" customFormat="1" ht="60">
       <c r="A20" s="22" t="s">
         <v>43</v>
       </c>
@@ -11439,7 +11079,7 @@
       </c>
       <c r="I21" s="24"/>
     </row>
-    <row r="22" spans="1:12" s="23" customFormat="1">
+    <row r="22" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A22" s="22" t="s">
         <v>45</v>
       </c>
@@ -11564,7 +11204,7 @@
       </c>
       <c r="I26" s="24"/>
     </row>
-    <row r="27" spans="1:12" s="23" customFormat="1" ht="150">
+    <row r="27" spans="1:12" s="23" customFormat="1" ht="165">
       <c r="A27" s="22" t="s">
         <v>50</v>
       </c>
@@ -11589,7 +11229,7 @@
       </c>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="1:12" s="23" customFormat="1" ht="135">
+    <row r="28" spans="1:12" s="23" customFormat="1" ht="165">
       <c r="A28" s="22" t="s">
         <v>51</v>
       </c>
@@ -11614,7 +11254,7 @@
       </c>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="1:12" s="23" customFormat="1">
+    <row r="29" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A29" s="22" t="s">
         <v>52</v>
       </c>
@@ -11689,7 +11329,7 @@
       </c>
       <c r="I31" s="24"/>
     </row>
-    <row r="32" spans="1:12" s="23" customFormat="1" ht="60">
+    <row r="32" spans="1:12" s="23" customFormat="1" ht="75">
       <c r="A32" s="22" t="s">
         <v>55</v>
       </c>
@@ -12118,7 +11758,7 @@
       </c>
       <c r="I48" s="31"/>
     </row>
-    <row r="49" spans="1:9" ht="45">
+    <row r="49" spans="1:9" ht="60">
       <c r="A49" s="29" t="s">
         <v>72</v>
       </c>
@@ -12328,7 +11968,7 @@
         <v>2866</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="45">
+    <row r="57" spans="1:9" ht="60">
       <c r="A57" s="29" t="s">
         <v>80</v>
       </c>
@@ -12382,7 +12022,7 @@
         <v>2868</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="45">
+    <row r="59" spans="1:9" ht="60">
       <c r="A59" s="29" t="s">
         <v>82</v>
       </c>
@@ -12409,7 +12049,7 @@
         <v>2867</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="45">
+    <row r="60" spans="1:9" ht="60">
       <c r="A60" s="29" t="s">
         <v>83</v>
       </c>
@@ -12436,7 +12076,7 @@
         <v>2867</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="45">
+    <row r="61" spans="1:9" ht="60">
       <c r="A61" s="29" t="s">
         <v>84</v>
       </c>
@@ -12463,7 +12103,7 @@
         <v>2867</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="45">
+    <row r="62" spans="1:9" ht="60">
       <c r="A62" s="29" t="s">
         <v>85</v>
       </c>
@@ -12490,7 +12130,7 @@
         <v>2867</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="30">
+    <row r="63" spans="1:9" ht="45">
       <c r="A63" s="29" t="s">
         <v>86</v>
       </c>
@@ -12565,7 +12205,7 @@
       </c>
       <c r="I65" s="31"/>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" ht="30">
       <c r="A66" s="29" t="s">
         <v>89</v>
       </c>
@@ -12590,7 +12230,7 @@
       </c>
       <c r="I66" s="31"/>
     </row>
-    <row r="67" spans="1:9" ht="225">
+    <row r="67" spans="1:9" ht="255">
       <c r="A67" s="29" t="s">
         <v>90</v>
       </c>
@@ -12615,7 +12255,7 @@
       </c>
       <c r="I67" s="31"/>
     </row>
-    <row r="68" spans="1:9" ht="30">
+    <row r="68" spans="1:9" ht="45">
       <c r="A68" s="29" t="s">
         <v>91</v>
       </c>
@@ -12815,7 +12455,7 @@
       </c>
       <c r="I75" s="31"/>
     </row>
-    <row r="76" spans="1:9" ht="30">
+    <row r="76" spans="1:9" ht="45">
       <c r="A76" s="29" t="s">
         <v>99</v>
       </c>
@@ -12840,7 +12480,7 @@
       </c>
       <c r="I76" s="31"/>
     </row>
-    <row r="77" spans="1:9" ht="30">
+    <row r="77" spans="1:9" ht="45">
       <c r="A77" s="29" t="s">
         <v>100</v>
       </c>
@@ -12990,7 +12630,7 @@
       </c>
       <c r="I82" s="31"/>
     </row>
-    <row r="83" spans="1:9" ht="30">
+    <row r="83" spans="1:9" ht="45">
       <c r="A83" s="29" t="s">
         <v>106</v>
       </c>
@@ -13115,7 +12755,7 @@
       </c>
       <c r="I87" s="31"/>
     </row>
-    <row r="88" spans="1:9" ht="30">
+    <row r="88" spans="1:9" ht="45">
       <c r="A88" s="29" t="s">
         <v>111</v>
       </c>
@@ -13140,7 +12780,7 @@
       </c>
       <c r="I88" s="31"/>
     </row>
-    <row r="89" spans="1:9" ht="75">
+    <row r="89" spans="1:9" ht="105">
       <c r="A89" s="29" t="s">
         <v>112</v>
       </c>
@@ -13167,7 +12807,7 @@
         <v>2869</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="30">
+    <row r="90" spans="1:9" ht="45">
       <c r="A90" s="29" t="s">
         <v>113</v>
       </c>
@@ -13219,7 +12859,7 @@
       </c>
       <c r="I91" s="31"/>
     </row>
-    <row r="92" spans="1:9" ht="45">
+    <row r="92" spans="1:9" ht="60">
       <c r="A92" s="29" t="s">
         <v>115</v>
       </c>
@@ -13271,7 +12911,7 @@
       </c>
       <c r="I93" s="31"/>
     </row>
-    <row r="94" spans="1:9" ht="45">
+    <row r="94" spans="1:9" ht="60">
       <c r="A94" s="29" t="s">
         <v>117</v>
       </c>
@@ -13323,7 +12963,7 @@
       </c>
       <c r="I95" s="31"/>
     </row>
-    <row r="96" spans="1:9" ht="120">
+    <row r="96" spans="1:9" ht="135">
       <c r="A96" s="29" t="s">
         <v>119</v>
       </c>
@@ -13423,7 +13063,7 @@
       </c>
       <c r="I99" s="31"/>
     </row>
-    <row r="100" spans="1:9" ht="30">
+    <row r="100" spans="1:9" ht="45">
       <c r="A100" s="29" t="s">
         <v>123</v>
       </c>
@@ -13523,7 +13163,7 @@
       </c>
       <c r="I103" s="31"/>
     </row>
-    <row r="104" spans="1:9" ht="30">
+    <row r="104" spans="1:9" ht="45">
       <c r="A104" s="29" t="s">
         <v>127</v>
       </c>
@@ -13598,7 +13238,7 @@
       </c>
       <c r="I106" s="31"/>
     </row>
-    <row r="107" spans="1:9" ht="30">
+    <row r="107" spans="1:9" ht="45">
       <c r="A107" s="29" t="s">
         <v>130</v>
       </c>
@@ -13673,7 +13313,7 @@
       </c>
       <c r="I109" s="31"/>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" ht="30">
       <c r="A110" s="29" t="s">
         <v>133</v>
       </c>
@@ -13698,7 +13338,7 @@
       </c>
       <c r="I110" s="31"/>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" ht="30">
       <c r="A111" s="29" t="s">
         <v>134</v>
       </c>
@@ -13748,7 +13388,7 @@
       </c>
       <c r="I112" s="31"/>
     </row>
-    <row r="113" spans="1:9">
+    <row r="113" spans="1:9" ht="30">
       <c r="A113" s="29" t="s">
         <v>136</v>
       </c>
@@ -13798,7 +13438,7 @@
       </c>
       <c r="I114" s="31"/>
     </row>
-    <row r="115" spans="1:9" ht="30">
+    <row r="115" spans="1:9" ht="45">
       <c r="A115" s="29" t="s">
         <v>138</v>
       </c>
@@ -13898,7 +13538,7 @@
       </c>
       <c r="I118" s="31"/>
     </row>
-    <row r="119" spans="1:9" ht="30">
+    <row r="119" spans="1:9" ht="45">
       <c r="A119" s="29" t="s">
         <v>142</v>
       </c>
@@ -14398,7 +14038,7 @@
       </c>
       <c r="I138" s="31"/>
     </row>
-    <row r="139" spans="1:9" ht="30">
+    <row r="139" spans="1:9" ht="45">
       <c r="A139" s="29" t="s">
         <v>162</v>
       </c>
@@ -14523,7 +14163,7 @@
       </c>
       <c r="I143" s="31"/>
     </row>
-    <row r="144" spans="1:9" ht="30">
+    <row r="144" spans="1:9" ht="45">
       <c r="A144" s="29" t="s">
         <v>167</v>
       </c>
@@ -14673,7 +14313,7 @@
       </c>
       <c r="I149" s="31"/>
     </row>
-    <row r="150" spans="1:9" ht="30">
+    <row r="150" spans="1:9" ht="45">
       <c r="A150" s="29" t="s">
         <v>173</v>
       </c>
@@ -14723,7 +14363,7 @@
       </c>
       <c r="I151" s="31"/>
     </row>
-    <row r="152" spans="1:9" ht="30">
+    <row r="152" spans="1:9" ht="45">
       <c r="A152" s="29" t="s">
         <v>175</v>
       </c>
@@ -14748,7 +14388,7 @@
       </c>
       <c r="I152" s="31"/>
     </row>
-    <row r="153" spans="1:9">
+    <row r="153" spans="1:9" ht="30">
       <c r="A153" s="29" t="s">
         <v>176</v>
       </c>
@@ -14823,7 +14463,7 @@
       </c>
       <c r="I155" s="31"/>
     </row>
-    <row r="156" spans="1:9">
+    <row r="156" spans="1:9" ht="30">
       <c r="A156" s="29" t="s">
         <v>179</v>
       </c>
@@ -14848,7 +14488,7 @@
       </c>
       <c r="I156" s="31"/>
     </row>
-    <row r="157" spans="1:9" ht="30">
+    <row r="157" spans="1:9" ht="45">
       <c r="A157" s="29" t="s">
         <v>180</v>
       </c>
@@ -14923,7 +14563,7 @@
       </c>
       <c r="I159" s="31"/>
     </row>
-    <row r="160" spans="1:9" ht="30">
+    <row r="160" spans="1:9" ht="45">
       <c r="A160" s="29" t="s">
         <v>183</v>
       </c>
@@ -14973,7 +14613,7 @@
       </c>
       <c r="I161" s="31"/>
     </row>
-    <row r="162" spans="1:9" ht="30">
+    <row r="162" spans="1:9" ht="45">
       <c r="A162" s="29" t="s">
         <v>185</v>
       </c>
@@ -15023,7 +14663,7 @@
       </c>
       <c r="I163" s="31"/>
     </row>
-    <row r="164" spans="1:9" ht="30">
+    <row r="164" spans="1:9" ht="45">
       <c r="A164" s="29" t="s">
         <v>187</v>
       </c>
@@ -15423,7 +15063,7 @@
       </c>
       <c r="I179" s="31"/>
     </row>
-    <row r="180" spans="1:9" ht="30">
+    <row r="180" spans="1:9" ht="45">
       <c r="A180" s="29" t="s">
         <v>203</v>
       </c>
@@ -15523,7 +15163,7 @@
       </c>
       <c r="I183" s="31"/>
     </row>
-    <row r="184" spans="1:9" ht="30">
+    <row r="184" spans="1:9" ht="45">
       <c r="A184" s="29" t="s">
         <v>207</v>
       </c>
@@ -15648,7 +15288,7 @@
       </c>
       <c r="I188" s="31"/>
     </row>
-    <row r="189" spans="1:9" ht="30">
+    <row r="189" spans="1:9" ht="45">
       <c r="A189" s="29" t="s">
         <v>212</v>
       </c>
@@ -15673,7 +15313,7 @@
       </c>
       <c r="I189" s="31"/>
     </row>
-    <row r="190" spans="1:9" ht="30">
+    <row r="190" spans="1:9" ht="45">
       <c r="A190" s="29" t="s">
         <v>213</v>
       </c>
@@ -15998,7 +15638,7 @@
       </c>
       <c r="I202" s="31"/>
     </row>
-    <row r="203" spans="1:9">
+    <row r="203" spans="1:9" ht="30">
       <c r="A203" s="29" t="s">
         <v>226</v>
       </c>
@@ -16023,7 +15663,7 @@
       </c>
       <c r="I203" s="31"/>
     </row>
-    <row r="204" spans="1:9">
+    <row r="204" spans="1:9" ht="30">
       <c r="A204" s="29" t="s">
         <v>227</v>
       </c>
@@ -16148,7 +15788,7 @@
       </c>
       <c r="I208" s="31"/>
     </row>
-    <row r="209" spans="1:9" ht="30">
+    <row r="209" spans="1:9" ht="45">
       <c r="A209" s="29" t="s">
         <v>232</v>
       </c>
@@ -16398,7 +16038,7 @@
       </c>
       <c r="I218" s="31"/>
     </row>
-    <row r="219" spans="1:9">
+    <row r="219" spans="1:9" ht="30">
       <c r="A219" s="29" t="s">
         <v>242</v>
       </c>
@@ -16423,7 +16063,7 @@
       </c>
       <c r="I219" s="31"/>
     </row>
-    <row r="220" spans="1:9">
+    <row r="220" spans="1:9" ht="30">
       <c r="A220" s="29" t="s">
         <v>243</v>
       </c>
@@ -16448,7 +16088,7 @@
       </c>
       <c r="I220" s="31"/>
     </row>
-    <row r="221" spans="1:9">
+    <row r="221" spans="1:9" ht="30">
       <c r="A221" s="29" t="s">
         <v>244</v>
       </c>
@@ -16648,7 +16288,7 @@
       </c>
       <c r="I228" s="31"/>
     </row>
-    <row r="229" spans="1:9">
+    <row r="229" spans="1:9" ht="30">
       <c r="A229" s="29" t="s">
         <v>252</v>
       </c>
@@ -16848,7 +16488,7 @@
       </c>
       <c r="I236" s="31"/>
     </row>
-    <row r="237" spans="1:9">
+    <row r="237" spans="1:9" ht="30">
       <c r="A237" s="29" t="s">
         <v>260</v>
       </c>
@@ -16873,7 +16513,7 @@
       </c>
       <c r="I237" s="31"/>
     </row>
-    <row r="238" spans="1:9">
+    <row r="238" spans="1:9" ht="30">
       <c r="A238" s="29" t="s">
         <v>261</v>
       </c>
@@ -16898,7 +16538,7 @@
       </c>
       <c r="I238" s="31"/>
     </row>
-    <row r="239" spans="1:9">
+    <row r="239" spans="1:9" ht="30">
       <c r="A239" s="29" t="s">
         <v>262</v>
       </c>
@@ -16923,7 +16563,7 @@
       </c>
       <c r="I239" s="31"/>
     </row>
-    <row r="240" spans="1:9">
+    <row r="240" spans="1:9" ht="30">
       <c r="A240" s="29" t="s">
         <v>263</v>
       </c>
@@ -17098,7 +16738,7 @@
       </c>
       <c r="I246" s="31"/>
     </row>
-    <row r="247" spans="1:9" ht="30">
+    <row r="247" spans="1:9" ht="45">
       <c r="A247" s="29" t="s">
         <v>270</v>
       </c>
@@ -17123,7 +16763,7 @@
       </c>
       <c r="I247" s="31"/>
     </row>
-    <row r="248" spans="1:9">
+    <row r="248" spans="1:9" ht="30">
       <c r="A248" s="29" t="s">
         <v>271</v>
       </c>
@@ -17148,7 +16788,7 @@
       </c>
       <c r="I248" s="31"/>
     </row>
-    <row r="249" spans="1:9">
+    <row r="249" spans="1:9" ht="30">
       <c r="A249" s="29" t="s">
         <v>272</v>
       </c>
@@ -17173,7 +16813,7 @@
       </c>
       <c r="I249" s="31"/>
     </row>
-    <row r="250" spans="1:9">
+    <row r="250" spans="1:9" ht="30">
       <c r="A250" s="29" t="s">
         <v>273</v>
       </c>
@@ -17198,7 +16838,7 @@
       </c>
       <c r="I250" s="31"/>
     </row>
-    <row r="251" spans="1:9">
+    <row r="251" spans="1:9" ht="30">
       <c r="A251" s="29" t="s">
         <v>274</v>
       </c>
@@ -17223,7 +16863,7 @@
       </c>
       <c r="I251" s="31"/>
     </row>
-    <row r="252" spans="1:9">
+    <row r="252" spans="1:9" ht="30">
       <c r="A252" s="29" t="s">
         <v>275</v>
       </c>
@@ -17448,7 +17088,7 @@
       </c>
       <c r="I260" s="31"/>
     </row>
-    <row r="261" spans="1:9">
+    <row r="261" spans="1:9" ht="30">
       <c r="A261" s="29" t="s">
         <v>284</v>
       </c>
@@ -17498,7 +17138,7 @@
       </c>
       <c r="I262" s="31"/>
     </row>
-    <row r="263" spans="1:9" ht="60">
+    <row r="263" spans="1:9" ht="75">
       <c r="A263" s="29" t="s">
         <v>286</v>
       </c>
@@ -17523,7 +17163,7 @@
       </c>
       <c r="I263" s="31"/>
     </row>
-    <row r="264" spans="1:9" ht="30">
+    <row r="264" spans="1:9" ht="45">
       <c r="A264" s="29" t="s">
         <v>287</v>
       </c>
@@ -17573,7 +17213,7 @@
       </c>
       <c r="I265" s="31"/>
     </row>
-    <row r="266" spans="1:9" ht="30">
+    <row r="266" spans="1:9" ht="45">
       <c r="A266" s="29" t="s">
         <v>289</v>
       </c>
@@ -17673,7 +17313,7 @@
       </c>
       <c r="I269" s="31"/>
     </row>
-    <row r="270" spans="1:9">
+    <row r="270" spans="1:9" ht="30">
       <c r="A270" s="29" t="s">
         <v>293</v>
       </c>
@@ -17748,7 +17388,7 @@
       </c>
       <c r="I272" s="31"/>
     </row>
-    <row r="273" spans="1:9" ht="30">
+    <row r="273" spans="1:9" ht="45">
       <c r="A273" s="29" t="s">
         <v>296</v>
       </c>
@@ -17923,7 +17563,7 @@
       </c>
       <c r="I279" s="31"/>
     </row>
-    <row r="280" spans="1:9">
+    <row r="280" spans="1:9" ht="30">
       <c r="A280" s="29" t="s">
         <v>303</v>
       </c>
@@ -18023,7 +17663,7 @@
       </c>
       <c r="I283" s="31"/>
     </row>
-    <row r="284" spans="1:9">
+    <row r="284" spans="1:9" ht="30">
       <c r="A284" s="29" t="s">
         <v>307</v>
       </c>
@@ -18152,7 +17792,7 @@
         <v>2870</v>
       </c>
     </row>
-    <row r="289" spans="1:9" ht="30">
+    <row r="289" spans="1:9" ht="45">
       <c r="A289" s="29" t="s">
         <v>312</v>
       </c>
@@ -18277,7 +17917,7 @@
       </c>
       <c r="I293" s="31"/>
     </row>
-    <row r="294" spans="1:9" ht="30">
+    <row r="294" spans="1:9" ht="45">
       <c r="A294" s="29" t="s">
         <v>317</v>
       </c>
@@ -18302,7 +17942,7 @@
       </c>
       <c r="I294" s="31"/>
     </row>
-    <row r="295" spans="1:9" ht="30">
+    <row r="295" spans="1:9" ht="45">
       <c r="A295" s="29" t="s">
         <v>318</v>
       </c>
@@ -18354,7 +17994,7 @@
         <v>2873</v>
       </c>
     </row>
-    <row r="297" spans="1:9" ht="30">
+    <row r="297" spans="1:9" ht="45">
       <c r="A297" s="29" t="s">
         <v>320</v>
       </c>
@@ -18404,7 +18044,7 @@
       </c>
       <c r="I298" s="31"/>
     </row>
-    <row r="299" spans="1:9" ht="30">
+    <row r="299" spans="1:9" ht="45">
       <c r="A299" s="29" t="s">
         <v>322</v>
       </c>
@@ -18456,7 +18096,7 @@
         <v>2874</v>
       </c>
     </row>
-    <row r="301" spans="1:9" ht="30">
+    <row r="301" spans="1:9" ht="45">
       <c r="A301" s="29" t="s">
         <v>324</v>
       </c>
@@ -18481,7 +18121,7 @@
       </c>
       <c r="I301" s="31"/>
     </row>
-    <row r="302" spans="1:9" ht="30">
+    <row r="302" spans="1:9" ht="45">
       <c r="A302" s="29" t="s">
         <v>325</v>
       </c>
@@ -18531,7 +18171,7 @@
       </c>
       <c r="I303" s="31"/>
     </row>
-    <row r="304" spans="1:9" ht="30">
+    <row r="304" spans="1:9" ht="45">
       <c r="A304" s="29" t="s">
         <v>327</v>
       </c>
@@ -18556,7 +18196,7 @@
       </c>
       <c r="I304" s="31"/>
     </row>
-    <row r="305" spans="1:9" ht="30">
+    <row r="305" spans="1:9" ht="45">
       <c r="A305" s="29" t="s">
         <v>328</v>
       </c>
@@ -18706,7 +18346,7 @@
       </c>
       <c r="I310" s="31"/>
     </row>
-    <row r="311" spans="1:9" ht="30">
+    <row r="311" spans="1:9" ht="45">
       <c r="A311" s="29" t="s">
         <v>334</v>
       </c>
@@ -18731,7 +18371,7 @@
       </c>
       <c r="I311" s="31"/>
     </row>
-    <row r="312" spans="1:9" ht="30">
+    <row r="312" spans="1:9" ht="45">
       <c r="A312" s="29" t="s">
         <v>335</v>
       </c>
@@ -18781,7 +18421,7 @@
       </c>
       <c r="I313" s="31"/>
     </row>
-    <row r="314" spans="1:9" ht="30">
+    <row r="314" spans="1:9" ht="45">
       <c r="A314" s="29" t="s">
         <v>337</v>
       </c>
@@ -18856,7 +18496,7 @@
       </c>
       <c r="I316" s="31"/>
     </row>
-    <row r="317" spans="1:9" ht="30">
+    <row r="317" spans="1:9" ht="45">
       <c r="A317" s="29" t="s">
         <v>340</v>
       </c>
@@ -18956,7 +18596,7 @@
       </c>
       <c r="I320" s="31"/>
     </row>
-    <row r="321" spans="1:9" ht="30">
+    <row r="321" spans="1:9" ht="45">
       <c r="A321" s="29" t="s">
         <v>344</v>
       </c>
@@ -19006,7 +18646,7 @@
       </c>
       <c r="I322" s="31"/>
     </row>
-    <row r="323" spans="1:9" ht="30">
+    <row r="323" spans="1:9" ht="45">
       <c r="A323" s="29" t="s">
         <v>346</v>
       </c>
@@ -19056,7 +18696,7 @@
       </c>
       <c r="I324" s="31"/>
     </row>
-    <row r="325" spans="1:9" ht="30">
+    <row r="325" spans="1:9" ht="45">
       <c r="A325" s="29" t="s">
         <v>348</v>
       </c>
@@ -19106,7 +18746,7 @@
       </c>
       <c r="I326" s="31"/>
     </row>
-    <row r="327" spans="1:9" ht="30">
+    <row r="327" spans="1:9" ht="45">
       <c r="A327" s="29" t="s">
         <v>350</v>
       </c>
@@ -19156,7 +18796,7 @@
       </c>
       <c r="I328" s="31"/>
     </row>
-    <row r="329" spans="1:9" ht="30">
+    <row r="329" spans="1:9" ht="45">
       <c r="A329" s="29" t="s">
         <v>352</v>
       </c>
@@ -19181,7 +18821,7 @@
       </c>
       <c r="I329" s="31"/>
     </row>
-    <row r="330" spans="1:9" ht="30">
+    <row r="330" spans="1:9" ht="45">
       <c r="A330" s="29" t="s">
         <v>353</v>
       </c>
@@ -19231,7 +18871,7 @@
       </c>
       <c r="I331" s="31"/>
     </row>
-    <row r="332" spans="1:9" ht="30">
+    <row r="332" spans="1:9" ht="45">
       <c r="A332" s="29" t="s">
         <v>355</v>
       </c>
@@ -19281,7 +18921,7 @@
       </c>
       <c r="I333" s="31"/>
     </row>
-    <row r="334" spans="1:9" ht="30">
+    <row r="334" spans="1:9" ht="45">
       <c r="A334" s="29" t="s">
         <v>357</v>
       </c>
@@ -19331,7 +18971,7 @@
       </c>
       <c r="I335" s="31"/>
     </row>
-    <row r="336" spans="1:9" ht="30">
+    <row r="336" spans="1:9" ht="45">
       <c r="A336" s="29" t="s">
         <v>359</v>
       </c>
@@ -19356,7 +18996,7 @@
       </c>
       <c r="I336" s="31"/>
     </row>
-    <row r="337" spans="1:9" ht="30">
+    <row r="337" spans="1:9" ht="45">
       <c r="A337" s="29" t="s">
         <v>360</v>
       </c>
@@ -19381,7 +19021,7 @@
       </c>
       <c r="I337" s="31"/>
     </row>
-    <row r="338" spans="1:9" ht="30">
+    <row r="338" spans="1:9" ht="45">
       <c r="A338" s="29" t="s">
         <v>361</v>
       </c>
@@ -19406,7 +19046,7 @@
       </c>
       <c r="I338" s="31"/>
     </row>
-    <row r="339" spans="1:9" ht="30">
+    <row r="339" spans="1:9" ht="45">
       <c r="A339" s="29" t="s">
         <v>362</v>
       </c>
@@ -19481,7 +19121,7 @@
       </c>
       <c r="I341" s="31"/>
     </row>
-    <row r="342" spans="1:9" ht="30">
+    <row r="342" spans="1:9" ht="45">
       <c r="A342" s="29" t="s">
         <v>365</v>
       </c>
@@ -19508,7 +19148,7 @@
         <v>2875</v>
       </c>
     </row>
-    <row r="343" spans="1:9">
+    <row r="343" spans="1:9" ht="30">
       <c r="A343" s="29" t="s">
         <v>366</v>
       </c>
@@ -19558,7 +19198,7 @@
       </c>
       <c r="I344" s="31"/>
     </row>
-    <row r="345" spans="1:9">
+    <row r="345" spans="1:9" ht="30">
       <c r="A345" s="29" t="s">
         <v>368</v>
       </c>
@@ -19583,7 +19223,7 @@
       </c>
       <c r="I345" s="31"/>
     </row>
-    <row r="346" spans="1:9">
+    <row r="346" spans="1:9" ht="30">
       <c r="A346" s="29" t="s">
         <v>369</v>
       </c>
@@ -19608,7 +19248,7 @@
       </c>
       <c r="I346" s="31"/>
     </row>
-    <row r="347" spans="1:9" ht="30">
+    <row r="347" spans="1:9" ht="45">
       <c r="A347" s="29" t="s">
         <v>370</v>
       </c>
@@ -19733,7 +19373,7 @@
       </c>
       <c r="I351" s="31"/>
     </row>
-    <row r="352" spans="1:9">
+    <row r="352" spans="1:9" ht="30">
       <c r="A352" s="29" t="s">
         <v>375</v>
       </c>
@@ -19808,7 +19448,7 @@
       </c>
       <c r="I354" s="31"/>
     </row>
-    <row r="355" spans="1:9" ht="30">
+    <row r="355" spans="1:9" ht="45">
       <c r="A355" s="29" t="s">
         <v>378</v>
       </c>
@@ -19858,7 +19498,7 @@
       </c>
       <c r="I356" s="31"/>
     </row>
-    <row r="357" spans="1:9">
+    <row r="357" spans="1:9" ht="30">
       <c r="A357" s="29" t="s">
         <v>380</v>
       </c>
@@ -19983,7 +19623,7 @@
       </c>
       <c r="I361" s="31"/>
     </row>
-    <row r="362" spans="1:9" ht="30">
+    <row r="362" spans="1:9" ht="45">
       <c r="A362" s="29" t="s">
         <v>385</v>
       </c>
@@ -20108,7 +19748,7 @@
       </c>
       <c r="I366" s="31"/>
     </row>
-    <row r="367" spans="1:9" ht="45">
+    <row r="367" spans="1:9" ht="60">
       <c r="A367" s="29" t="s">
         <v>390</v>
       </c>
@@ -20258,7 +19898,7 @@
       </c>
       <c r="I372" s="31"/>
     </row>
-    <row r="373" spans="1:9">
+    <row r="373" spans="1:9" ht="30">
       <c r="A373" s="29" t="s">
         <v>396</v>
       </c>
@@ -20333,7 +19973,7 @@
       </c>
       <c r="I375" s="31"/>
     </row>
-    <row r="376" spans="1:9" ht="30">
+    <row r="376" spans="1:9" ht="45">
       <c r="A376" s="29" t="s">
         <v>399</v>
       </c>
@@ -20358,7 +19998,7 @@
       </c>
       <c r="I376" s="31"/>
     </row>
-    <row r="377" spans="1:9">
+    <row r="377" spans="1:9" ht="30">
       <c r="A377" s="29" t="s">
         <v>400</v>
       </c>
@@ -20408,7 +20048,7 @@
       </c>
       <c r="I378" s="31"/>
     </row>
-    <row r="379" spans="1:9" ht="75">
+    <row r="379" spans="1:9" ht="105">
       <c r="A379" s="29" t="s">
         <v>402</v>
       </c>
@@ -20510,7 +20150,7 @@
       </c>
       <c r="I382" s="31"/>
     </row>
-    <row r="383" spans="1:9">
+    <row r="383" spans="1:9" ht="30">
       <c r="A383" s="29" t="s">
         <v>406</v>
       </c>
@@ -20560,7 +20200,7 @@
       </c>
       <c r="I384" s="31"/>
     </row>
-    <row r="385" spans="1:9" ht="90">
+    <row r="385" spans="1:9" ht="105">
       <c r="A385" s="29" t="s">
         <v>408</v>
       </c>
@@ -20637,7 +20277,7 @@
       </c>
       <c r="I387" s="31"/>
     </row>
-    <row r="388" spans="1:9">
+    <row r="388" spans="1:9" ht="30">
       <c r="A388" s="29" t="s">
         <v>411</v>
       </c>
@@ -20662,7 +20302,7 @@
       </c>
       <c r="I388" s="31"/>
     </row>
-    <row r="389" spans="1:9">
+    <row r="389" spans="1:9" ht="30">
       <c r="A389" s="29" t="s">
         <v>412</v>
       </c>
@@ -20739,7 +20379,7 @@
       </c>
       <c r="I391" s="31"/>
     </row>
-    <row r="392" spans="1:9" ht="30">
+    <row r="392" spans="1:9" ht="45">
       <c r="A392" s="29" t="s">
         <v>415</v>
       </c>
@@ -20764,7 +20404,7 @@
       </c>
       <c r="I392" s="31"/>
     </row>
-    <row r="393" spans="1:9" ht="30">
+    <row r="393" spans="1:9" ht="45">
       <c r="A393" s="29" t="s">
         <v>416</v>
       </c>
@@ -20789,7 +20429,7 @@
       </c>
       <c r="I393" s="31"/>
     </row>
-    <row r="394" spans="1:9">
+    <row r="394" spans="1:9" ht="30">
       <c r="A394" s="29" t="s">
         <v>417</v>
       </c>
@@ -20814,7 +20454,7 @@
       </c>
       <c r="I394" s="31"/>
     </row>
-    <row r="395" spans="1:9">
+    <row r="395" spans="1:9" ht="30">
       <c r="A395" s="29" t="s">
         <v>418</v>
       </c>
@@ -20839,7 +20479,7 @@
       </c>
       <c r="I395" s="31"/>
     </row>
-    <row r="396" spans="1:9">
+    <row r="396" spans="1:9" ht="30">
       <c r="A396" s="29" t="s">
         <v>419</v>
       </c>
@@ -20864,7 +20504,7 @@
       </c>
       <c r="I396" s="31"/>
     </row>
-    <row r="397" spans="1:9">
+    <row r="397" spans="1:9" ht="30">
       <c r="A397" s="29" t="s">
         <v>420</v>
       </c>
@@ -20943,7 +20583,7 @@
         <v>2880</v>
       </c>
     </row>
-    <row r="400" spans="1:9" ht="30">
+    <row r="400" spans="1:9" ht="45">
       <c r="A400" s="29" t="s">
         <v>423</v>
       </c>
@@ -20968,7 +20608,7 @@
       </c>
       <c r="I400" s="31"/>
     </row>
-    <row r="401" spans="1:9">
+    <row r="401" spans="1:9" ht="30">
       <c r="A401" s="29" t="s">
         <v>424</v>
       </c>
@@ -20993,7 +20633,7 @@
       </c>
       <c r="I401" s="31"/>
     </row>
-    <row r="402" spans="1:9">
+    <row r="402" spans="1:9" ht="30">
       <c r="A402" s="29" t="s">
         <v>425</v>
       </c>
@@ -21070,7 +20710,7 @@
       </c>
       <c r="I404" s="31"/>
     </row>
-    <row r="405" spans="1:9">
+    <row r="405" spans="1:9" ht="30">
       <c r="A405" s="29" t="s">
         <v>428</v>
       </c>
@@ -21095,7 +20735,7 @@
       </c>
       <c r="I405" s="31"/>
     </row>
-    <row r="406" spans="1:9">
+    <row r="406" spans="1:9" ht="30">
       <c r="A406" s="29" t="s">
         <v>429</v>
       </c>
@@ -21120,7 +20760,7 @@
       </c>
       <c r="I406" s="31"/>
     </row>
-    <row r="407" spans="1:9">
+    <row r="407" spans="1:9" ht="30">
       <c r="A407" s="29" t="s">
         <v>430</v>
       </c>
@@ -21145,7 +20785,7 @@
       </c>
       <c r="I407" s="31"/>
     </row>
-    <row r="408" spans="1:9">
+    <row r="408" spans="1:9" ht="30">
       <c r="A408" s="29" t="s">
         <v>431</v>
       </c>
@@ -21170,7 +20810,7 @@
       </c>
       <c r="I408" s="31"/>
     </row>
-    <row r="409" spans="1:9">
+    <row r="409" spans="1:9" ht="30">
       <c r="A409" s="29" t="s">
         <v>432</v>
       </c>
@@ -21195,7 +20835,7 @@
       </c>
       <c r="I409" s="31"/>
     </row>
-    <row r="410" spans="1:9">
+    <row r="410" spans="1:9" ht="30">
       <c r="A410" s="29" t="s">
         <v>433</v>
       </c>
@@ -21299,7 +20939,7 @@
       </c>
       <c r="I413" s="31"/>
     </row>
-    <row r="414" spans="1:9">
+    <row r="414" spans="1:9" ht="30">
       <c r="A414" s="29" t="s">
         <v>437</v>
       </c>
@@ -21324,7 +20964,7 @@
       </c>
       <c r="I414" s="31"/>
     </row>
-    <row r="415" spans="1:9">
+    <row r="415" spans="1:9" ht="30">
       <c r="A415" s="29" t="s">
         <v>438</v>
       </c>
@@ -21349,7 +20989,7 @@
       </c>
       <c r="I415" s="31"/>
     </row>
-    <row r="416" spans="1:9">
+    <row r="416" spans="1:9" ht="30">
       <c r="A416" s="29" t="s">
         <v>439</v>
       </c>
@@ -21374,7 +21014,7 @@
       </c>
       <c r="I416" s="31"/>
     </row>
-    <row r="417" spans="1:9">
+    <row r="417" spans="1:9" ht="30">
       <c r="A417" s="29" t="s">
         <v>440</v>
       </c>
@@ -21399,7 +21039,7 @@
       </c>
       <c r="I417" s="31"/>
     </row>
-    <row r="418" spans="1:9" ht="45">
+    <row r="418" spans="1:9" ht="60">
       <c r="A418" s="29" t="s">
         <v>441</v>
       </c>
@@ -21576,7 +21216,7 @@
       </c>
       <c r="I424" s="31"/>
     </row>
-    <row r="425" spans="1:9" ht="30">
+    <row r="425" spans="1:9" ht="45">
       <c r="A425" s="29" t="s">
         <v>448</v>
       </c>
@@ -21603,7 +21243,7 @@
         <v>2885</v>
       </c>
     </row>
-    <row r="426" spans="1:9" ht="30">
+    <row r="426" spans="1:9" ht="45">
       <c r="A426" s="29" t="s">
         <v>449</v>
       </c>
@@ -21680,7 +21320,7 @@
       </c>
       <c r="I428" s="31"/>
     </row>
-    <row r="429" spans="1:9" ht="30">
+    <row r="429" spans="1:9" ht="45">
       <c r="A429" s="29" t="s">
         <v>452</v>
       </c>
@@ -21805,7 +21445,7 @@
       </c>
       <c r="I433" s="31"/>
     </row>
-    <row r="434" spans="1:9" ht="30">
+    <row r="434" spans="1:9" ht="45">
       <c r="A434" s="29" t="s">
         <v>457</v>
       </c>
@@ -21855,7 +21495,7 @@
       </c>
       <c r="I435" s="31"/>
     </row>
-    <row r="436" spans="1:9" ht="30">
+    <row r="436" spans="1:9" ht="45">
       <c r="A436" s="29" t="s">
         <v>459</v>
       </c>
@@ -21905,7 +21545,7 @@
       </c>
       <c r="I437" s="31"/>
     </row>
-    <row r="438" spans="1:9" ht="45">
+    <row r="438" spans="1:9" ht="60">
       <c r="A438" s="29" t="s">
         <v>461</v>
       </c>
@@ -21930,7 +21570,7 @@
       </c>
       <c r="I438" s="31"/>
     </row>
-    <row r="439" spans="1:9" ht="60">
+    <row r="439" spans="1:9" ht="75">
       <c r="A439" s="29" t="s">
         <v>462</v>
       </c>
@@ -21980,7 +21620,7 @@
       </c>
       <c r="I440" s="31"/>
     </row>
-    <row r="441" spans="1:9" ht="30">
+    <row r="441" spans="1:9" ht="45">
       <c r="A441" s="29" t="s">
         <v>464</v>
       </c>
@@ -22105,7 +21745,7 @@
       </c>
       <c r="I445" s="31"/>
     </row>
-    <row r="446" spans="1:9">
+    <row r="446" spans="1:9" ht="30">
       <c r="A446" s="29" t="s">
         <v>469</v>
       </c>
@@ -22230,7 +21870,7 @@
       </c>
       <c r="I450" s="31"/>
     </row>
-    <row r="451" spans="1:9" ht="45">
+    <row r="451" spans="1:9" ht="60">
       <c r="A451" s="29" t="s">
         <v>474</v>
       </c>
@@ -22280,7 +21920,7 @@
       </c>
       <c r="I452" s="31"/>
     </row>
-    <row r="453" spans="1:9" ht="45">
+    <row r="453" spans="1:9" ht="60">
       <c r="A453" s="29" t="s">
         <v>476</v>
       </c>
@@ -22457,7 +22097,7 @@
       </c>
       <c r="I459" s="31"/>
     </row>
-    <row r="460" spans="1:9">
+    <row r="460" spans="1:9" ht="30">
       <c r="A460" s="29" t="s">
         <v>483</v>
       </c>
@@ -22482,7 +22122,7 @@
       </c>
       <c r="I460" s="31"/>
     </row>
-    <row r="461" spans="1:9">
+    <row r="461" spans="1:9" ht="30">
       <c r="A461" s="29" t="s">
         <v>484</v>
       </c>
@@ -22507,7 +22147,7 @@
       </c>
       <c r="I461" s="31"/>
     </row>
-    <row r="462" spans="1:9" ht="30">
+    <row r="462" spans="1:9" ht="45">
       <c r="A462" s="29" t="s">
         <v>485</v>
       </c>
@@ -22582,7 +22222,7 @@
       </c>
       <c r="I464" s="31"/>
     </row>
-    <row r="465" spans="1:9" ht="45">
+    <row r="465" spans="1:9" ht="60">
       <c r="A465" s="29" t="s">
         <v>488</v>
       </c>
@@ -22607,7 +22247,7 @@
       </c>
       <c r="I465" s="31"/>
     </row>
-    <row r="466" spans="1:9" ht="30">
+    <row r="466" spans="1:9" ht="45">
       <c r="A466" s="29" t="s">
         <v>489</v>
       </c>
@@ -22682,7 +22322,7 @@
       </c>
       <c r="I468" s="31"/>
     </row>
-    <row r="469" spans="1:9" ht="30">
+    <row r="469" spans="1:9" ht="45">
       <c r="A469" s="29" t="s">
         <v>492</v>
       </c>
@@ -22857,7 +22497,7 @@
       </c>
       <c r="I475" s="31"/>
     </row>
-    <row r="476" spans="1:9" ht="45">
+    <row r="476" spans="1:9" ht="60">
       <c r="A476" s="29" t="s">
         <v>499</v>
       </c>
@@ -22882,7 +22522,7 @@
       </c>
       <c r="I476" s="31"/>
     </row>
-    <row r="477" spans="1:9" ht="30">
+    <row r="477" spans="1:9" ht="45">
       <c r="A477" s="29" t="s">
         <v>500</v>
       </c>
@@ -22934,7 +22574,7 @@
       </c>
       <c r="I478" s="31"/>
     </row>
-    <row r="479" spans="1:9" ht="45">
+    <row r="479" spans="1:9" ht="60">
       <c r="A479" s="29" t="s">
         <v>502</v>
       </c>
@@ -22959,7 +22599,7 @@
       </c>
       <c r="I479" s="31"/>
     </row>
-    <row r="480" spans="1:9" ht="30">
+    <row r="480" spans="1:9" ht="45">
       <c r="A480" s="29" t="s">
         <v>503</v>
       </c>
@@ -23290,7 +22930,7 @@
       </c>
       <c r="I492" s="31"/>
     </row>
-    <row r="493" spans="1:9" ht="45">
+    <row r="493" spans="1:9" ht="60">
       <c r="A493" s="29" t="s">
         <v>516</v>
       </c>
@@ -23415,7 +23055,7 @@
       </c>
       <c r="I497" s="31"/>
     </row>
-    <row r="498" spans="1:9" ht="30">
+    <row r="498" spans="1:9" ht="45">
       <c r="A498" s="29" t="s">
         <v>521</v>
       </c>
@@ -23490,7 +23130,7 @@
       </c>
       <c r="I500" s="31"/>
     </row>
-    <row r="501" spans="1:9" ht="45">
+    <row r="501" spans="1:9" ht="60">
       <c r="A501" s="29" t="s">
         <v>524</v>
       </c>
@@ -23515,7 +23155,7 @@
       </c>
       <c r="I501" s="31"/>
     </row>
-    <row r="502" spans="1:9" ht="60">
+    <row r="502" spans="1:9" ht="75">
       <c r="A502" s="29" t="s">
         <v>525</v>
       </c>
@@ -23540,7 +23180,7 @@
       </c>
       <c r="I502" s="31"/>
     </row>
-    <row r="503" spans="1:9" ht="45">
+    <row r="503" spans="1:9" ht="60">
       <c r="A503" s="29" t="s">
         <v>526</v>
       </c>
@@ -23592,7 +23232,7 @@
       </c>
       <c r="I504" s="31"/>
     </row>
-    <row r="505" spans="1:9" ht="30">
+    <row r="505" spans="1:9" ht="45">
       <c r="A505" s="29" t="s">
         <v>528</v>
       </c>
@@ -23767,7 +23407,7 @@
       </c>
       <c r="I511" s="31"/>
     </row>
-    <row r="512" spans="1:9" ht="30">
+    <row r="512" spans="1:9" ht="45">
       <c r="A512" s="29" t="s">
         <v>535</v>
       </c>
@@ -23794,7 +23434,7 @@
         <v>2891</v>
       </c>
     </row>
-    <row r="513" spans="1:9" ht="45">
+    <row r="513" spans="1:9" ht="60">
       <c r="A513" s="29" t="s">
         <v>536</v>
       </c>
@@ -23973,7 +23613,7 @@
       </c>
       <c r="I519" s="31"/>
     </row>
-    <row r="520" spans="1:9">
+    <row r="520" spans="1:9" ht="30">
       <c r="A520" s="29" t="s">
         <v>543</v>
       </c>
@@ -23998,7 +23638,7 @@
       </c>
       <c r="I520" s="31"/>
     </row>
-    <row r="521" spans="1:9" ht="30">
+    <row r="521" spans="1:9" ht="45">
       <c r="A521" s="29" t="s">
         <v>544</v>
       </c>
@@ -24048,7 +23688,7 @@
       </c>
       <c r="I522" s="31"/>
     </row>
-    <row r="523" spans="1:9">
+    <row r="523" spans="1:9" ht="30">
       <c r="A523" s="29" t="s">
         <v>546</v>
       </c>
@@ -24098,7 +23738,7 @@
       </c>
       <c r="I524" s="31"/>
     </row>
-    <row r="525" spans="1:9" ht="90">
+    <row r="525" spans="1:9" ht="105">
       <c r="A525" s="29" t="s">
         <v>548</v>
       </c>
@@ -24123,7 +23763,7 @@
       </c>
       <c r="I525" s="31"/>
     </row>
-    <row r="526" spans="1:9" ht="45">
+    <row r="526" spans="1:9" ht="60">
       <c r="A526" s="29" t="s">
         <v>549</v>
       </c>
@@ -24150,7 +23790,7 @@
         <v>2894</v>
       </c>
     </row>
-    <row r="527" spans="1:9" ht="30">
+    <row r="527" spans="1:9" ht="45">
       <c r="A527" s="29" t="s">
         <v>550</v>
       </c>
@@ -24200,7 +23840,7 @@
       </c>
       <c r="I528" s="31"/>
     </row>
-    <row r="529" spans="1:9" ht="30">
+    <row r="529" spans="1:9" ht="45">
       <c r="A529" s="29" t="s">
         <v>552</v>
       </c>
@@ -24500,7 +24140,7 @@
       </c>
       <c r="I540" s="31"/>
     </row>
-    <row r="541" spans="1:9" ht="30">
+    <row r="541" spans="1:9" ht="45">
       <c r="A541" s="29" t="s">
         <v>564</v>
       </c>
@@ -24550,7 +24190,7 @@
       </c>
       <c r="I542" s="31"/>
     </row>
-    <row r="543" spans="1:9" ht="30">
+    <row r="543" spans="1:9" ht="45">
       <c r="A543" s="29" t="s">
         <v>566</v>
       </c>
@@ -24702,7 +24342,7 @@
         <v>2895</v>
       </c>
     </row>
-    <row r="549" spans="1:9" ht="45">
+    <row r="549" spans="1:9" ht="60">
       <c r="A549" s="29" t="s">
         <v>572</v>
       </c>
@@ -24752,7 +24392,7 @@
       </c>
       <c r="I550" s="31"/>
     </row>
-    <row r="551" spans="1:9" ht="30">
+    <row r="551" spans="1:9" ht="45">
       <c r="A551" s="29" t="s">
         <v>574</v>
       </c>
@@ -25054,7 +24694,7 @@
       </c>
       <c r="I562" s="31"/>
     </row>
-    <row r="563" spans="1:9">
+    <row r="563" spans="1:9" ht="30">
       <c r="A563" s="29" t="s">
         <v>586</v>
       </c>
@@ -25129,7 +24769,7 @@
       </c>
       <c r="I565" s="31"/>
     </row>
-    <row r="566" spans="1:9">
+    <row r="566" spans="1:9" ht="30">
       <c r="A566" s="29" t="s">
         <v>589</v>
       </c>
@@ -25204,7 +24844,7 @@
       </c>
       <c r="I568" s="31"/>
     </row>
-    <row r="569" spans="1:9">
+    <row r="569" spans="1:9" ht="30">
       <c r="A569" s="29" t="s">
         <v>592</v>
       </c>
@@ -25254,7 +24894,7 @@
       </c>
       <c r="I570" s="31"/>
     </row>
-    <row r="571" spans="1:9" ht="45">
+    <row r="571" spans="1:9" ht="60">
       <c r="A571" s="29" t="s">
         <v>594</v>
       </c>
@@ -25304,7 +24944,7 @@
       </c>
       <c r="I572" s="31"/>
     </row>
-    <row r="573" spans="1:9" ht="30">
+    <row r="573" spans="1:9" ht="45">
       <c r="A573" s="29" t="s">
         <v>596</v>
       </c>
@@ -25379,7 +25019,7 @@
       </c>
       <c r="I575" s="31"/>
     </row>
-    <row r="576" spans="1:9">
+    <row r="576" spans="1:9" ht="30">
       <c r="A576" s="29" t="s">
         <v>599</v>
       </c>
@@ -25454,7 +25094,7 @@
       </c>
       <c r="I578" s="31"/>
     </row>
-    <row r="579" spans="1:9">
+    <row r="579" spans="1:9" ht="30">
       <c r="A579" s="29" t="s">
         <v>602</v>
       </c>
@@ -25529,7 +25169,7 @@
       </c>
       <c r="I581" s="31"/>
     </row>
-    <row r="582" spans="1:9">
+    <row r="582" spans="1:9" ht="30">
       <c r="A582" s="29" t="s">
         <v>605</v>
       </c>
@@ -25579,7 +25219,7 @@
       </c>
       <c r="I583" s="31"/>
     </row>
-    <row r="584" spans="1:9" ht="45">
+    <row r="584" spans="1:9" ht="60">
       <c r="A584" s="29" t="s">
         <v>607</v>
       </c>
@@ -25629,7 +25269,7 @@
       </c>
       <c r="I585" s="31"/>
     </row>
-    <row r="586" spans="1:9" ht="30">
+    <row r="586" spans="1:9" ht="45">
       <c r="A586" s="29" t="s">
         <v>609</v>
       </c>
@@ -25754,7 +25394,7 @@
       </c>
       <c r="I590" s="31"/>
     </row>
-    <row r="591" spans="1:9" ht="30">
+    <row r="591" spans="1:9" ht="45">
       <c r="A591" s="29" t="s">
         <v>614</v>
       </c>
@@ -25779,7 +25419,7 @@
       </c>
       <c r="I591" s="31"/>
     </row>
-    <row r="592" spans="1:9" ht="30">
+    <row r="592" spans="1:9" ht="45">
       <c r="A592" s="29" t="s">
         <v>615</v>
       </c>
@@ -25804,7 +25444,7 @@
       </c>
       <c r="I592" s="31"/>
     </row>
-    <row r="593" spans="1:9" ht="30">
+    <row r="593" spans="1:9" ht="45">
       <c r="A593" s="29" t="s">
         <v>616</v>
       </c>
@@ -25829,7 +25469,7 @@
       </c>
       <c r="I593" s="31"/>
     </row>
-    <row r="594" spans="1:9" ht="30">
+    <row r="594" spans="1:9" ht="45">
       <c r="A594" s="29" t="s">
         <v>617</v>
       </c>
@@ -25929,7 +25569,7 @@
       </c>
       <c r="I597" s="31"/>
     </row>
-    <row r="598" spans="1:9">
+    <row r="598" spans="1:9" ht="30">
       <c r="A598" s="29" t="s">
         <v>621</v>
       </c>
@@ -25979,7 +25619,7 @@
       </c>
       <c r="I599" s="31"/>
     </row>
-    <row r="600" spans="1:9">
+    <row r="600" spans="1:9" ht="30">
       <c r="A600" s="29" t="s">
         <v>623</v>
       </c>
@@ -26179,7 +25819,7 @@
       </c>
       <c r="I607" s="31"/>
     </row>
-    <row r="608" spans="1:9" ht="30">
+    <row r="608" spans="1:9" ht="45">
       <c r="A608" s="29" t="s">
         <v>631</v>
       </c>
@@ -26404,7 +26044,7 @@
       </c>
       <c r="I616" s="31"/>
     </row>
-    <row r="617" spans="1:9">
+    <row r="617" spans="1:9" ht="30">
       <c r="A617" s="29" t="s">
         <v>640</v>
       </c>
@@ -26454,7 +26094,7 @@
       </c>
       <c r="I618" s="31"/>
     </row>
-    <row r="619" spans="1:9">
+    <row r="619" spans="1:9" ht="30">
       <c r="A619" s="29" t="s">
         <v>642</v>
       </c>
@@ -26504,7 +26144,7 @@
       </c>
       <c r="I620" s="31"/>
     </row>
-    <row r="621" spans="1:9" ht="30">
+    <row r="621" spans="1:9" ht="45">
       <c r="A621" s="29" t="s">
         <v>644</v>
       </c>
@@ -26729,7 +26369,7 @@
       </c>
       <c r="I629" s="31"/>
     </row>
-    <row r="630" spans="1:9">
+    <row r="630" spans="1:9" ht="30">
       <c r="A630" s="29" t="s">
         <v>653</v>
       </c>
@@ -26804,7 +26444,7 @@
       </c>
       <c r="I632" s="31"/>
     </row>
-    <row r="633" spans="1:9">
+    <row r="633" spans="1:9" ht="30">
       <c r="A633" s="29" t="s">
         <v>656</v>
       </c>
@@ -26829,7 +26469,7 @@
       </c>
       <c r="I633" s="31"/>
     </row>
-    <row r="634" spans="1:9" ht="30">
+    <row r="634" spans="1:9" ht="45">
       <c r="A634" s="29" t="s">
         <v>657</v>
       </c>
@@ -27104,7 +26744,7 @@
       </c>
       <c r="I644" s="31"/>
     </row>
-    <row r="645" spans="1:9">
+    <row r="645" spans="1:9" ht="30">
       <c r="A645" s="29" t="s">
         <v>668</v>
       </c>
@@ -27354,7 +26994,7 @@
       </c>
       <c r="I654" s="31"/>
     </row>
-    <row r="655" spans="1:9" ht="30">
+    <row r="655" spans="1:9" ht="45">
       <c r="A655" s="29" t="s">
         <v>678</v>
       </c>
@@ -27379,7 +27019,7 @@
       </c>
       <c r="I655" s="31"/>
     </row>
-    <row r="656" spans="1:9" ht="30">
+    <row r="656" spans="1:9" ht="45">
       <c r="A656" s="29" t="s">
         <v>679</v>
       </c>
@@ -27804,7 +27444,7 @@
       </c>
       <c r="I672" s="31"/>
     </row>
-    <row r="673" spans="1:9" ht="30">
+    <row r="673" spans="1:9" ht="45">
       <c r="A673" s="29" t="s">
         <v>696</v>
       </c>
@@ -27829,7 +27469,7 @@
       </c>
       <c r="I673" s="31"/>
     </row>
-    <row r="674" spans="1:9" ht="30">
+    <row r="674" spans="1:9" ht="45">
       <c r="A674" s="29" t="s">
         <v>697</v>
       </c>
@@ -27929,7 +27569,7 @@
       </c>
       <c r="I677" s="31"/>
     </row>
-    <row r="678" spans="1:9" ht="30">
+    <row r="678" spans="1:9" ht="45">
       <c r="A678" s="29" t="s">
         <v>701</v>
       </c>
@@ -27979,7 +27619,7 @@
       </c>
       <c r="I679" s="31"/>
     </row>
-    <row r="680" spans="1:9">
+    <row r="680" spans="1:9" ht="30">
       <c r="A680" s="29" t="s">
         <v>703</v>
       </c>
@@ -28129,7 +27769,7 @@
       </c>
       <c r="I685" s="31"/>
     </row>
-    <row r="686" spans="1:9">
+    <row r="686" spans="1:9" ht="30">
       <c r="A686" s="29" t="s">
         <v>709</v>
       </c>
@@ -28254,7 +27894,7 @@
       </c>
       <c r="I690" s="31"/>
     </row>
-    <row r="691" spans="1:9" ht="45">
+    <row r="691" spans="1:9" ht="60">
       <c r="A691" s="29" t="s">
         <v>714</v>
       </c>
@@ -28279,7 +27919,7 @@
       </c>
       <c r="I691" s="31"/>
     </row>
-    <row r="692" spans="1:9" ht="45">
+    <row r="692" spans="1:9" ht="60">
       <c r="A692" s="29" t="s">
         <v>715</v>
       </c>
@@ -28304,7 +27944,7 @@
       </c>
       <c r="I692" s="31"/>
     </row>
-    <row r="693" spans="1:9" ht="45">
+    <row r="693" spans="1:9" ht="60">
       <c r="A693" s="29" t="s">
         <v>716</v>
       </c>
@@ -28329,7 +27969,7 @@
       </c>
       <c r="I693" s="31"/>
     </row>
-    <row r="694" spans="1:9" ht="45">
+    <row r="694" spans="1:9" ht="60">
       <c r="A694" s="29" t="s">
         <v>717</v>
       </c>
@@ -28354,7 +27994,7 @@
       </c>
       <c r="I694" s="31"/>
     </row>
-    <row r="695" spans="1:9" ht="30">
+    <row r="695" spans="1:9" ht="45">
       <c r="A695" s="29" t="s">
         <v>718</v>
       </c>
@@ -28404,7 +28044,7 @@
       </c>
       <c r="I696" s="31"/>
     </row>
-    <row r="697" spans="1:9" ht="45">
+    <row r="697" spans="1:9" ht="60">
       <c r="A697" s="29" t="s">
         <v>720</v>
       </c>
@@ -28429,7 +28069,7 @@
       </c>
       <c r="I697" s="31"/>
     </row>
-    <row r="698" spans="1:9" ht="30">
+    <row r="698" spans="1:9" ht="45">
       <c r="A698" s="29" t="s">
         <v>721</v>
       </c>
@@ -28504,7 +28144,7 @@
       </c>
       <c r="I700" s="31"/>
     </row>
-    <row r="701" spans="1:9" ht="30">
+    <row r="701" spans="1:9" ht="45">
       <c r="A701" s="29" t="s">
         <v>724</v>
       </c>
@@ -28554,7 +28194,7 @@
       </c>
       <c r="I702" s="31"/>
     </row>
-    <row r="703" spans="1:9" ht="30">
+    <row r="703" spans="1:9" ht="45">
       <c r="A703" s="29" t="s">
         <v>726</v>
       </c>
@@ -28579,7 +28219,7 @@
       </c>
       <c r="I703" s="31"/>
     </row>
-    <row r="704" spans="1:9" ht="60">
+    <row r="704" spans="1:9" ht="75">
       <c r="A704" s="29" t="s">
         <v>727</v>
       </c>
@@ -28654,7 +28294,7 @@
       </c>
       <c r="I706" s="31"/>
     </row>
-    <row r="707" spans="1:9">
+    <row r="707" spans="1:9" ht="30">
       <c r="A707" s="29" t="s">
         <v>730</v>
       </c>
@@ -28704,7 +28344,7 @@
       </c>
       <c r="I708" s="31"/>
     </row>
-    <row r="709" spans="1:9" ht="165">
+    <row r="709" spans="1:9" ht="240">
       <c r="A709" s="29" t="s">
         <v>732</v>
       </c>
@@ -28906,7 +28546,7 @@
       </c>
       <c r="I716" s="31"/>
     </row>
-    <row r="717" spans="1:9">
+    <row r="717" spans="1:9" ht="30">
       <c r="A717" s="29" t="s">
         <v>740</v>
       </c>
@@ -28981,7 +28621,7 @@
       </c>
       <c r="I719" s="31"/>
     </row>
-    <row r="720" spans="1:9" ht="30">
+    <row r="720" spans="1:9" ht="45">
       <c r="A720" s="29" t="s">
         <v>743</v>
       </c>
@@ -29183,7 +28823,7 @@
       </c>
       <c r="I727" s="31"/>
     </row>
-    <row r="728" spans="1:9" ht="75">
+    <row r="728" spans="1:9" ht="105">
       <c r="A728" s="29" t="s">
         <v>751</v>
       </c>
@@ -29210,7 +28850,7 @@
         <v>2869</v>
       </c>
     </row>
-    <row r="729" spans="1:9" ht="45">
+    <row r="729" spans="1:9" ht="60">
       <c r="A729" s="29" t="s">
         <v>752</v>
       </c>
@@ -29237,7 +28877,7 @@
         <v>2897</v>
       </c>
     </row>
-    <row r="730" spans="1:9" ht="30">
+    <row r="730" spans="1:9" ht="45">
       <c r="A730" s="29" t="s">
         <v>753</v>
       </c>
@@ -29316,7 +28956,7 @@
       </c>
       <c r="I732" s="31"/>
     </row>
-    <row r="733" spans="1:9" ht="30">
+    <row r="733" spans="1:9" ht="45">
       <c r="A733" s="29" t="s">
         <v>756</v>
       </c>
@@ -29341,7 +28981,7 @@
       </c>
       <c r="I733" s="31"/>
     </row>
-    <row r="734" spans="1:9" ht="45">
+    <row r="734" spans="1:9" ht="60">
       <c r="A734" s="29" t="s">
         <v>757</v>
       </c>
@@ -29368,7 +29008,7 @@
         <v>2872</v>
       </c>
     </row>
-    <row r="735" spans="1:9" ht="30">
+    <row r="735" spans="1:9" ht="45">
       <c r="A735" s="29" t="s">
         <v>758</v>
       </c>
@@ -29418,7 +29058,7 @@
       </c>
       <c r="I736" s="31"/>
     </row>
-    <row r="737" spans="1:9" ht="90">
+    <row r="737" spans="1:9" ht="120">
       <c r="A737" s="29" t="s">
         <v>760</v>
       </c>
@@ -29682,7 +29322,7 @@
       </c>
       <c r="I746" s="31"/>
     </row>
-    <row r="747" spans="1:9">
+    <row r="747" spans="1:9" ht="30">
       <c r="A747" s="29" t="s">
         <v>770</v>
       </c>
@@ -29734,7 +29374,7 @@
         <v>2899</v>
       </c>
     </row>
-    <row r="749" spans="1:9" ht="30">
+    <row r="749" spans="1:9" ht="45">
       <c r="A749" s="29" t="s">
         <v>772</v>
       </c>
@@ -29759,7 +29399,7 @@
       </c>
       <c r="I749" s="31"/>
     </row>
-    <row r="750" spans="1:9">
+    <row r="750" spans="1:9" ht="30">
       <c r="A750" s="29" t="s">
         <v>773</v>
       </c>
@@ -29784,7 +29424,7 @@
       </c>
       <c r="I750" s="31"/>
     </row>
-    <row r="751" spans="1:9">
+    <row r="751" spans="1:9" ht="30">
       <c r="A751" s="29" t="s">
         <v>774</v>
       </c>
@@ -29909,7 +29549,7 @@
       </c>
       <c r="I755" s="31"/>
     </row>
-    <row r="756" spans="1:9" ht="30">
+    <row r="756" spans="1:9" ht="45">
       <c r="A756" s="29" t="s">
         <v>779</v>
       </c>
@@ -29934,7 +29574,7 @@
       </c>
       <c r="I756" s="31"/>
     </row>
-    <row r="757" spans="1:9" ht="30">
+    <row r="757" spans="1:9" ht="45">
       <c r="A757" s="29" t="s">
         <v>780</v>
       </c>
@@ -30259,7 +29899,7 @@
       </c>
       <c r="I769" s="31"/>
     </row>
-    <row r="770" spans="1:9" ht="30">
+    <row r="770" spans="1:9" ht="45">
       <c r="A770" s="29" t="s">
         <v>793</v>
       </c>
@@ -30309,7 +29949,7 @@
       </c>
       <c r="I771" s="31"/>
     </row>
-    <row r="772" spans="1:9" ht="30">
+    <row r="772" spans="1:9" ht="45">
       <c r="A772" s="29" t="s">
         <v>795</v>
       </c>
@@ -30334,7 +29974,7 @@
       </c>
       <c r="I772" s="31"/>
     </row>
-    <row r="773" spans="1:9" ht="30">
+    <row r="773" spans="1:9" ht="45">
       <c r="A773" s="29" t="s">
         <v>796</v>
       </c>
@@ -30384,7 +30024,7 @@
       </c>
       <c r="I774" s="31"/>
     </row>
-    <row r="775" spans="1:9" ht="30">
+    <row r="775" spans="1:9" ht="45">
       <c r="A775" s="29" t="s">
         <v>798</v>
       </c>
@@ -30509,7 +30149,7 @@
       </c>
       <c r="I779" s="31"/>
     </row>
-    <row r="780" spans="1:9">
+    <row r="780" spans="1:9" ht="30">
       <c r="A780" s="29" t="s">
         <v>803</v>
       </c>
@@ -30709,7 +30349,7 @@
       </c>
       <c r="I787" s="31"/>
     </row>
-    <row r="788" spans="1:9" ht="30">
+    <row r="788" spans="1:9" ht="45">
       <c r="A788" s="29" t="s">
         <v>811</v>
       </c>
@@ -30734,7 +30374,7 @@
       </c>
       <c r="I788" s="31"/>
     </row>
-    <row r="789" spans="1:9" ht="30">
+    <row r="789" spans="1:9" ht="45">
       <c r="A789" s="29" t="s">
         <v>812</v>
       </c>
@@ -30784,7 +30424,7 @@
       </c>
       <c r="I790" s="31"/>
     </row>
-    <row r="791" spans="1:9" ht="45">
+    <row r="791" spans="1:9" ht="60">
       <c r="A791" s="29" t="s">
         <v>814</v>
       </c>
@@ -31036,7 +30676,7 @@
       </c>
       <c r="I800" s="31"/>
     </row>
-    <row r="801" spans="1:9" ht="45">
+    <row r="801" spans="1:9" ht="60">
       <c r="A801" s="29" t="s">
         <v>824</v>
       </c>
@@ -31063,7 +30703,7 @@
         <v>2901</v>
       </c>
     </row>
-    <row r="802" spans="1:9">
+    <row r="802" spans="1:9" ht="30">
       <c r="A802" s="29" t="s">
         <v>825</v>
       </c>
@@ -31213,7 +30853,7 @@
       </c>
       <c r="I807" s="31"/>
     </row>
-    <row r="808" spans="1:9">
+    <row r="808" spans="1:9" ht="30">
       <c r="A808" s="29" t="s">
         <v>831</v>
       </c>
@@ -31313,7 +30953,7 @@
       </c>
       <c r="I811" s="31"/>
     </row>
-    <row r="812" spans="1:9" ht="45">
+    <row r="812" spans="1:9" ht="60">
       <c r="A812" s="29" t="s">
         <v>835</v>
       </c>
@@ -31340,7 +30980,7 @@
         <v>2902</v>
       </c>
     </row>
-    <row r="813" spans="1:9">
+    <row r="813" spans="1:9" ht="30">
       <c r="A813" s="29" t="s">
         <v>836</v>
       </c>
@@ -31365,7 +31005,7 @@
       </c>
       <c r="I813" s="31"/>
     </row>
-    <row r="814" spans="1:9" ht="45">
+    <row r="814" spans="1:9" ht="60">
       <c r="A814" s="29" t="s">
         <v>837</v>
       </c>
@@ -31417,7 +31057,7 @@
       </c>
       <c r="I815" s="31"/>
     </row>
-    <row r="816" spans="1:9">
+    <row r="816" spans="1:9" ht="30">
       <c r="A816" s="29" t="s">
         <v>839</v>
       </c>
@@ -31517,7 +31157,7 @@
       </c>
       <c r="I819" s="31"/>
     </row>
-    <row r="820" spans="1:9" ht="30">
+    <row r="820" spans="1:9" ht="45">
       <c r="A820" s="29" t="s">
         <v>843</v>
       </c>
@@ -31544,7 +31184,7 @@
         <v>2904</v>
       </c>
     </row>
-    <row r="821" spans="1:9">
+    <row r="821" spans="1:9" ht="30">
       <c r="A821" s="29" t="s">
         <v>844</v>
       </c>
@@ -31596,7 +31236,7 @@
       </c>
       <c r="I822" s="31"/>
     </row>
-    <row r="823" spans="1:9" ht="45">
+    <row r="823" spans="1:9" ht="60">
       <c r="A823" s="29" t="s">
         <v>846</v>
       </c>
@@ -31623,7 +31263,7 @@
         <v>2905</v>
       </c>
     </row>
-    <row r="824" spans="1:9" ht="30">
+    <row r="824" spans="1:9" ht="45">
       <c r="A824" s="29" t="s">
         <v>847</v>
       </c>
@@ -31648,7 +31288,7 @@
       </c>
       <c r="I824" s="31"/>
     </row>
-    <row r="825" spans="1:9" ht="30">
+    <row r="825" spans="1:9" ht="45">
       <c r="A825" s="29" t="s">
         <v>848</v>
       </c>
@@ -31698,7 +31338,7 @@
       </c>
       <c r="I826" s="31"/>
     </row>
-    <row r="827" spans="1:9">
+    <row r="827" spans="1:9" ht="30">
       <c r="A827" s="29" t="s">
         <v>850</v>
       </c>
@@ -31923,7 +31563,7 @@
       </c>
       <c r="I835" s="31"/>
     </row>
-    <row r="836" spans="1:9" ht="45">
+    <row r="836" spans="1:9" ht="60">
       <c r="A836" s="29" t="s">
         <v>859</v>
       </c>
@@ -31975,7 +31615,7 @@
       </c>
       <c r="I837" s="31"/>
     </row>
-    <row r="838" spans="1:9" ht="45">
+    <row r="838" spans="1:9" ht="60">
       <c r="A838" s="29" t="s">
         <v>861</v>
       </c>
@@ -32027,7 +31667,7 @@
       </c>
       <c r="I839" s="31"/>
     </row>
-    <row r="840" spans="1:9" ht="30">
+    <row r="840" spans="1:9" ht="45">
       <c r="A840" s="29" t="s">
         <v>863</v>
       </c>
@@ -32106,7 +31746,7 @@
       </c>
       <c r="I842" s="31"/>
     </row>
-    <row r="843" spans="1:9" ht="30">
+    <row r="843" spans="1:9" ht="45">
       <c r="A843" s="29" t="s">
         <v>866</v>
       </c>
@@ -32156,7 +31796,7 @@
       </c>
       <c r="I844" s="31"/>
     </row>
-    <row r="845" spans="1:9">
+    <row r="845" spans="1:9" ht="30">
       <c r="A845" s="29" t="s">
         <v>868</v>
       </c>
@@ -32206,7 +31846,7 @@
       </c>
       <c r="I846" s="31"/>
     </row>
-    <row r="847" spans="1:9" ht="30">
+    <row r="847" spans="1:9" ht="45">
       <c r="A847" s="29" t="s">
         <v>870</v>
       </c>
@@ -32231,7 +31871,7 @@
       </c>
       <c r="I847" s="31"/>
     </row>
-    <row r="848" spans="1:9" ht="30">
+    <row r="848" spans="1:9" ht="45">
       <c r="A848" s="29" t="s">
         <v>871</v>
       </c>
@@ -32256,7 +31896,7 @@
       </c>
       <c r="I848" s="31"/>
     </row>
-    <row r="849" spans="1:9" ht="45">
+    <row r="849" spans="1:9" ht="60">
       <c r="A849" s="29" t="s">
         <v>872</v>
       </c>
@@ -32281,7 +31921,7 @@
       </c>
       <c r="I849" s="31"/>
     </row>
-    <row r="850" spans="1:9">
+    <row r="850" spans="1:9" ht="30">
       <c r="A850" s="29" t="s">
         <v>873</v>
       </c>
@@ -32381,7 +32021,7 @@
       </c>
       <c r="I853" s="31"/>
     </row>
-    <row r="854" spans="1:9" ht="30">
+    <row r="854" spans="1:9" ht="45">
       <c r="A854" s="29" t="s">
         <v>877</v>
       </c>
@@ -32431,7 +32071,7 @@
       </c>
       <c r="I855" s="31"/>
     </row>
-    <row r="856" spans="1:9" ht="30">
+    <row r="856" spans="1:9" ht="45">
       <c r="A856" s="29" t="s">
         <v>879</v>
       </c>
@@ -32458,7 +32098,7 @@
         <v>2908</v>
       </c>
     </row>
-    <row r="857" spans="1:9" ht="45">
+    <row r="857" spans="1:9" ht="60">
       <c r="A857" s="29" t="s">
         <v>880</v>
       </c>
@@ -32508,7 +32148,7 @@
       </c>
       <c r="I858" s="31"/>
     </row>
-    <row r="859" spans="1:9" ht="30">
+    <row r="859" spans="1:9" ht="45">
       <c r="A859" s="29" t="s">
         <v>882</v>
       </c>
@@ -32760,7 +32400,7 @@
       </c>
       <c r="I868" s="31"/>
     </row>
-    <row r="869" spans="1:9" ht="45">
+    <row r="869" spans="1:9" ht="60">
       <c r="A869" s="29" t="s">
         <v>892</v>
       </c>
@@ -32787,7 +32427,7 @@
         <v>2909</v>
       </c>
     </row>
-    <row r="870" spans="1:9" ht="30">
+    <row r="870" spans="1:9" ht="45">
       <c r="A870" s="29" t="s">
         <v>893</v>
       </c>
@@ -32814,7 +32454,7 @@
         <v>2910</v>
       </c>
     </row>
-    <row r="871" spans="1:9" ht="30">
+    <row r="871" spans="1:9" ht="45">
       <c r="A871" s="29" t="s">
         <v>894</v>
       </c>
@@ -32864,7 +32504,7 @@
       </c>
       <c r="I872" s="31"/>
     </row>
-    <row r="873" spans="1:9">
+    <row r="873" spans="1:9" ht="30">
       <c r="A873" s="29" t="s">
         <v>896</v>
       </c>
@@ -32914,7 +32554,7 @@
       </c>
       <c r="I874" s="31"/>
     </row>
-    <row r="875" spans="1:9" ht="30">
+    <row r="875" spans="1:9" ht="45">
       <c r="A875" s="29" t="s">
         <v>898</v>
       </c>
@@ -32989,7 +32629,7 @@
       </c>
       <c r="I877" s="31"/>
     </row>
-    <row r="878" spans="1:9" ht="30">
+    <row r="878" spans="1:9" ht="45">
       <c r="A878" s="29" t="s">
         <v>901</v>
       </c>
@@ -33039,7 +32679,7 @@
       </c>
       <c r="I879" s="31"/>
     </row>
-    <row r="880" spans="1:9" ht="30">
+    <row r="880" spans="1:9" ht="45">
       <c r="A880" s="29" t="s">
         <v>903</v>
       </c>
@@ -33064,7 +32704,7 @@
       </c>
       <c r="I880" s="31"/>
     </row>
-    <row r="881" spans="1:9" ht="45">
+    <row r="881" spans="1:9" ht="60">
       <c r="A881" s="29" t="s">
         <v>904</v>
       </c>
@@ -33114,7 +32754,7 @@
       </c>
       <c r="I882" s="31"/>
     </row>
-    <row r="883" spans="1:9">
+    <row r="883" spans="1:9" ht="30">
       <c r="A883" s="29" t="s">
         <v>906</v>
       </c>
@@ -33264,7 +32904,7 @@
       </c>
       <c r="I888" s="31"/>
     </row>
-    <row r="889" spans="1:9" ht="30">
+    <row r="889" spans="1:9" ht="45">
       <c r="A889" s="29" t="s">
         <v>912</v>
       </c>
@@ -33289,7 +32929,7 @@
       </c>
       <c r="I889" s="31"/>
     </row>
-    <row r="890" spans="1:9">
+    <row r="890" spans="1:9" ht="30">
       <c r="A890" s="29" t="s">
         <v>913</v>
       </c>
@@ -33314,7 +32954,7 @@
       </c>
       <c r="I890" s="31"/>
     </row>
-    <row r="891" spans="1:9" ht="30">
+    <row r="891" spans="1:9" ht="45">
       <c r="A891" s="29" t="s">
         <v>914</v>
       </c>
@@ -33339,7 +32979,7 @@
       </c>
       <c r="I891" s="31"/>
     </row>
-    <row r="892" spans="1:9" ht="30">
+    <row r="892" spans="1:9" ht="45">
       <c r="A892" s="29" t="s">
         <v>915</v>
       </c>
@@ -33364,7 +33004,7 @@
       </c>
       <c r="I892" s="31"/>
     </row>
-    <row r="893" spans="1:9">
+    <row r="893" spans="1:9" ht="30">
       <c r="A893" s="29" t="s">
         <v>916</v>
       </c>
@@ -33414,7 +33054,7 @@
       </c>
       <c r="I894" s="31"/>
     </row>
-    <row r="895" spans="1:9" ht="60">
+    <row r="895" spans="1:9" ht="75">
       <c r="A895" s="29" t="s">
         <v>918</v>
       </c>
@@ -33439,7 +33079,7 @@
       </c>
       <c r="I895" s="31"/>
     </row>
-    <row r="896" spans="1:9" ht="30">
+    <row r="896" spans="1:9" ht="45">
       <c r="A896" s="29" t="s">
         <v>919</v>
       </c>
@@ -33491,7 +33131,7 @@
       </c>
       <c r="I897" s="31"/>
     </row>
-    <row r="898" spans="1:9" ht="30">
+    <row r="898" spans="1:9" ht="45">
       <c r="A898" s="29" t="s">
         <v>921</v>
       </c>
@@ -33593,7 +33233,7 @@
       </c>
       <c r="I901" s="31"/>
     </row>
-    <row r="902" spans="1:9" ht="45">
+    <row r="902" spans="1:9" ht="60">
       <c r="A902" s="29" t="s">
         <v>925</v>
       </c>
@@ -33643,7 +33283,7 @@
       </c>
       <c r="I903" s="31"/>
     </row>
-    <row r="904" spans="1:9" ht="45">
+    <row r="904" spans="1:9" ht="60">
       <c r="A904" s="29" t="s">
         <v>927</v>
       </c>
@@ -33670,7 +33310,7 @@
         <v>2912</v>
       </c>
     </row>
-    <row r="905" spans="1:9" ht="45">
+    <row r="905" spans="1:9" ht="60">
       <c r="A905" s="29" t="s">
         <v>928</v>
       </c>
@@ -33722,7 +33362,7 @@
       </c>
       <c r="I906" s="31"/>
     </row>
-    <row r="907" spans="1:9" ht="90">
+    <row r="907" spans="1:9" ht="105">
       <c r="A907" s="29" t="s">
         <v>930</v>
       </c>
@@ -33797,7 +33437,7 @@
       </c>
       <c r="I909" s="31"/>
     </row>
-    <row r="910" spans="1:9" ht="30">
+    <row r="910" spans="1:9" ht="45">
       <c r="A910" s="29" t="s">
         <v>933</v>
       </c>
@@ -33872,7 +33512,7 @@
       </c>
       <c r="I912" s="31"/>
     </row>
-    <row r="913" spans="1:9" ht="45">
+    <row r="913" spans="1:9" ht="60">
       <c r="A913" s="29" t="s">
         <v>936</v>
       </c>
@@ -34047,7 +33687,7 @@
       </c>
       <c r="I919" s="31"/>
     </row>
-    <row r="920" spans="1:9" ht="45">
+    <row r="920" spans="1:9" ht="60">
       <c r="A920" s="29" t="s">
         <v>943</v>
       </c>
@@ -34122,7 +33762,7 @@
       </c>
       <c r="I922" s="31"/>
     </row>
-    <row r="923" spans="1:9" ht="45">
+    <row r="923" spans="1:9" ht="60">
       <c r="A923" s="29" t="s">
         <v>946</v>
       </c>
@@ -34176,7 +33816,7 @@
         <v>2914</v>
       </c>
     </row>
-    <row r="925" spans="1:9" ht="30">
+    <row r="925" spans="1:9" ht="45">
       <c r="A925" s="29" t="s">
         <v>948</v>
       </c>
@@ -34201,7 +33841,7 @@
       </c>
       <c r="I925" s="31"/>
     </row>
-    <row r="926" spans="1:9">
+    <row r="926" spans="1:9" ht="30">
       <c r="A926" s="29" t="s">
         <v>949</v>
       </c>
@@ -34326,7 +33966,7 @@
       </c>
       <c r="I930" s="31"/>
     </row>
-    <row r="931" spans="1:9" ht="135">
+    <row r="931" spans="1:9" ht="195">
       <c r="A931" s="29" t="s">
         <v>954</v>
       </c>
@@ -34700,7 +34340,7 @@
       </c>
       <c r="I944" s="31"/>
     </row>
-    <row r="945" spans="1:9">
+    <row r="945" spans="1:9" ht="30">
       <c r="A945" s="29" t="s">
         <v>968</v>
       </c>
@@ -34775,7 +34415,7 @@
       </c>
       <c r="I947" s="31"/>
     </row>
-    <row r="948" spans="1:9" ht="30">
+    <row r="948" spans="1:9" ht="45">
       <c r="A948" s="29" t="s">
         <v>971</v>
       </c>
@@ -34902,7 +34542,7 @@
         <v>2916</v>
       </c>
     </row>
-    <row r="953" spans="1:9">
+    <row r="953" spans="1:9" ht="30">
       <c r="A953" s="29" t="s">
         <v>976</v>
       </c>
@@ -35002,7 +34642,7 @@
       </c>
       <c r="I956" s="31"/>
     </row>
-    <row r="957" spans="1:9" ht="30">
+    <row r="957" spans="1:9" ht="45">
       <c r="A957" s="29" t="s">
         <v>980</v>
       </c>
@@ -35052,7 +34692,7 @@
       </c>
       <c r="I958" s="31"/>
     </row>
-    <row r="959" spans="1:9">
+    <row r="959" spans="1:9" ht="30">
       <c r="A959" s="29" t="s">
         <v>982</v>
       </c>
@@ -35177,7 +34817,7 @@
       </c>
       <c r="I963" s="31"/>
     </row>
-    <row r="964" spans="1:9" ht="30">
+    <row r="964" spans="1:9" ht="45">
       <c r="A964" s="29" t="s">
         <v>987</v>
       </c>
@@ -35252,7 +34892,7 @@
       </c>
       <c r="I966" s="31"/>
     </row>
-    <row r="967" spans="1:9">
+    <row r="967" spans="1:9" ht="30">
       <c r="A967" s="29" t="s">
         <v>990</v>
       </c>
@@ -35327,7 +34967,7 @@
       </c>
       <c r="I969" s="31"/>
     </row>
-    <row r="970" spans="1:9" ht="45">
+    <row r="970" spans="1:9" ht="60">
       <c r="A970" s="29" t="s">
         <v>993</v>
       </c>
@@ -35354,7 +34994,7 @@
         <v>2917</v>
       </c>
     </row>
-    <row r="971" spans="1:9" ht="45">
+    <row r="971" spans="1:9" ht="60">
       <c r="A971" s="29" t="s">
         <v>994</v>
       </c>
@@ -35431,7 +35071,7 @@
       </c>
       <c r="I973" s="31"/>
     </row>
-    <row r="974" spans="1:9" ht="30">
+    <row r="974" spans="1:9" ht="45">
       <c r="A974" s="29" t="s">
         <v>997</v>
       </c>
@@ -35485,7 +35125,7 @@
         <v>2880</v>
       </c>
     </row>
-    <row r="976" spans="1:9" ht="30">
+    <row r="976" spans="1:9" ht="45">
       <c r="A976" s="29" t="s">
         <v>999</v>
       </c>
@@ -35560,7 +35200,7 @@
       </c>
       <c r="I978" s="31"/>
     </row>
-    <row r="979" spans="1:9" ht="30">
+    <row r="979" spans="1:9" ht="45">
       <c r="A979" s="29" t="s">
         <v>1002</v>
       </c>
@@ -35764,7 +35404,7 @@
       </c>
       <c r="I986" s="31"/>
     </row>
-    <row r="987" spans="1:9" ht="30">
+    <row r="987" spans="1:9" ht="45">
       <c r="A987" s="29" t="s">
         <v>1010</v>
       </c>
@@ -35839,7 +35479,7 @@
       </c>
       <c r="I989" s="31"/>
     </row>
-    <row r="990" spans="1:9">
+    <row r="990" spans="1:9" ht="30">
       <c r="A990" s="29" t="s">
         <v>1013</v>
       </c>
@@ -35864,7 +35504,7 @@
       </c>
       <c r="I990" s="31"/>
     </row>
-    <row r="991" spans="1:9" ht="45">
+    <row r="991" spans="1:9" ht="60">
       <c r="A991" s="29" t="s">
         <v>1014</v>
       </c>
@@ -36264,7 +35904,7 @@
       </c>
       <c r="I1006" s="31"/>
     </row>
-    <row r="1007" spans="1:9">
+    <row r="1007" spans="1:9" ht="30">
       <c r="A1007" s="29" t="s">
         <v>1030</v>
       </c>
@@ -36289,7 +35929,7 @@
       </c>
       <c r="I1007" s="31"/>
     </row>
-    <row r="1008" spans="1:9" ht="30">
+    <row r="1008" spans="1:9" ht="45">
       <c r="A1008" s="29" t="s">
         <v>1031</v>
       </c>
@@ -36564,7 +36204,7 @@
       </c>
       <c r="I1018" s="31"/>
     </row>
-    <row r="1019" spans="1:9">
+    <row r="1019" spans="1:9" ht="30">
       <c r="A1019" s="29" t="s">
         <v>1042</v>
       </c>
@@ -37064,7 +36704,7 @@
       </c>
       <c r="I1038" s="31"/>
     </row>
-    <row r="1039" spans="1:9" ht="30">
+    <row r="1039" spans="1:9" ht="45">
       <c r="A1039" s="29" t="s">
         <v>1062</v>
       </c>
@@ -37114,7 +36754,7 @@
       </c>
       <c r="I1040" s="31"/>
     </row>
-    <row r="1041" spans="1:9" ht="30">
+    <row r="1041" spans="1:9" ht="45">
       <c r="A1041" s="29" t="s">
         <v>1064</v>
       </c>
@@ -37264,7 +36904,7 @@
       </c>
       <c r="I1046" s="31"/>
     </row>
-    <row r="1047" spans="1:9" ht="30">
+    <row r="1047" spans="1:9" ht="45">
       <c r="A1047" s="29" t="s">
         <v>1070</v>
       </c>
@@ -37314,7 +36954,7 @@
       </c>
       <c r="I1048" s="31"/>
     </row>
-    <row r="1049" spans="1:9" ht="30">
+    <row r="1049" spans="1:9" ht="45">
       <c r="A1049" s="29" t="s">
         <v>1072</v>
       </c>
@@ -37339,7 +36979,7 @@
       </c>
       <c r="I1049" s="31"/>
     </row>
-    <row r="1050" spans="1:9" ht="30">
+    <row r="1050" spans="1:9" ht="45">
       <c r="A1050" s="29" t="s">
         <v>1073</v>
       </c>
@@ -37364,7 +37004,7 @@
       </c>
       <c r="I1050" s="31"/>
     </row>
-    <row r="1051" spans="1:9" ht="30">
+    <row r="1051" spans="1:9" ht="45">
       <c r="A1051" s="29" t="s">
         <v>1074</v>
       </c>
@@ -37414,7 +37054,7 @@
       </c>
       <c r="I1052" s="31"/>
     </row>
-    <row r="1053" spans="1:9" ht="30">
+    <row r="1053" spans="1:9" ht="45">
       <c r="A1053" s="29" t="s">
         <v>1076</v>
       </c>
@@ -37514,7 +37154,7 @@
       </c>
       <c r="I1056" s="31"/>
     </row>
-    <row r="1057" spans="1:9" ht="30">
+    <row r="1057" spans="1:9" ht="45">
       <c r="A1057" s="29" t="s">
         <v>1080</v>
       </c>
@@ -37639,7 +37279,7 @@
       </c>
       <c r="I1061" s="31"/>
     </row>
-    <row r="1062" spans="1:9">
+    <row r="1062" spans="1:9" ht="30">
       <c r="A1062" s="29" t="s">
         <v>1085</v>
       </c>
@@ -37714,7 +37354,7 @@
       </c>
       <c r="I1064" s="31"/>
     </row>
-    <row r="1065" spans="1:9" ht="30">
+    <row r="1065" spans="1:9" ht="45">
       <c r="A1065" s="29" t="s">
         <v>1088</v>
       </c>
@@ -37739,7 +37379,7 @@
       </c>
       <c r="I1065" s="31"/>
     </row>
-    <row r="1066" spans="1:9" ht="45">
+    <row r="1066" spans="1:9" ht="60">
       <c r="A1066" s="29" t="s">
         <v>1089</v>
       </c>
@@ -37914,7 +37554,7 @@
       </c>
       <c r="I1072" s="31"/>
     </row>
-    <row r="1073" spans="1:9">
+    <row r="1073" spans="1:9" ht="30">
       <c r="A1073" s="29" t="s">
         <v>1096</v>
       </c>
@@ -37964,7 +37604,7 @@
       </c>
       <c r="I1074" s="31"/>
     </row>
-    <row r="1075" spans="1:9">
+    <row r="1075" spans="1:9" ht="30">
       <c r="A1075" s="29" t="s">
         <v>1098</v>
       </c>
@@ -38089,7 +37729,7 @@
       </c>
       <c r="I1079" s="31"/>
     </row>
-    <row r="1080" spans="1:9">
+    <row r="1080" spans="1:9" ht="30">
       <c r="A1080" s="29" t="s">
         <v>1103</v>
       </c>
@@ -38114,7 +37754,7 @@
       </c>
       <c r="I1080" s="31"/>
     </row>
-    <row r="1081" spans="1:9">
+    <row r="1081" spans="1:9" ht="30">
       <c r="A1081" s="29" t="s">
         <v>1104</v>
       </c>
@@ -38139,7 +37779,7 @@
       </c>
       <c r="I1081" s="31"/>
     </row>
-    <row r="1082" spans="1:9">
+    <row r="1082" spans="1:9" ht="30">
       <c r="A1082" s="29" t="s">
         <v>1105</v>
       </c>
@@ -38214,7 +37854,7 @@
       </c>
       <c r="I1084" s="31"/>
     </row>
-    <row r="1085" spans="1:9">
+    <row r="1085" spans="1:9" ht="30">
       <c r="A1085" s="29" t="s">
         <v>1108</v>
       </c>
@@ -38314,7 +37954,7 @@
       </c>
       <c r="I1088" s="31"/>
     </row>
-    <row r="1089" spans="1:9">
+    <row r="1089" spans="1:9" ht="30">
       <c r="A1089" s="29" t="s">
         <v>1112</v>
       </c>
@@ -38339,7 +37979,7 @@
       </c>
       <c r="I1089" s="31"/>
     </row>
-    <row r="1090" spans="1:9">
+    <row r="1090" spans="1:9" ht="30">
       <c r="A1090" s="29" t="s">
         <v>1113</v>
       </c>
@@ -38414,7 +38054,7 @@
       </c>
       <c r="I1092" s="31"/>
     </row>
-    <row r="1093" spans="1:9" ht="30">
+    <row r="1093" spans="1:9" ht="45">
       <c r="A1093" s="29" t="s">
         <v>1116</v>
       </c>
@@ -38439,7 +38079,7 @@
       </c>
       <c r="I1093" s="31"/>
     </row>
-    <row r="1094" spans="1:9" ht="30">
+    <row r="1094" spans="1:9" ht="45">
       <c r="A1094" s="29" t="s">
         <v>1117</v>
       </c>
@@ -38541,7 +38181,7 @@
       </c>
       <c r="I1097" s="31"/>
     </row>
-    <row r="1098" spans="1:9" ht="30">
+    <row r="1098" spans="1:9" ht="45">
       <c r="A1098" s="29" t="s">
         <v>1121</v>
       </c>
@@ -38566,7 +38206,7 @@
       </c>
       <c r="I1098" s="31"/>
     </row>
-    <row r="1099" spans="1:9" ht="30">
+    <row r="1099" spans="1:9" ht="45">
       <c r="A1099" s="29" t="s">
         <v>1122</v>
       </c>
@@ -38591,7 +38231,7 @@
       </c>
       <c r="I1099" s="31"/>
     </row>
-    <row r="1100" spans="1:9">
+    <row r="1100" spans="1:9" ht="30">
       <c r="A1100" s="29" t="s">
         <v>1123</v>
       </c>
@@ -38641,7 +38281,7 @@
       </c>
       <c r="I1101" s="31"/>
     </row>
-    <row r="1102" spans="1:9" ht="30">
+    <row r="1102" spans="1:9" ht="45">
       <c r="A1102" s="29" t="s">
         <v>1125</v>
       </c>
@@ -38691,7 +38331,7 @@
       </c>
       <c r="I1103" s="31"/>
     </row>
-    <row r="1104" spans="1:9" ht="45">
+    <row r="1104" spans="1:9" ht="60">
       <c r="A1104" s="29" t="s">
         <v>1127</v>
       </c>
@@ -38766,7 +38406,7 @@
       </c>
       <c r="I1106" s="31"/>
     </row>
-    <row r="1107" spans="1:9">
+    <row r="1107" spans="1:9" ht="30">
       <c r="A1107" s="29" t="s">
         <v>1130</v>
       </c>
@@ -38841,7 +38481,7 @@
       </c>
       <c r="I1109" s="31"/>
     </row>
-    <row r="1110" spans="1:9" ht="30">
+    <row r="1110" spans="1:9" ht="45">
       <c r="A1110" s="29" t="s">
         <v>1133</v>
       </c>
@@ -38868,7 +38508,7 @@
         <v>2895</v>
       </c>
     </row>
-    <row r="1111" spans="1:9">
+    <row r="1111" spans="1:9" ht="30">
       <c r="A1111" s="29" t="s">
         <v>1134</v>
       </c>
@@ -38893,7 +38533,7 @@
       </c>
       <c r="I1111" s="31"/>
     </row>
-    <row r="1112" spans="1:9" ht="30">
+    <row r="1112" spans="1:9" ht="45">
       <c r="A1112" s="29" t="s">
         <v>1135</v>
       </c>
@@ -38920,7 +38560,7 @@
         <v>2922</v>
       </c>
     </row>
-    <row r="1113" spans="1:9" ht="30">
+    <row r="1113" spans="1:9" ht="45">
       <c r="A1113" s="29" t="s">
         <v>1136</v>
       </c>
@@ -38945,7 +38585,7 @@
       </c>
       <c r="I1113" s="31"/>
     </row>
-    <row r="1114" spans="1:9" ht="165">
+    <row r="1114" spans="1:9" ht="240">
       <c r="A1114" s="29" t="s">
         <v>1137</v>
       </c>
@@ -38972,7 +38612,7 @@
         <v>2923</v>
       </c>
     </row>
-    <row r="1115" spans="1:9" ht="135">
+    <row r="1115" spans="1:9" ht="195">
       <c r="A1115" s="29" t="s">
         <v>1138</v>
       </c>
@@ -38999,7 +38639,7 @@
         <v>2924</v>
       </c>
     </row>
-    <row r="1116" spans="1:9">
+    <row r="1116" spans="1:9" ht="30">
       <c r="A1116" s="29" t="s">
         <v>1139</v>
       </c>
@@ -39074,7 +38714,7 @@
       </c>
       <c r="I1118" s="31"/>
     </row>
-    <row r="1119" spans="1:9" ht="30">
+    <row r="1119" spans="1:9" ht="45">
       <c r="A1119" s="29" t="s">
         <v>1142</v>
       </c>
@@ -39149,7 +38789,7 @@
       </c>
       <c r="I1121" s="31"/>
     </row>
-    <row r="1122" spans="1:9">
+    <row r="1122" spans="1:9" ht="30">
       <c r="A1122" s="29" t="s">
         <v>1145</v>
       </c>
@@ -39326,7 +38966,7 @@
       </c>
       <c r="I1128" s="31"/>
     </row>
-    <row r="1129" spans="1:9" ht="60">
+    <row r="1129" spans="1:9" ht="75">
       <c r="A1129" s="29" t="s">
         <v>1152</v>
       </c>
@@ -39351,7 +38991,7 @@
       </c>
       <c r="I1129" s="31"/>
     </row>
-    <row r="1130" spans="1:9" ht="45">
+    <row r="1130" spans="1:9" ht="60">
       <c r="A1130" s="29" t="s">
         <v>1153</v>
       </c>
@@ -39376,7 +39016,7 @@
       </c>
       <c r="I1130" s="31"/>
     </row>
-    <row r="1131" spans="1:9" ht="45">
+    <row r="1131" spans="1:9" ht="60">
       <c r="A1131" s="29" t="s">
         <v>1154</v>
       </c>
@@ -39451,7 +39091,7 @@
       </c>
       <c r="I1133" s="31"/>
     </row>
-    <row r="1134" spans="1:9" ht="30">
+    <row r="1134" spans="1:9" ht="45">
       <c r="A1134" s="29" t="s">
         <v>1157</v>
       </c>
@@ -39476,7 +39116,7 @@
       </c>
       <c r="I1134" s="31"/>
     </row>
-    <row r="1135" spans="1:9" ht="30">
+    <row r="1135" spans="1:9" ht="45">
       <c r="A1135" s="29" t="s">
         <v>1158</v>
       </c>
@@ -39501,7 +39141,7 @@
       </c>
       <c r="I1135" s="31"/>
     </row>
-    <row r="1136" spans="1:9" ht="30">
+    <row r="1136" spans="1:9" ht="45">
       <c r="A1136" s="29" t="s">
         <v>1159</v>
       </c>
@@ -39526,7 +39166,7 @@
       </c>
       <c r="I1136" s="31"/>
     </row>
-    <row r="1137" spans="1:9" ht="30">
+    <row r="1137" spans="1:9" ht="45">
       <c r="A1137" s="29" t="s">
         <v>1160</v>
       </c>
@@ -39551,7 +39191,7 @@
       </c>
       <c r="I1137" s="31"/>
     </row>
-    <row r="1138" spans="1:9" ht="30">
+    <row r="1138" spans="1:9" ht="45">
       <c r="A1138" s="29" t="s">
         <v>1161</v>
       </c>
@@ -39601,7 +39241,7 @@
       </c>
       <c r="I1139" s="31"/>
     </row>
-    <row r="1140" spans="1:9" ht="30">
+    <row r="1140" spans="1:9" ht="45">
       <c r="A1140" s="29" t="s">
         <v>1163</v>
       </c>
@@ -39701,7 +39341,7 @@
       </c>
       <c r="I1143" s="31"/>
     </row>
-    <row r="1144" spans="1:9" ht="30">
+    <row r="1144" spans="1:9" ht="45">
       <c r="A1144" s="29" t="s">
         <v>1167</v>
       </c>
@@ -39751,7 +39391,7 @@
       </c>
       <c r="I1145" s="31"/>
     </row>
-    <row r="1146" spans="1:9" ht="30">
+    <row r="1146" spans="1:9" ht="45">
       <c r="A1146" s="29" t="s">
         <v>1169</v>
       </c>
@@ -39826,7 +39466,7 @@
       </c>
       <c r="I1148" s="31"/>
     </row>
-    <row r="1149" spans="1:9" ht="30">
+    <row r="1149" spans="1:9" ht="45">
       <c r="A1149" s="29" t="s">
         <v>1172</v>
       </c>
@@ -39976,7 +39616,7 @@
       </c>
       <c r="I1154" s="31"/>
     </row>
-    <row r="1155" spans="1:9">
+    <row r="1155" spans="1:9" ht="30">
       <c r="A1155" s="29" t="s">
         <v>1178</v>
       </c>
@@ -40101,7 +39741,7 @@
       </c>
       <c r="I1159" s="31"/>
     </row>
-    <row r="1160" spans="1:9" ht="75">
+    <row r="1160" spans="1:9" ht="90">
       <c r="A1160" s="29" t="s">
         <v>1183</v>
       </c>
@@ -40126,7 +39766,7 @@
       </c>
       <c r="I1160" s="31"/>
     </row>
-    <row r="1161" spans="1:9" ht="60">
+    <row r="1161" spans="1:9" ht="75">
       <c r="A1161" s="29" t="s">
         <v>1184</v>
       </c>
@@ -40251,7 +39891,7 @@
       </c>
       <c r="I1165" s="31"/>
     </row>
-    <row r="1166" spans="1:9" ht="30">
+    <row r="1166" spans="1:9" ht="45">
       <c r="A1166" s="29" t="s">
         <v>1189</v>
       </c>
@@ -40276,7 +39916,7 @@
       </c>
       <c r="I1166" s="31"/>
     </row>
-    <row r="1167" spans="1:9" ht="30">
+    <row r="1167" spans="1:9" ht="45">
       <c r="A1167" s="29" t="s">
         <v>1190</v>
       </c>
@@ -40351,7 +39991,7 @@
       </c>
       <c r="I1169" s="31"/>
     </row>
-    <row r="1170" spans="1:9" ht="45">
+    <row r="1170" spans="1:9" ht="60">
       <c r="A1170" s="29" t="s">
         <v>1193</v>
       </c>
@@ -40376,7 +40016,7 @@
       </c>
       <c r="I1170" s="31"/>
     </row>
-    <row r="1171" spans="1:9" ht="60">
+    <row r="1171" spans="1:9" ht="75">
       <c r="A1171" s="29" t="s">
         <v>1194</v>
       </c>
@@ -40403,7 +40043,7 @@
       </c>
       <c r="I1171" s="31"/>
     </row>
-    <row r="1172" spans="1:9" ht="45">
+    <row r="1172" spans="1:9" ht="60">
       <c r="A1172" s="29" t="s">
         <v>1195</v>
       </c>
@@ -40430,7 +40070,7 @@
       </c>
       <c r="I1172" s="31"/>
     </row>
-    <row r="1173" spans="1:9" ht="30">
+    <row r="1173" spans="1:9" ht="45">
       <c r="A1173" s="29" t="s">
         <v>1196</v>
       </c>
@@ -40455,7 +40095,7 @@
       </c>
       <c r="I1173" s="31"/>
     </row>
-    <row r="1174" spans="1:9" ht="30">
+    <row r="1174" spans="1:9" ht="45">
       <c r="A1174" s="29" t="s">
         <v>1197</v>
       </c>
@@ -40507,7 +40147,7 @@
       </c>
       <c r="I1175" s="31"/>
     </row>
-    <row r="1176" spans="1:9" ht="30">
+    <row r="1176" spans="1:9" ht="45">
       <c r="A1176" s="29" t="s">
         <v>1199</v>
       </c>
@@ -40557,7 +40197,7 @@
       </c>
       <c r="I1177" s="31"/>
     </row>
-    <row r="1178" spans="1:9" ht="30">
+    <row r="1178" spans="1:9" ht="45">
       <c r="A1178" s="29" t="s">
         <v>1201</v>
       </c>
@@ -40607,7 +40247,7 @@
       </c>
       <c r="I1179" s="31"/>
     </row>
-    <row r="1180" spans="1:9" ht="30">
+    <row r="1180" spans="1:9" ht="45">
       <c r="A1180" s="29" t="s">
         <v>1203</v>
       </c>
@@ -40682,7 +40322,7 @@
       </c>
       <c r="I1182" s="31"/>
     </row>
-    <row r="1183" spans="1:9" ht="30">
+    <row r="1183" spans="1:9" ht="45">
       <c r="A1183" s="29" t="s">
         <v>1206</v>
       </c>
@@ -40732,7 +40372,7 @@
       </c>
       <c r="I1184" s="31"/>
     </row>
-    <row r="1185" spans="1:9" ht="45">
+    <row r="1185" spans="1:9" ht="60">
       <c r="A1185" s="29" t="s">
         <v>1208</v>
       </c>
@@ -40757,7 +40397,7 @@
       </c>
       <c r="I1185" s="31"/>
     </row>
-    <row r="1186" spans="1:9" ht="30">
+    <row r="1186" spans="1:9" ht="45">
       <c r="A1186" s="29" t="s">
         <v>1209</v>
       </c>
@@ -40782,7 +40422,7 @@
       </c>
       <c r="I1186" s="31"/>
     </row>
-    <row r="1187" spans="1:9">
+    <row r="1187" spans="1:9" ht="30">
       <c r="A1187" s="29" t="s">
         <v>1210</v>
       </c>
@@ -40884,7 +40524,7 @@
         <v>2895</v>
       </c>
     </row>
-    <row r="1191" spans="1:9" ht="30">
+    <row r="1191" spans="1:9" ht="45">
       <c r="A1191" s="29" t="s">
         <v>1214</v>
       </c>
@@ -40911,7 +40551,7 @@
         <v>2922</v>
       </c>
     </row>
-    <row r="1192" spans="1:9" ht="30">
+    <row r="1192" spans="1:9" ht="45">
       <c r="A1192" s="29" t="s">
         <v>1215</v>
       </c>
@@ -40936,7 +40576,7 @@
       </c>
       <c r="I1192" s="31"/>
     </row>
-    <row r="1193" spans="1:9" ht="45">
+    <row r="1193" spans="1:9" ht="60">
       <c r="A1193" s="29" t="s">
         <v>1216</v>
       </c>
@@ -40963,7 +40603,7 @@
         <v>2913</v>
       </c>
     </row>
-    <row r="1194" spans="1:9" ht="45">
+    <row r="1194" spans="1:9" ht="60">
       <c r="A1194" s="29" t="s">
         <v>1217</v>
       </c>
@@ -41090,7 +40730,7 @@
       </c>
       <c r="I1198" s="31"/>
     </row>
-    <row r="1199" spans="1:9" ht="45">
+    <row r="1199" spans="1:9" ht="60">
       <c r="A1199" s="29" t="s">
         <v>1222</v>
       </c>
@@ -41140,7 +40780,7 @@
       </c>
       <c r="I1200" s="31"/>
     </row>
-    <row r="1201" spans="1:9" ht="30">
+    <row r="1201" spans="1:9" ht="45">
       <c r="A1201" s="29" t="s">
         <v>1224</v>
       </c>
@@ -41190,7 +40830,7 @@
       </c>
       <c r="I1202" s="31"/>
     </row>
-    <row r="1203" spans="1:9">
+    <row r="1203" spans="1:9" ht="30">
       <c r="A1203" s="29" t="s">
         <v>1226</v>
       </c>
@@ -41290,7 +40930,7 @@
       </c>
       <c r="I1206" s="31"/>
     </row>
-    <row r="1207" spans="1:9" ht="30">
+    <row r="1207" spans="1:9" ht="45">
       <c r="A1207" s="29" t="s">
         <v>1230</v>
       </c>
@@ -41315,7 +40955,7 @@
       </c>
       <c r="I1207" s="31"/>
     </row>
-    <row r="1208" spans="1:9" ht="90">
+    <row r="1208" spans="1:9" ht="105">
       <c r="A1208" s="29" t="s">
         <v>1231</v>
       </c>
@@ -41340,7 +40980,7 @@
       </c>
       <c r="I1208" s="31"/>
     </row>
-    <row r="1209" spans="1:9" ht="75">
+    <row r="1209" spans="1:9" ht="90">
       <c r="A1209" s="29" t="s">
         <v>1232</v>
       </c>
@@ -41365,7 +41005,7 @@
       </c>
       <c r="I1209" s="31"/>
     </row>
-    <row r="1210" spans="1:9" ht="75">
+    <row r="1210" spans="1:9" ht="90">
       <c r="A1210" s="29" t="s">
         <v>1233</v>
       </c>
@@ -41390,7 +41030,7 @@
       </c>
       <c r="I1210" s="31"/>
     </row>
-    <row r="1211" spans="1:9" ht="30">
+    <row r="1211" spans="1:9" ht="45">
       <c r="A1211" s="29" t="s">
         <v>1234</v>
       </c>
@@ -41440,7 +41080,7 @@
       </c>
       <c r="I1212" s="31"/>
     </row>
-    <row r="1213" spans="1:9" ht="30">
+    <row r="1213" spans="1:9" ht="45">
       <c r="A1213" s="29" t="s">
         <v>1236</v>
       </c>
@@ -41465,7 +41105,7 @@
       </c>
       <c r="I1213" s="31"/>
     </row>
-    <row r="1214" spans="1:9" ht="30">
+    <row r="1214" spans="1:9" ht="45">
       <c r="A1214" s="29" t="s">
         <v>1237</v>
       </c>
@@ -41540,7 +41180,7 @@
       </c>
       <c r="I1216" s="31"/>
     </row>
-    <row r="1217" spans="1:9" ht="30">
+    <row r="1217" spans="1:9" ht="45">
       <c r="A1217" s="29" t="s">
         <v>1240</v>
       </c>
@@ -41590,7 +41230,7 @@
       </c>
       <c r="I1218" s="31"/>
     </row>
-    <row r="1219" spans="1:9" ht="30">
+    <row r="1219" spans="1:9" ht="45">
       <c r="A1219" s="29" t="s">
         <v>1242</v>
       </c>
@@ -41640,7 +41280,7 @@
       </c>
       <c r="I1220" s="31"/>
     </row>
-    <row r="1221" spans="1:9" ht="30">
+    <row r="1221" spans="1:9" ht="45">
       <c r="A1221" s="29" t="s">
         <v>1244</v>
       </c>
@@ -41665,7 +41305,7 @@
       </c>
       <c r="I1221" s="31"/>
     </row>
-    <row r="1222" spans="1:9" ht="30">
+    <row r="1222" spans="1:9" ht="45">
       <c r="A1222" s="29" t="s">
         <v>1245</v>
       </c>
@@ -41740,7 +41380,7 @@
       </c>
       <c r="I1224" s="31"/>
     </row>
-    <row r="1225" spans="1:9" ht="30">
+    <row r="1225" spans="1:9" ht="45">
       <c r="A1225" s="29" t="s">
         <v>1248</v>
       </c>
@@ -41765,7 +41405,7 @@
       </c>
       <c r="I1225" s="31"/>
     </row>
-    <row r="1226" spans="1:9" ht="30">
+    <row r="1226" spans="1:9" ht="45">
       <c r="A1226" s="29" t="s">
         <v>1249</v>
       </c>
@@ -41790,7 +41430,7 @@
       </c>
       <c r="I1226" s="31"/>
     </row>
-    <row r="1227" spans="1:9" ht="45">
+    <row r="1227" spans="1:9" ht="60">
       <c r="A1227" s="29" t="s">
         <v>1250</v>
       </c>
@@ -41915,7 +41555,7 @@
       </c>
       <c r="I1231" s="31"/>
     </row>
-    <row r="1232" spans="1:9" ht="60">
+    <row r="1232" spans="1:9" ht="75">
       <c r="A1232" s="29" t="s">
         <v>1255</v>
       </c>
@@ -41965,7 +41605,7 @@
       </c>
       <c r="I1233" s="31"/>
     </row>
-    <row r="1234" spans="1:9" ht="75">
+    <row r="1234" spans="1:9" ht="90">
       <c r="A1234" s="29" t="s">
         <v>1257</v>
       </c>
@@ -41990,7 +41630,7 @@
       </c>
       <c r="I1234" s="31"/>
     </row>
-    <row r="1235" spans="1:9" ht="30">
+    <row r="1235" spans="1:9" ht="45">
       <c r="A1235" s="29" t="s">
         <v>1258</v>
       </c>
@@ -42065,7 +41705,7 @@
       </c>
       <c r="I1237" s="31"/>
     </row>
-    <row r="1238" spans="1:9" ht="90">
+    <row r="1238" spans="1:9" ht="105">
       <c r="A1238" s="29" t="s">
         <v>1261</v>
       </c>
@@ -42140,7 +41780,7 @@
       </c>
       <c r="I1240" s="31"/>
     </row>
-    <row r="1241" spans="1:9" ht="30">
+    <row r="1241" spans="1:9" ht="45">
       <c r="A1241" s="29" t="s">
         <v>1264</v>
       </c>
@@ -42215,7 +41855,7 @@
       </c>
       <c r="I1243" s="31"/>
     </row>
-    <row r="1244" spans="1:9" ht="75">
+    <row r="1244" spans="1:9" ht="90">
       <c r="A1244" s="29" t="s">
         <v>1267</v>
       </c>
@@ -42240,7 +41880,7 @@
       </c>
       <c r="I1244" s="31"/>
     </row>
-    <row r="1245" spans="1:9" ht="30">
+    <row r="1245" spans="1:9" ht="45">
       <c r="A1245" s="29" t="s">
         <v>1268</v>
       </c>
@@ -42265,7 +41905,7 @@
       </c>
       <c r="I1245" s="31"/>
     </row>
-    <row r="1246" spans="1:9" ht="75">
+    <row r="1246" spans="1:9" ht="90">
       <c r="A1246" s="29" t="s">
         <v>1269</v>
       </c>
@@ -42290,7 +41930,7 @@
       </c>
       <c r="I1246" s="31"/>
     </row>
-    <row r="1247" spans="1:9" ht="30">
+    <row r="1247" spans="1:9" ht="45">
       <c r="A1247" s="29" t="s">
         <v>1270</v>
       </c>
@@ -42340,7 +41980,7 @@
       </c>
       <c r="I1248" s="31"/>
     </row>
-    <row r="1249" spans="1:9" ht="30">
+    <row r="1249" spans="1:9" ht="45">
       <c r="A1249" s="29" t="s">
         <v>1272</v>
       </c>
@@ -42365,7 +42005,7 @@
       </c>
       <c r="I1249" s="31"/>
     </row>
-    <row r="1250" spans="1:9" ht="90">
+    <row r="1250" spans="1:9" ht="105">
       <c r="A1250" s="29" t="s">
         <v>1273</v>
       </c>
@@ -42590,7 +42230,7 @@
       </c>
       <c r="I1258" s="31"/>
     </row>
-    <row r="1259" spans="1:9" ht="45">
+    <row r="1259" spans="1:9" ht="60">
       <c r="A1259" s="29" t="s">
         <v>1282</v>
       </c>
@@ -42640,7 +42280,7 @@
       </c>
       <c r="I1260" s="31"/>
     </row>
-    <row r="1261" spans="1:9" ht="30">
+    <row r="1261" spans="1:9" ht="45">
       <c r="A1261" s="29" t="s">
         <v>1284</v>
       </c>
@@ -42765,7 +42405,7 @@
       </c>
       <c r="I1265" s="31"/>
     </row>
-    <row r="1266" spans="1:9" ht="75">
+    <row r="1266" spans="1:9" ht="90">
       <c r="A1266" s="29" t="s">
         <v>1289</v>
       </c>
@@ -42840,7 +42480,7 @@
       </c>
       <c r="I1268" s="31"/>
     </row>
-    <row r="1269" spans="1:9">
+    <row r="1269" spans="1:9" ht="30">
       <c r="A1269" s="29" t="s">
         <v>1292</v>
       </c>
@@ -42865,7 +42505,7 @@
       </c>
       <c r="I1269" s="31"/>
     </row>
-    <row r="1270" spans="1:9" ht="30">
+    <row r="1270" spans="1:9" ht="45">
       <c r="A1270" s="29" t="s">
         <v>1293</v>
       </c>
@@ -42915,7 +42555,7 @@
       </c>
       <c r="I1271" s="31"/>
     </row>
-    <row r="1272" spans="1:9" ht="30">
+    <row r="1272" spans="1:9" ht="45">
       <c r="A1272" s="29" t="s">
         <v>1295</v>
       </c>
@@ -43015,7 +42655,7 @@
       </c>
       <c r="I1275" s="31"/>
     </row>
-    <row r="1276" spans="1:9">
+    <row r="1276" spans="1:9" ht="30">
       <c r="A1276" s="29" t="s">
         <v>1299</v>
       </c>
@@ -43092,7 +42732,7 @@
       </c>
       <c r="I1278" s="31"/>
     </row>
-    <row r="1279" spans="1:9">
+    <row r="1279" spans="1:9" ht="30">
       <c r="A1279" s="29" t="s">
         <v>1302</v>
       </c>
@@ -43192,7 +42832,7 @@
       </c>
       <c r="I1282" s="31"/>
     </row>
-    <row r="1283" spans="1:9" ht="30">
+    <row r="1283" spans="1:9" ht="45">
       <c r="A1283" s="29" t="s">
         <v>1306</v>
       </c>
@@ -43267,7 +42907,7 @@
       </c>
       <c r="I1285" s="31"/>
     </row>
-    <row r="1286" spans="1:9" ht="30">
+    <row r="1286" spans="1:9" ht="45">
       <c r="A1286" s="29" t="s">
         <v>1309</v>
       </c>
@@ -43417,7 +43057,7 @@
       </c>
       <c r="I1291" s="31"/>
     </row>
-    <row r="1292" spans="1:9" ht="30">
+    <row r="1292" spans="1:9" ht="45">
       <c r="A1292" s="29" t="s">
         <v>1315</v>
       </c>
@@ -43444,7 +43084,7 @@
         <v>2927</v>
       </c>
     </row>
-    <row r="1293" spans="1:9" ht="30">
+    <row r="1293" spans="1:9" ht="45">
       <c r="A1293" s="29" t="s">
         <v>1316</v>
       </c>
@@ -43496,7 +43136,7 @@
       </c>
       <c r="I1294" s="31"/>
     </row>
-    <row r="1295" spans="1:9">
+    <row r="1295" spans="1:9" ht="30">
       <c r="A1295" s="29" t="s">
         <v>1318</v>
       </c>
@@ -43546,7 +43186,7 @@
       </c>
       <c r="I1296" s="31"/>
     </row>
-    <row r="1297" spans="1:9" ht="45">
+    <row r="1297" spans="1:9" ht="60">
       <c r="A1297" s="29" t="s">
         <v>1320</v>
       </c>
@@ -43650,7 +43290,7 @@
         <v>2930</v>
       </c>
     </row>
-    <row r="1301" spans="1:9">
+    <row r="1301" spans="1:9" ht="30">
       <c r="A1301" s="29" t="s">
         <v>1324</v>
       </c>
@@ -43675,7 +43315,7 @@
       </c>
       <c r="I1301" s="31"/>
     </row>
-    <row r="1302" spans="1:9">
+    <row r="1302" spans="1:9" ht="30">
       <c r="A1302" s="29" t="s">
         <v>1325</v>
       </c>
@@ -43725,7 +43365,7 @@
       </c>
       <c r="I1303" s="31"/>
     </row>
-    <row r="1304" spans="1:9" ht="30">
+    <row r="1304" spans="1:9" ht="45">
       <c r="A1304" s="29" t="s">
         <v>1327</v>
       </c>
@@ -43775,7 +43415,7 @@
       </c>
       <c r="I1305" s="31"/>
     </row>
-    <row r="1306" spans="1:9" ht="30">
+    <row r="1306" spans="1:9" ht="45">
       <c r="A1306" s="29" t="s">
         <v>1329</v>
       </c>
@@ -43977,7 +43617,7 @@
         <v>2931</v>
       </c>
     </row>
-    <row r="1314" spans="1:9" ht="45">
+    <row r="1314" spans="1:9" ht="60">
       <c r="A1314" s="29" t="s">
         <v>1337</v>
       </c>
@@ -44027,7 +43667,7 @@
       </c>
       <c r="I1315" s="31"/>
     </row>
-    <row r="1316" spans="1:9">
+    <row r="1316" spans="1:9" ht="30">
       <c r="A1316" s="29" t="s">
         <v>1339</v>
       </c>
@@ -44102,7 +43742,7 @@
       </c>
       <c r="I1318" s="31"/>
     </row>
-    <row r="1319" spans="1:9" ht="30">
+    <row r="1319" spans="1:9" ht="45">
       <c r="A1319" s="29" t="s">
         <v>1342</v>
       </c>
@@ -44127,7 +43767,7 @@
       </c>
       <c r="I1319" s="31"/>
     </row>
-    <row r="1320" spans="1:9">
+    <row r="1320" spans="1:9" ht="30">
       <c r="A1320" s="29" t="s">
         <v>1343</v>
       </c>
@@ -44177,7 +43817,7 @@
       </c>
       <c r="I1321" s="31"/>
     </row>
-    <row r="1322" spans="1:9" ht="30">
+    <row r="1322" spans="1:9" ht="45">
       <c r="A1322" s="29" t="s">
         <v>1345</v>
       </c>
@@ -44227,7 +43867,7 @@
       </c>
       <c r="I1323" s="31"/>
     </row>
-    <row r="1324" spans="1:9" ht="30">
+    <row r="1324" spans="1:9" ht="45">
       <c r="A1324" s="29" t="s">
         <v>1347</v>
       </c>
@@ -44277,7 +43917,7 @@
       </c>
       <c r="I1325" s="31"/>
     </row>
-    <row r="1326" spans="1:9" ht="45">
+    <row r="1326" spans="1:9" ht="60">
       <c r="A1326" s="29" t="s">
         <v>1349</v>
       </c>
@@ -44402,7 +44042,7 @@
       </c>
       <c r="I1330" s="31"/>
     </row>
-    <row r="1331" spans="1:9" ht="30">
+    <row r="1331" spans="1:9" ht="45">
       <c r="A1331" s="29" t="s">
         <v>1354</v>
       </c>
@@ -44645,7 +44285,7 @@
       </c>
       <c r="I1339" s="31"/>
     </row>
-    <row r="1340" spans="1:9" ht="30">
+    <row r="1340" spans="1:9" ht="45">
       <c r="A1340" s="29" t="s">
         <v>1363</v>
       </c>
@@ -44745,7 +44385,7 @@
       </c>
       <c r="I1343" s="31"/>
     </row>
-    <row r="1344" spans="1:9" ht="45">
+    <row r="1344" spans="1:9" ht="60">
       <c r="A1344" s="29" t="s">
         <v>1368</v>
       </c>
@@ -44853,7 +44493,7 @@
       </c>
       <c r="I1347" s="31"/>
     </row>
-    <row r="1348" spans="1:9" ht="45">
+    <row r="1348" spans="1:9" ht="60">
       <c r="A1348" s="29" t="s">
         <v>3089</v>
       </c>
@@ -45100,7 +44740,7 @@
         <v>2932</v>
       </c>
     </row>
-    <row r="1357" spans="1:9" ht="30">
+    <row r="1357" spans="1:9" ht="45">
       <c r="A1357" s="29" t="s">
         <v>1379</v>
       </c>
@@ -45127,7 +44767,7 @@
       </c>
       <c r="I1357" s="31"/>
     </row>
-    <row r="1358" spans="1:9" ht="30">
+    <row r="1358" spans="1:9" ht="45">
       <c r="A1358" s="29" t="s">
         <v>1380</v>
       </c>
@@ -45210,7 +44850,7 @@
       </c>
       <c r="I1360" s="31"/>
     </row>
-    <row r="1361" spans="1:9" ht="75">
+    <row r="1361" spans="1:9" ht="90">
       <c r="A1361" s="29" t="s">
         <v>1383</v>
       </c>
@@ -45239,7 +44879,7 @@
         <v>2932</v>
       </c>
     </row>
-    <row r="1362" spans="1:9" ht="45">
+    <row r="1362" spans="1:9" ht="60">
       <c r="A1362" s="29" t="s">
         <v>1384</v>
       </c>
@@ -45264,7 +44904,7 @@
       </c>
       <c r="I1362" s="31"/>
     </row>
-    <row r="1363" spans="1:9" ht="30">
+    <row r="1363" spans="1:9" ht="45">
       <c r="A1363" s="29" t="s">
         <v>1385</v>
       </c>
@@ -45320,7 +44960,7 @@
         <v>2932</v>
       </c>
     </row>
-    <row r="1365" spans="1:9" ht="30">
+    <row r="1365" spans="1:9" ht="45">
       <c r="A1365" s="29" t="s">
         <v>1387</v>
       </c>
@@ -45376,7 +45016,7 @@
         <v>2932</v>
       </c>
     </row>
-    <row r="1367" spans="1:9" ht="75">
+    <row r="1367" spans="1:9" ht="90">
       <c r="A1367" s="29" t="s">
         <v>1389</v>
       </c>
@@ -45851,7 +45491,7 @@
         <v>2932</v>
       </c>
     </row>
-    <row r="1384" spans="1:9" ht="45">
+    <row r="1384" spans="1:9" ht="60">
       <c r="A1384" s="29" t="s">
         <v>1406</v>
       </c>
@@ -45880,7 +45520,7 @@
         <v>2932</v>
       </c>
     </row>
-    <row r="1385" spans="1:9" ht="60">
+    <row r="1385" spans="1:9" ht="75">
       <c r="A1385" s="29" t="s">
         <v>3013</v>
       </c>
@@ -45909,7 +45549,7 @@
         <v>2932</v>
       </c>
     </row>
-    <row r="1386" spans="1:9" ht="45">
+    <row r="1386" spans="1:9" ht="60">
       <c r="A1386" s="29" t="s">
         <v>1407</v>
       </c>
@@ -45996,7 +45636,7 @@
         <v>2932</v>
       </c>
     </row>
-    <row r="1389" spans="1:9" ht="30">
+    <row r="1389" spans="1:9" ht="45">
       <c r="A1389" s="29" t="s">
         <v>1411</v>
       </c>
@@ -46313,7 +45953,7 @@
         <v>2932</v>
       </c>
     </row>
-    <row r="1400" spans="1:9" ht="45">
+    <row r="1400" spans="1:9" ht="60">
       <c r="A1400" s="29" t="s">
         <v>1420</v>
       </c>
@@ -46371,7 +46011,7 @@
         <v>2932</v>
       </c>
     </row>
-    <row r="1402" spans="1:9" ht="30">
+    <row r="1402" spans="1:9" ht="45">
       <c r="A1402" s="29" t="s">
         <v>1422</v>
       </c>
@@ -46427,7 +46067,7 @@
       </c>
       <c r="I1403" s="31"/>
     </row>
-    <row r="1404" spans="1:9" ht="45">
+    <row r="1404" spans="1:9" ht="60">
       <c r="A1404" s="29" t="s">
         <v>1424</v>
       </c>
@@ -46456,7 +46096,7 @@
         <v>2932</v>
       </c>
     </row>
-    <row r="1405" spans="1:9" ht="45">
+    <row r="1405" spans="1:9" ht="60">
       <c r="A1405" s="29" t="s">
         <v>1425</v>
       </c>
@@ -46485,7 +46125,7 @@
         <v>2932</v>
       </c>
     </row>
-    <row r="1406" spans="1:9" ht="30">
+    <row r="1406" spans="1:9" ht="45">
       <c r="A1406" s="29" t="s">
         <v>1426</v>
       </c>
@@ -46510,7 +46150,7 @@
       </c>
       <c r="I1406" s="31"/>
     </row>
-    <row r="1407" spans="1:9" ht="30">
+    <row r="1407" spans="1:9" ht="45">
       <c r="A1407" s="29" t="s">
         <v>1427</v>
       </c>
@@ -46535,7 +46175,7 @@
       </c>
       <c r="I1407" s="31"/>
     </row>
-    <row r="1408" spans="1:9" ht="30">
+    <row r="1408" spans="1:9" ht="45">
       <c r="A1408" s="29" t="s">
         <v>1428</v>
       </c>
@@ -46560,7 +46200,7 @@
       </c>
       <c r="I1408" s="31"/>
     </row>
-    <row r="1409" spans="1:9" ht="30">
+    <row r="1409" spans="1:9" ht="45">
       <c r="A1409" s="29" t="s">
         <v>1429</v>
       </c>
@@ -46585,7 +46225,7 @@
       </c>
       <c r="I1409" s="31"/>
     </row>
-    <row r="1410" spans="1:9" ht="30">
+    <row r="1410" spans="1:9" ht="45">
       <c r="A1410" s="29" t="s">
         <v>1430</v>
       </c>
@@ -46610,7 +46250,7 @@
       </c>
       <c r="I1410" s="31"/>
     </row>
-    <row r="1411" spans="1:9" ht="30">
+    <row r="1411" spans="1:9" ht="45">
       <c r="A1411" s="29" t="s">
         <v>1431</v>
       </c>
@@ -46635,7 +46275,7 @@
       </c>
       <c r="I1411" s="31"/>
     </row>
-    <row r="1412" spans="1:9" ht="30">
+    <row r="1412" spans="1:9" ht="45">
       <c r="A1412" s="29" t="s">
         <v>1432</v>
       </c>
@@ -46660,7 +46300,7 @@
       </c>
       <c r="I1412" s="31"/>
     </row>
-    <row r="1413" spans="1:9" ht="30">
+    <row r="1413" spans="1:9" ht="45">
       <c r="A1413" s="29" t="s">
         <v>1433</v>
       </c>
@@ -46685,7 +46325,7 @@
       </c>
       <c r="I1413" s="31"/>
     </row>
-    <row r="1414" spans="1:9" ht="30">
+    <row r="1414" spans="1:9" ht="45">
       <c r="A1414" s="29" t="s">
         <v>1434</v>
       </c>
@@ -46710,7 +46350,7 @@
       </c>
       <c r="I1414" s="31"/>
     </row>
-    <row r="1415" spans="1:9" ht="30">
+    <row r="1415" spans="1:9" ht="45">
       <c r="A1415" s="29" t="s">
         <v>1435</v>
       </c>
@@ -46735,7 +46375,7 @@
       </c>
       <c r="I1415" s="31"/>
     </row>
-    <row r="1416" spans="1:9" ht="30">
+    <row r="1416" spans="1:9" ht="45">
       <c r="A1416" s="29" t="s">
         <v>1436</v>
       </c>
@@ -46760,7 +46400,7 @@
       </c>
       <c r="I1416" s="31"/>
     </row>
-    <row r="1417" spans="1:9" ht="30">
+    <row r="1417" spans="1:9" ht="45">
       <c r="A1417" s="29" t="s">
         <v>1437</v>
       </c>
@@ -46785,7 +46425,7 @@
       </c>
       <c r="I1417" s="31"/>
     </row>
-    <row r="1418" spans="1:9" ht="30">
+    <row r="1418" spans="1:9" ht="45">
       <c r="A1418" s="29" t="s">
         <v>1438</v>
       </c>
@@ -46810,7 +46450,7 @@
       </c>
       <c r="I1418" s="31"/>
     </row>
-    <row r="1419" spans="1:9" ht="30">
+    <row r="1419" spans="1:9" ht="45">
       <c r="A1419" s="29" t="s">
         <v>1439</v>
       </c>
@@ -46835,7 +46475,7 @@
       </c>
       <c r="I1419" s="31"/>
     </row>
-    <row r="1420" spans="1:9" ht="30">
+    <row r="1420" spans="1:9" ht="45">
       <c r="A1420" s="29" t="s">
         <v>1440</v>
       </c>
@@ -46860,7 +46500,7 @@
       </c>
       <c r="I1420" s="31"/>
     </row>
-    <row r="1421" spans="1:9" ht="30">
+    <row r="1421" spans="1:9" ht="45">
       <c r="A1421" s="29" t="s">
         <v>1441</v>
       </c>
@@ -46885,7 +46525,7 @@
       </c>
       <c r="I1421" s="31"/>
     </row>
-    <row r="1422" spans="1:9" ht="30">
+    <row r="1422" spans="1:9" ht="45">
       <c r="A1422" s="29" t="s">
         <v>1442</v>
       </c>
@@ -46910,7 +46550,7 @@
       </c>
       <c r="I1422" s="31"/>
     </row>
-    <row r="1423" spans="1:9" ht="30">
+    <row r="1423" spans="1:9" ht="45">
       <c r="A1423" s="29" t="s">
         <v>1443</v>
       </c>
@@ -46935,7 +46575,7 @@
       </c>
       <c r="I1423" s="31"/>
     </row>
-    <row r="1424" spans="1:9" ht="30">
+    <row r="1424" spans="1:9" ht="45">
       <c r="A1424" s="29" t="s">
         <v>1444</v>
       </c>
@@ -46960,7 +46600,7 @@
       </c>
       <c r="I1424" s="31"/>
     </row>
-    <row r="1425" spans="1:9" ht="30">
+    <row r="1425" spans="1:9" ht="45">
       <c r="A1425" s="29" t="s">
         <v>1445</v>
       </c>
@@ -46985,7 +46625,7 @@
       </c>
       <c r="I1425" s="31"/>
     </row>
-    <row r="1426" spans="1:9" ht="30">
+    <row r="1426" spans="1:9" ht="45">
       <c r="A1426" s="29" t="s">
         <v>1446</v>
       </c>
@@ -47010,7 +46650,7 @@
       </c>
       <c r="I1426" s="31"/>
     </row>
-    <row r="1427" spans="1:9" ht="30">
+    <row r="1427" spans="1:9" ht="45">
       <c r="A1427" s="29" t="s">
         <v>1447</v>
       </c>
@@ -47035,7 +46675,7 @@
       </c>
       <c r="I1427" s="31"/>
     </row>
-    <row r="1428" spans="1:9" ht="30">
+    <row r="1428" spans="1:9" ht="45">
       <c r="A1428" s="29" t="s">
         <v>1448</v>
       </c>
@@ -47060,7 +46700,7 @@
       </c>
       <c r="I1428" s="31"/>
     </row>
-    <row r="1429" spans="1:9" ht="30">
+    <row r="1429" spans="1:9" ht="45">
       <c r="A1429" s="29" t="s">
         <v>1449</v>
       </c>
@@ -47110,7 +46750,7 @@
       </c>
       <c r="I1430" s="31"/>
     </row>
-    <row r="1431" spans="1:9" ht="45">
+    <row r="1431" spans="1:9" ht="60">
       <c r="A1431" s="29" t="s">
         <v>1451</v>
       </c>
@@ -47185,7 +46825,7 @@
       </c>
       <c r="I1433" s="31"/>
     </row>
-    <row r="1434" spans="1:9" ht="30">
+    <row r="1434" spans="1:9" ht="45">
       <c r="A1434" s="29" t="s">
         <v>1454</v>
       </c>
@@ -47310,7 +46950,7 @@
       </c>
       <c r="I1438" s="31"/>
     </row>
-    <row r="1439" spans="1:9" ht="30">
+    <row r="1439" spans="1:9" ht="45">
       <c r="A1439" s="29" t="s">
         <v>1459</v>
       </c>
@@ -47418,7 +47058,7 @@
         <v>2932</v>
       </c>
     </row>
-    <row r="1443" spans="1:9" ht="45">
+    <row r="1443" spans="1:9" ht="60">
       <c r="A1443" s="29" t="s">
         <v>1463</v>
       </c>
@@ -47499,7 +47139,7 @@
       </c>
       <c r="I1445" s="31"/>
     </row>
-    <row r="1446" spans="1:9" ht="45">
+    <row r="1446" spans="1:9" ht="60">
       <c r="A1446" s="29" t="s">
         <v>1466</v>
       </c>
@@ -47549,32 +47189,32 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:I1446">
-    <cfRule type="expression" dxfId="98" priority="53">
+    <cfRule type="expression" dxfId="26" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="54">
+    <cfRule type="expression" dxfId="25" priority="54">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="61">
+    <cfRule type="expression" dxfId="24" priority="61">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:I1446">
-    <cfRule type="expression" dxfId="95" priority="7">
+    <cfRule type="expression" dxfId="23" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="8">
+    <cfRule type="expression" dxfId="22" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="9">
+    <cfRule type="expression" dxfId="21" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F1446">
-    <cfRule type="expression" dxfId="92" priority="13">
+    <cfRule type="expression" dxfId="20" priority="13">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="14">
+    <cfRule type="expression" dxfId="19" priority="14">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
[MS-OXCRPC]: Fix watchman issues.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCRPC/MS-OXCRPC_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCRPC/MS-OXCRPC_RequirementSpecification.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10265" uniqueCount="3090">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10264" uniqueCount="3090">
   <si>
     <t>Req ID</t>
   </si>
@@ -8971,18 +8971,12 @@
     <t>Verified by derived requirements: MS-OXCRPC_R1899, MS-OXCRPC_R1934.</t>
   </si>
   <si>
-    <t>Verified by derived requirements: MS-OXCRPC_R1374, MS-OXCRPC_R1939.</t>
-  </si>
-  <si>
     <t>Verified by derived requirements: MS-OXCRPC_R1900, MS-OXCRPC_R1508.</t>
   </si>
   <si>
     <t>Partially verified by derived requirement: MS-OXCRPC_R4852.</t>
   </si>
   <si>
-    <t>Verified by derived requirements: MS-OXCRPC_R664, MS-OXCRPC_R1924.</t>
-  </si>
-  <si>
     <t>Verified by derived requirements: MS-OXCRPC_R1403, MS-OXCRPC_R1926.</t>
   </si>
   <si>
@@ -9071,9 +9065,6 @@
   </si>
   <si>
     <t>Verified by requirement: MS-OXCRPC_R1845.</t>
-  </si>
-  <si>
-    <t>Verified by derived requirement: MS-OXCRPC_R1558.</t>
   </si>
   <si>
     <t>[In Appendix B: Product Behavior] Implementation does fail with error code ecRpcFailed (0x80040115) if the request buffer is smaller than the size of RPC_HEADER_EXT (0x00000008 bytes). (Microsoft Exchange Server 2010 SP2 and above follow this behavior.)</t>
@@ -9534,6 +9525,15 @@
   <si>
     <t>MS-OXCRPC_R1748</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Verified by derived requirements: MS-OXCRPC_R1374, MS-OXCRPC_R2001, MS-OXCRPC_R1939.</t>
+  </si>
+  <si>
+    <t>Verified by derived requirements: MS-OXCRPC_R664, MS-OXCRPC_R1924, MS-OXCRPC_R2002.</t>
+  </si>
+  <si>
+    <t>Verified by derived requirements: MS-OXCRPC_R4880, MS-OXCRPC_R1558.</t>
   </si>
 </sst>
 </file>
@@ -9808,6 +9808,21 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -9831,21 +9846,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10718,7 +10718,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>2933</v>
+        <v>2931</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>27</v>
@@ -10728,7 +10728,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="6" t="s">
-        <v>2934</v>
+        <v>2932</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -10742,7 +10742,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>2939</v>
+        <v>2936</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>26</v>
@@ -10753,127 +10753,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -10886,12 +10886,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -10904,12 +10904,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -10922,12 +10922,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -10940,60 +10940,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -17546,7 +17546,7 @@
         <v>1492</v>
       </c>
       <c r="C279" s="31" t="s">
-        <v>2940</v>
+        <v>2937</v>
       </c>
       <c r="D279" s="29"/>
       <c r="E279" s="29" t="s">
@@ -17646,7 +17646,7 @@
         <v>1492</v>
       </c>
       <c r="C283" s="31" t="s">
-        <v>2941</v>
+        <v>2938</v>
       </c>
       <c r="D283" s="29"/>
       <c r="E283" s="29" t="s">
@@ -17950,7 +17950,7 @@
         <v>1495</v>
       </c>
       <c r="C295" s="31" t="s">
-        <v>2942</v>
+        <v>2939</v>
       </c>
       <c r="D295" s="29"/>
       <c r="E295" s="29" t="s">
@@ -17975,7 +17975,7 @@
         <v>1495</v>
       </c>
       <c r="C296" s="31" t="s">
-        <v>2943</v>
+        <v>2940</v>
       </c>
       <c r="D296" s="29"/>
       <c r="E296" s="29" t="s">
@@ -20006,7 +20006,7 @@
         <v>1503</v>
       </c>
       <c r="C377" s="31" t="s">
-        <v>2944</v>
+        <v>2941</v>
       </c>
       <c r="D377" s="29"/>
       <c r="E377" s="29" t="s">
@@ -20235,7 +20235,7 @@
         <v>1504</v>
       </c>
       <c r="C386" s="31" t="s">
-        <v>2945</v>
+        <v>2942</v>
       </c>
       <c r="D386" s="29"/>
       <c r="E386" s="29" t="s">
@@ -20260,7 +20260,7 @@
         <v>1504</v>
       </c>
       <c r="C387" s="31" t="s">
-        <v>2946</v>
+        <v>2943</v>
       </c>
       <c r="D387" s="29"/>
       <c r="E387" s="29" t="s">
@@ -20285,7 +20285,7 @@
         <v>1504</v>
       </c>
       <c r="C388" s="31" t="s">
-        <v>2947</v>
+        <v>2944</v>
       </c>
       <c r="D388" s="29"/>
       <c r="E388" s="29" t="s">
@@ -20437,7 +20437,7 @@
         <v>1504</v>
       </c>
       <c r="C394" s="31" t="s">
-        <v>2948</v>
+        <v>2945</v>
       </c>
       <c r="D394" s="29"/>
       <c r="E394" s="29" t="s">
@@ -20487,7 +20487,7 @@
         <v>1504</v>
       </c>
       <c r="C396" s="31" t="s">
-        <v>2949</v>
+        <v>2946</v>
       </c>
       <c r="D396" s="29"/>
       <c r="E396" s="29" t="s">
@@ -20616,7 +20616,7 @@
         <v>1504</v>
       </c>
       <c r="C401" s="31" t="s">
-        <v>2950</v>
+        <v>2947</v>
       </c>
       <c r="D401" s="29"/>
       <c r="E401" s="29" t="s">
@@ -20718,7 +20718,7 @@
         <v>1504</v>
       </c>
       <c r="C405" s="31" t="s">
-        <v>2951</v>
+        <v>2948</v>
       </c>
       <c r="D405" s="29"/>
       <c r="E405" s="29" t="s">
@@ -20768,7 +20768,7 @@
         <v>1504</v>
       </c>
       <c r="C407" s="31" t="s">
-        <v>2952</v>
+        <v>2949</v>
       </c>
       <c r="D407" s="29"/>
       <c r="E407" s="29" t="s">
@@ -20818,7 +20818,7 @@
         <v>1504</v>
       </c>
       <c r="C409" s="31" t="s">
-        <v>2953</v>
+        <v>2950</v>
       </c>
       <c r="D409" s="29"/>
       <c r="E409" s="29" t="s">
@@ -20947,7 +20947,7 @@
         <v>1504</v>
       </c>
       <c r="C414" s="31" t="s">
-        <v>2954</v>
+        <v>2951</v>
       </c>
       <c r="D414" s="29"/>
       <c r="E414" s="29" t="s">
@@ -20997,7 +20997,7 @@
         <v>1504</v>
       </c>
       <c r="C416" s="31" t="s">
-        <v>2955</v>
+        <v>2952</v>
       </c>
       <c r="D416" s="29"/>
       <c r="E416" s="29" t="s">
@@ -21628,7 +21628,7 @@
         <v>32</v>
       </c>
       <c r="C441" s="31" t="s">
-        <v>3085</v>
+        <v>3082</v>
       </c>
       <c r="D441" s="29"/>
       <c r="E441" s="29" t="s">
@@ -21653,7 +21653,7 @@
         <v>32</v>
       </c>
       <c r="C442" s="31" t="s">
-        <v>2956</v>
+        <v>2953</v>
       </c>
       <c r="D442" s="29"/>
       <c r="E442" s="29" t="s">
@@ -21928,7 +21928,7 @@
         <v>32</v>
       </c>
       <c r="C453" s="31" t="s">
-        <v>2957</v>
+        <v>2954</v>
       </c>
       <c r="D453" s="29"/>
       <c r="E453" s="29" t="s">
@@ -21980,7 +21980,7 @@
         <v>32</v>
       </c>
       <c r="C455" s="31" t="s">
-        <v>2958</v>
+        <v>2955</v>
       </c>
       <c r="D455" s="29"/>
       <c r="E455" s="29" t="s">
@@ -22530,7 +22530,7 @@
         <v>32</v>
       </c>
       <c r="C477" s="31" t="s">
-        <v>2959</v>
+        <v>2956</v>
       </c>
       <c r="D477" s="29"/>
       <c r="E477" s="29" t="s">
@@ -22661,7 +22661,7 @@
         <v>32</v>
       </c>
       <c r="C482" s="31" t="s">
-        <v>2960</v>
+        <v>2957</v>
       </c>
       <c r="D482" s="29"/>
       <c r="E482" s="29" t="s">
@@ -22686,7 +22686,7 @@
         <v>32</v>
       </c>
       <c r="C483" s="31" t="s">
-        <v>2961</v>
+        <v>2958</v>
       </c>
       <c r="D483" s="29"/>
       <c r="E483" s="29" t="s">
@@ -23188,7 +23188,7 @@
         <v>32</v>
       </c>
       <c r="C503" s="31" t="s">
-        <v>2962</v>
+        <v>2959</v>
       </c>
       <c r="D503" s="29"/>
       <c r="E503" s="29" t="s">
@@ -23415,7 +23415,7 @@
         <v>32</v>
       </c>
       <c r="C512" s="31" t="s">
-        <v>2963</v>
+        <v>2960</v>
       </c>
       <c r="D512" s="29"/>
       <c r="E512" s="29" t="s">
@@ -23442,7 +23442,7 @@
         <v>32</v>
       </c>
       <c r="C513" s="31" t="s">
-        <v>2964</v>
+        <v>2961</v>
       </c>
       <c r="D513" s="29"/>
       <c r="E513" s="29" t="s">
@@ -23771,7 +23771,7 @@
         <v>32</v>
       </c>
       <c r="C526" s="31" t="s">
-        <v>2965</v>
+        <v>2962</v>
       </c>
       <c r="D526" s="29"/>
       <c r="E526" s="29" t="s">
@@ -28858,7 +28858,7 @@
         <v>1522</v>
       </c>
       <c r="C729" s="31" t="s">
-        <v>2966</v>
+        <v>2963</v>
       </c>
       <c r="D729" s="29"/>
       <c r="E729" s="29" t="s">
@@ -28989,7 +28989,7 @@
         <v>1522</v>
       </c>
       <c r="C734" s="31" t="s">
-        <v>2967</v>
+        <v>2964</v>
       </c>
       <c r="D734" s="29"/>
       <c r="E734" s="29" t="s">
@@ -30684,7 +30684,7 @@
         <v>33</v>
       </c>
       <c r="C801" s="31" t="s">
-        <v>2968</v>
+        <v>2965</v>
       </c>
       <c r="D801" s="29"/>
       <c r="E801" s="29" t="s">
@@ -30953,7 +30953,7 @@
       </c>
       <c r="I811" s="31"/>
     </row>
-    <row r="812" spans="1:9" ht="60">
+    <row r="812" spans="1:9" ht="75">
       <c r="A812" s="29" t="s">
         <v>835</v>
       </c>
@@ -30961,7 +30961,7 @@
         <v>33</v>
       </c>
       <c r="C812" s="31" t="s">
-        <v>2969</v>
+        <v>2966</v>
       </c>
       <c r="D812" s="29"/>
       <c r="E812" s="29" t="s">
@@ -30977,7 +30977,7 @@
         <v>17</v>
       </c>
       <c r="I812" s="31" t="s">
-        <v>2902</v>
+        <v>3087</v>
       </c>
     </row>
     <row r="813" spans="1:9" ht="30">
@@ -31013,7 +31013,7 @@
         <v>33</v>
       </c>
       <c r="C814" s="31" t="s">
-        <v>2970</v>
+        <v>2967</v>
       </c>
       <c r="D814" s="29"/>
       <c r="E814" s="29" t="s">
@@ -31029,7 +31029,7 @@
         <v>17</v>
       </c>
       <c r="I814" s="31" t="s">
-        <v>2903</v>
+        <v>2902</v>
       </c>
     </row>
     <row r="815" spans="1:9">
@@ -31181,7 +31181,7 @@
         <v>17</v>
       </c>
       <c r="I820" s="31" t="s">
-        <v>2904</v>
+        <v>2903</v>
       </c>
     </row>
     <row r="821" spans="1:9" ht="30">
@@ -31236,7 +31236,7 @@
       </c>
       <c r="I822" s="31"/>
     </row>
-    <row r="823" spans="1:9" ht="60">
+    <row r="823" spans="1:9" ht="75">
       <c r="A823" s="29" t="s">
         <v>846</v>
       </c>
@@ -31244,7 +31244,7 @@
         <v>33</v>
       </c>
       <c r="C823" s="31" t="s">
-        <v>2971</v>
+        <v>2968</v>
       </c>
       <c r="D823" s="29"/>
       <c r="E823" s="29" t="s">
@@ -31260,7 +31260,7 @@
         <v>17</v>
       </c>
       <c r="I823" s="31" t="s">
-        <v>2905</v>
+        <v>3088</v>
       </c>
     </row>
     <row r="824" spans="1:9" ht="45">
@@ -31571,7 +31571,7 @@
         <v>33</v>
       </c>
       <c r="C836" s="31" t="s">
-        <v>2972</v>
+        <v>2969</v>
       </c>
       <c r="D836" s="29"/>
       <c r="E836" s="29" t="s">
@@ -31587,7 +31587,7 @@
         <v>17</v>
       </c>
       <c r="I836" s="31" t="s">
-        <v>2938</v>
+        <v>2935</v>
       </c>
     </row>
     <row r="837" spans="1:9">
@@ -31623,7 +31623,7 @@
         <v>33</v>
       </c>
       <c r="C838" s="31" t="s">
-        <v>2973</v>
+        <v>2970</v>
       </c>
       <c r="D838" s="29"/>
       <c r="E838" s="29" t="s">
@@ -31639,7 +31639,7 @@
         <v>17</v>
       </c>
       <c r="I838" s="31" t="s">
-        <v>2906</v>
+        <v>2904</v>
       </c>
     </row>
     <row r="839" spans="1:9" ht="30">
@@ -31691,7 +31691,7 @@
         <v>17</v>
       </c>
       <c r="I840" s="31" t="s">
-        <v>2907</v>
+        <v>2905</v>
       </c>
     </row>
     <row r="841" spans="1:9" ht="30">
@@ -32095,7 +32095,7 @@
         <v>17</v>
       </c>
       <c r="I856" s="31" t="s">
-        <v>2908</v>
+        <v>2906</v>
       </c>
     </row>
     <row r="857" spans="1:9" ht="60">
@@ -32172,7 +32172,7 @@
         <v>17</v>
       </c>
       <c r="I859" s="31" t="s">
-        <v>2908</v>
+        <v>2906</v>
       </c>
     </row>
     <row r="860" spans="1:9" ht="30">
@@ -32424,7 +32424,7 @@
         <v>17</v>
       </c>
       <c r="I869" s="31" t="s">
-        <v>2909</v>
+        <v>2907</v>
       </c>
     </row>
     <row r="870" spans="1:9" ht="45">
@@ -32451,7 +32451,7 @@
         <v>17</v>
       </c>
       <c r="I870" s="31" t="s">
-        <v>2910</v>
+        <v>2908</v>
       </c>
     </row>
     <row r="871" spans="1:9" ht="45">
@@ -33103,7 +33103,7 @@
         <v>17</v>
       </c>
       <c r="I896" s="31" t="s">
-        <v>2911</v>
+        <v>2909</v>
       </c>
     </row>
     <row r="897" spans="1:9" ht="45">
@@ -33155,7 +33155,7 @@
         <v>17</v>
       </c>
       <c r="I898" s="31" t="s">
-        <v>2910</v>
+        <v>2908</v>
       </c>
     </row>
     <row r="899" spans="1:9" ht="30">
@@ -33216,7 +33216,7 @@
         <v>1532</v>
       </c>
       <c r="C901" s="31" t="s">
-        <v>2974</v>
+        <v>2971</v>
       </c>
       <c r="D901" s="29"/>
       <c r="E901" s="29" t="s">
@@ -33307,7 +33307,7 @@
         <v>17</v>
       </c>
       <c r="I904" s="31" t="s">
-        <v>2912</v>
+        <v>2910</v>
       </c>
     </row>
     <row r="905" spans="1:9" ht="60">
@@ -33334,7 +33334,7 @@
         <v>17</v>
       </c>
       <c r="I905" s="31" t="s">
-        <v>2912</v>
+        <v>2910</v>
       </c>
     </row>
     <row r="906" spans="1:9" ht="30">
@@ -33786,7 +33786,7 @@
         <v>17</v>
       </c>
       <c r="I923" s="31" t="s">
-        <v>2913</v>
+        <v>2911</v>
       </c>
     </row>
     <row r="924" spans="1:9" ht="45">
@@ -33797,7 +33797,7 @@
         <v>1535</v>
       </c>
       <c r="C924" s="31" t="s">
-        <v>2975</v>
+        <v>2972</v>
       </c>
       <c r="D924" s="29"/>
       <c r="E924" s="29" t="s">
@@ -33813,7 +33813,7 @@
         <v>17</v>
       </c>
       <c r="I924" s="31" t="s">
-        <v>2914</v>
+        <v>2912</v>
       </c>
     </row>
     <row r="925" spans="1:9" ht="45">
@@ -33990,7 +33990,7 @@
         <v>17</v>
       </c>
       <c r="I931" s="31" t="s">
-        <v>2915</v>
+        <v>2913</v>
       </c>
     </row>
     <row r="932" spans="1:9" ht="30">
@@ -34539,7 +34539,7 @@
         <v>17</v>
       </c>
       <c r="I952" s="31" t="s">
-        <v>2916</v>
+        <v>2914</v>
       </c>
     </row>
     <row r="953" spans="1:9" ht="30">
@@ -34975,7 +34975,7 @@
         <v>1538</v>
       </c>
       <c r="C970" s="31" t="s">
-        <v>2976</v>
+        <v>2973</v>
       </c>
       <c r="D970" s="29"/>
       <c r="E970" s="29" t="s">
@@ -34991,7 +34991,7 @@
         <v>17</v>
       </c>
       <c r="I970" s="31" t="s">
-        <v>2917</v>
+        <v>2915</v>
       </c>
     </row>
     <row r="971" spans="1:9" ht="60">
@@ -35018,7 +35018,7 @@
         <v>17</v>
       </c>
       <c r="I971" s="31" t="s">
-        <v>2918</v>
+        <v>2916</v>
       </c>
     </row>
     <row r="972" spans="1:9" ht="30">
@@ -35071,7 +35071,7 @@
       </c>
       <c r="I973" s="31"/>
     </row>
-    <row r="974" spans="1:9" ht="45">
+    <row r="974" spans="1:9" ht="60">
       <c r="A974" s="29" t="s">
         <v>997</v>
       </c>
@@ -35079,7 +35079,7 @@
         <v>1539</v>
       </c>
       <c r="C974" s="31" t="s">
-        <v>2977</v>
+        <v>2974</v>
       </c>
       <c r="D974" s="29"/>
       <c r="E974" s="29" t="s">
@@ -35095,7 +35095,7 @@
         <v>17</v>
       </c>
       <c r="I974" s="31" t="s">
-        <v>2936</v>
+        <v>3089</v>
       </c>
     </row>
     <row r="975" spans="1:9" ht="30">
@@ -35224,7 +35224,7 @@
         <v>17</v>
       </c>
       <c r="I979" s="31" t="s">
-        <v>2919</v>
+        <v>2917</v>
       </c>
     </row>
     <row r="980" spans="1:9" ht="30">
@@ -35326,7 +35326,7 @@
         <v>17</v>
       </c>
       <c r="I983" s="31" t="s">
-        <v>2920</v>
+        <v>2918</v>
       </c>
     </row>
     <row r="984" spans="1:9" ht="30">
@@ -36987,7 +36987,7 @@
         <v>1552</v>
       </c>
       <c r="C1050" s="31" t="s">
-        <v>2978</v>
+        <v>2975</v>
       </c>
       <c r="D1050" s="29"/>
       <c r="E1050" s="29" t="s">
@@ -37062,7 +37062,7 @@
         <v>1553</v>
       </c>
       <c r="C1053" s="31" t="s">
-        <v>2979</v>
+        <v>2976</v>
       </c>
       <c r="D1053" s="29"/>
       <c r="E1053" s="29" t="s">
@@ -37337,7 +37337,7 @@
         <v>1553</v>
       </c>
       <c r="C1064" s="31" t="s">
-        <v>2980</v>
+        <v>2977</v>
       </c>
       <c r="D1064" s="29"/>
       <c r="E1064" s="29" t="s">
@@ -37387,7 +37387,7 @@
         <v>1553</v>
       </c>
       <c r="C1066" s="31" t="s">
-        <v>2981</v>
+        <v>2978</v>
       </c>
       <c r="D1066" s="29"/>
       <c r="E1066" s="29" t="s">
@@ -38012,7 +38012,7 @@
         <v>1553</v>
       </c>
       <c r="C1091" s="31" t="s">
-        <v>2982</v>
+        <v>2979</v>
       </c>
       <c r="D1091" s="29"/>
       <c r="E1091" s="29" t="s">
@@ -38103,7 +38103,7 @@
         <v>17</v>
       </c>
       <c r="I1094" s="31" t="s">
-        <v>2921</v>
+        <v>2919</v>
       </c>
     </row>
     <row r="1095" spans="1:9" ht="30">
@@ -38364,7 +38364,7 @@
         <v>1553</v>
       </c>
       <c r="C1105" s="31" t="s">
-        <v>2983</v>
+        <v>2980</v>
       </c>
       <c r="D1105" s="29"/>
       <c r="E1105" s="29" t="s">
@@ -38557,7 +38557,7 @@
         <v>17</v>
       </c>
       <c r="I1112" s="31" t="s">
-        <v>2922</v>
+        <v>2920</v>
       </c>
     </row>
     <row r="1113" spans="1:9" ht="45">
@@ -38609,7 +38609,7 @@
         <v>17</v>
       </c>
       <c r="I1114" s="31" t="s">
-        <v>2923</v>
+        <v>2921</v>
       </c>
     </row>
     <row r="1115" spans="1:9" ht="195">
@@ -38636,7 +38636,7 @@
         <v>17</v>
       </c>
       <c r="I1115" s="31" t="s">
-        <v>2924</v>
+        <v>2922</v>
       </c>
     </row>
     <row r="1116" spans="1:9" ht="30">
@@ -39049,7 +39049,7 @@
         <v>1556</v>
       </c>
       <c r="C1132" s="31" t="s">
-        <v>2984</v>
+        <v>2981</v>
       </c>
       <c r="D1132" s="29"/>
       <c r="E1132" s="29" t="s">
@@ -39449,7 +39449,7 @@
         <v>1556</v>
       </c>
       <c r="C1148" s="31" t="s">
-        <v>2985</v>
+        <v>2982</v>
       </c>
       <c r="D1148" s="29"/>
       <c r="E1148" s="29" t="s">
@@ -39774,7 +39774,7 @@
         <v>1560</v>
       </c>
       <c r="C1161" s="31" t="s">
-        <v>2986</v>
+        <v>2983</v>
       </c>
       <c r="D1161" s="29"/>
       <c r="E1161" s="29" t="s">
@@ -39999,7 +39999,7 @@
         <v>1560</v>
       </c>
       <c r="C1170" s="31" t="s">
-        <v>2987</v>
+        <v>2984</v>
       </c>
       <c r="D1170" s="29"/>
       <c r="E1170" s="29" t="s">
@@ -40012,7 +40012,7 @@
         <v>15</v>
       </c>
       <c r="H1170" s="29" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I1170" s="31"/>
     </row>
@@ -40024,7 +40024,7 @@
         <v>1560</v>
       </c>
       <c r="C1171" s="31" t="s">
-        <v>3086</v>
+        <v>3083</v>
       </c>
       <c r="D1171" s="29" t="s">
         <v>2836</v>
@@ -40119,7 +40119,7 @@
         <v>17</v>
       </c>
       <c r="I1174" s="31" t="s">
-        <v>2925</v>
+        <v>2923</v>
       </c>
     </row>
     <row r="1175" spans="1:9" ht="30">
@@ -40548,7 +40548,7 @@
         <v>17</v>
       </c>
       <c r="I1191" s="31" t="s">
-        <v>2922</v>
+        <v>2920</v>
       </c>
     </row>
     <row r="1192" spans="1:9" ht="45">
@@ -40600,7 +40600,7 @@
         <v>17</v>
       </c>
       <c r="I1193" s="31" t="s">
-        <v>2913</v>
+        <v>2911</v>
       </c>
     </row>
     <row r="1194" spans="1:9" ht="60">
@@ -40627,7 +40627,7 @@
         <v>17</v>
       </c>
       <c r="I1194" s="31" t="s">
-        <v>2913</v>
+        <v>2911</v>
       </c>
     </row>
     <row r="1195" spans="1:9" ht="30">
@@ -42413,7 +42413,7 @@
         <v>1569</v>
       </c>
       <c r="C1266" s="31" t="s">
-        <v>2988</v>
+        <v>2985</v>
       </c>
       <c r="D1266" s="29"/>
       <c r="E1266" s="29" t="s">
@@ -42704,7 +42704,7 @@
         <v>17</v>
       </c>
       <c r="I1277" s="31" t="s">
-        <v>2926</v>
+        <v>2924</v>
       </c>
     </row>
     <row r="1278" spans="1:9" ht="30">
@@ -42890,7 +42890,7 @@
         <v>1572</v>
       </c>
       <c r="C1285" s="31" t="s">
-        <v>2989</v>
+        <v>2986</v>
       </c>
       <c r="D1285" s="29"/>
       <c r="E1285" s="29" t="s">
@@ -43065,7 +43065,7 @@
         <v>1573</v>
       </c>
       <c r="C1292" s="31" t="s">
-        <v>2990</v>
+        <v>2987</v>
       </c>
       <c r="D1292" s="29"/>
       <c r="E1292" s="29" t="s">
@@ -43081,7 +43081,7 @@
         <v>17</v>
       </c>
       <c r="I1292" s="31" t="s">
-        <v>2927</v>
+        <v>2925</v>
       </c>
     </row>
     <row r="1293" spans="1:9" ht="45">
@@ -43108,7 +43108,7 @@
         <v>17</v>
       </c>
       <c r="I1293" s="31" t="s">
-        <v>2928</v>
+        <v>2926</v>
       </c>
     </row>
     <row r="1294" spans="1:9" ht="45">
@@ -43194,7 +43194,7 @@
         <v>1574</v>
       </c>
       <c r="C1297" s="31" t="s">
-        <v>2991</v>
+        <v>2988</v>
       </c>
       <c r="D1297" s="29"/>
       <c r="E1297" s="29" t="s">
@@ -43210,7 +43210,7 @@
         <v>17</v>
       </c>
       <c r="I1297" s="31" t="s">
-        <v>2929</v>
+        <v>2927</v>
       </c>
     </row>
     <row r="1298" spans="1:9" ht="30">
@@ -43287,7 +43287,7 @@
         <v>17</v>
       </c>
       <c r="I1300" s="31" t="s">
-        <v>2930</v>
+        <v>2928</v>
       </c>
     </row>
     <row r="1301" spans="1:9" ht="30">
@@ -43614,7 +43614,7 @@
         <v>17</v>
       </c>
       <c r="I1313" s="31" t="s">
-        <v>2931</v>
+        <v>2929</v>
       </c>
     </row>
     <row r="1314" spans="1:9" ht="60">
@@ -43750,7 +43750,7 @@
         <v>1574</v>
       </c>
       <c r="C1319" s="31" t="s">
-        <v>2992</v>
+        <v>2989</v>
       </c>
       <c r="D1319" s="29"/>
       <c r="E1319" s="29" t="s">
@@ -44000,7 +44000,7 @@
         <v>1577</v>
       </c>
       <c r="C1329" s="31" t="s">
-        <v>2993</v>
+        <v>2990</v>
       </c>
       <c r="D1329" s="29"/>
       <c r="E1329" s="29" t="s">
@@ -44143,7 +44143,7 @@
         <v>21</v>
       </c>
       <c r="I1334" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1335" spans="1:9" ht="30">
@@ -44154,7 +44154,7 @@
         <v>1578</v>
       </c>
       <c r="C1335" s="31" t="s">
-        <v>2994</v>
+        <v>2991</v>
       </c>
       <c r="D1335" s="29" t="s">
         <v>2837</v>
@@ -44199,7 +44199,7 @@
         <v>21</v>
       </c>
       <c r="I1336" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1337" spans="1:9" ht="45">
@@ -44228,7 +44228,7 @@
         <v>21</v>
       </c>
       <c r="I1337" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1338" spans="1:9" ht="45">
@@ -44239,7 +44239,7 @@
         <v>1578</v>
       </c>
       <c r="C1338" s="31" t="s">
-        <v>2995</v>
+        <v>2992</v>
       </c>
       <c r="D1338" s="29" t="s">
         <v>2838</v>
@@ -44257,7 +44257,7 @@
         <v>21</v>
       </c>
       <c r="I1338" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1339" spans="1:9" ht="60">
@@ -44268,7 +44268,7 @@
         <v>1578</v>
       </c>
       <c r="C1339" s="31" t="s">
-        <v>3017</v>
+        <v>3014</v>
       </c>
       <c r="D1339" s="29"/>
       <c r="E1339" s="29" t="s">
@@ -44293,7 +44293,7 @@
         <v>1578</v>
       </c>
       <c r="C1340" s="31" t="s">
-        <v>2996</v>
+        <v>2993</v>
       </c>
       <c r="D1340" s="29"/>
       <c r="E1340" s="29" t="s">
@@ -44318,7 +44318,7 @@
         <v>1578</v>
       </c>
       <c r="C1341" s="31" t="s">
-        <v>3019</v>
+        <v>3016</v>
       </c>
       <c r="D1341" s="29"/>
       <c r="E1341" s="29" t="s">
@@ -44343,7 +44343,7 @@
         <v>1578</v>
       </c>
       <c r="C1342" s="31" t="s">
-        <v>3018</v>
+        <v>3015</v>
       </c>
       <c r="D1342" s="29"/>
       <c r="E1342" s="29" t="s">
@@ -44368,7 +44368,7 @@
         <v>1578</v>
       </c>
       <c r="C1343" s="31" t="s">
-        <v>3020</v>
+        <v>3017</v>
       </c>
       <c r="D1343" s="29"/>
       <c r="E1343" s="29" t="s">
@@ -44420,7 +44420,7 @@
         <v>7</v>
       </c>
       <c r="C1345" s="31" t="s">
-        <v>2997</v>
+        <v>2994</v>
       </c>
       <c r="D1345" s="29" t="s">
         <v>2839</v>
@@ -44462,10 +44462,10 @@
         <v>15</v>
       </c>
       <c r="H1346" s="29" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I1346" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1347" spans="1:9" ht="30">
@@ -44476,7 +44476,7 @@
         <v>1578</v>
       </c>
       <c r="C1347" s="31" t="s">
-        <v>2998</v>
+        <v>2995</v>
       </c>
       <c r="D1347" s="29"/>
       <c r="E1347" s="29" t="s">
@@ -44495,13 +44495,13 @@
     </row>
     <row r="1348" spans="1:9" ht="60">
       <c r="A1348" s="29" t="s">
-        <v>3089</v>
+        <v>3086</v>
       </c>
       <c r="B1348" s="30" t="s">
         <v>1578</v>
       </c>
       <c r="C1348" s="31" t="s">
-        <v>3021</v>
+        <v>3018</v>
       </c>
       <c r="D1348" s="29"/>
       <c r="E1348" s="29" t="s">
@@ -44544,7 +44544,7 @@
         <v>20</v>
       </c>
       <c r="I1349" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1350" spans="1:9" ht="45">
@@ -44573,7 +44573,7 @@
         <v>20</v>
       </c>
       <c r="I1350" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1351" spans="1:9" ht="45">
@@ -44602,7 +44602,7 @@
         <v>20</v>
       </c>
       <c r="I1351" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1352" spans="1:9" ht="45">
@@ -44640,7 +44640,7 @@
         <v>1578</v>
       </c>
       <c r="C1353" s="31" t="s">
-        <v>3022</v>
+        <v>3019</v>
       </c>
       <c r="D1353" s="29"/>
       <c r="E1353" s="29" t="s">
@@ -44683,7 +44683,7 @@
         <v>20</v>
       </c>
       <c r="I1354" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1355" spans="1:9" ht="45">
@@ -44694,7 +44694,7 @@
         <v>1578</v>
       </c>
       <c r="C1355" s="31" t="s">
-        <v>3023</v>
+        <v>3020</v>
       </c>
       <c r="D1355" s="29"/>
       <c r="E1355" s="29" t="s">
@@ -44737,7 +44737,7 @@
         <v>20</v>
       </c>
       <c r="I1356" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1357" spans="1:9" ht="45">
@@ -44748,7 +44748,7 @@
         <v>1578</v>
       </c>
       <c r="C1357" s="31" t="s">
-        <v>3024</v>
+        <v>3021</v>
       </c>
       <c r="D1357" s="29" t="s">
         <v>2841</v>
@@ -44775,7 +44775,7 @@
         <v>1578</v>
       </c>
       <c r="C1358" s="31" t="s">
-        <v>3025</v>
+        <v>3022</v>
       </c>
       <c r="D1358" s="29" t="s">
         <v>2842</v>
@@ -44820,7 +44820,7 @@
         <v>20</v>
       </c>
       <c r="I1359" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1360" spans="1:9" ht="60">
@@ -44831,7 +44831,7 @@
         <v>1578</v>
       </c>
       <c r="C1360" s="31" t="s">
-        <v>2999</v>
+        <v>2996</v>
       </c>
       <c r="D1360" s="29" t="s">
         <v>2842</v>
@@ -44858,7 +44858,7 @@
         <v>1578</v>
       </c>
       <c r="C1361" s="31" t="s">
-        <v>3026</v>
+        <v>3023</v>
       </c>
       <c r="D1361" s="29" t="s">
         <v>2842</v>
@@ -44876,7 +44876,7 @@
         <v>20</v>
       </c>
       <c r="I1361" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1362" spans="1:9" ht="60">
@@ -44887,7 +44887,7 @@
         <v>1578</v>
       </c>
       <c r="C1362" s="31" t="s">
-        <v>3027</v>
+        <v>3024</v>
       </c>
       <c r="D1362" s="29"/>
       <c r="E1362" s="29" t="s">
@@ -44912,7 +44912,7 @@
         <v>1578</v>
       </c>
       <c r="C1363" s="31" t="s">
-        <v>3028</v>
+        <v>3025</v>
       </c>
       <c r="D1363" s="29" t="s">
         <v>2843</v>
@@ -44957,7 +44957,7 @@
         <v>20</v>
       </c>
       <c r="I1364" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1365" spans="1:9" ht="45">
@@ -44968,7 +44968,7 @@
         <v>1578</v>
       </c>
       <c r="C1365" s="31" t="s">
-        <v>3029</v>
+        <v>3026</v>
       </c>
       <c r="D1365" s="29" t="s">
         <v>2844</v>
@@ -45013,7 +45013,7 @@
         <v>20</v>
       </c>
       <c r="I1366" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1367" spans="1:9" ht="90">
@@ -45024,7 +45024,7 @@
         <v>1578</v>
       </c>
       <c r="C1367" s="31" t="s">
-        <v>3000</v>
+        <v>2997</v>
       </c>
       <c r="D1367" s="29" t="s">
         <v>2844</v>
@@ -45042,7 +45042,7 @@
         <v>20</v>
       </c>
       <c r="I1367" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1368" spans="1:9" ht="60">
@@ -45053,7 +45053,7 @@
         <v>1578</v>
       </c>
       <c r="C1368" s="31" t="s">
-        <v>3001</v>
+        <v>2998</v>
       </c>
       <c r="D1368" s="29" t="s">
         <v>2844</v>
@@ -45080,7 +45080,7 @@
         <v>1578</v>
       </c>
       <c r="C1369" s="31" t="s">
-        <v>3002</v>
+        <v>2999</v>
       </c>
       <c r="D1369" s="29" t="s">
         <v>2845</v>
@@ -45095,10 +45095,10 @@
         <v>15</v>
       </c>
       <c r="H1369" s="29" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I1369" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1370" spans="1:9" ht="45">
@@ -45127,7 +45127,7 @@
         <v>20</v>
       </c>
       <c r="I1370" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1371" spans="1:9" ht="60">
@@ -45138,7 +45138,7 @@
         <v>1578</v>
       </c>
       <c r="C1371" s="31" t="s">
-        <v>3003</v>
+        <v>3000</v>
       </c>
       <c r="D1371" s="29"/>
       <c r="E1371" s="29" t="s">
@@ -45163,7 +45163,7 @@
         <v>1578</v>
       </c>
       <c r="C1372" s="31" t="s">
-        <v>3004</v>
+        <v>3001</v>
       </c>
       <c r="D1372" s="29" t="s">
         <v>2846</v>
@@ -45181,7 +45181,7 @@
         <v>20</v>
       </c>
       <c r="I1372" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1373" spans="1:9" ht="45">
@@ -45210,7 +45210,7 @@
         <v>20</v>
       </c>
       <c r="I1373" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1374" spans="1:9" ht="45">
@@ -45221,7 +45221,7 @@
         <v>1578</v>
       </c>
       <c r="C1374" s="31" t="s">
-        <v>3005</v>
+        <v>3002</v>
       </c>
       <c r="D1374" s="29" t="s">
         <v>2847</v>
@@ -45239,7 +45239,7 @@
         <v>20</v>
       </c>
       <c r="I1374" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1375" spans="1:9" ht="45">
@@ -45250,7 +45250,7 @@
         <v>1578</v>
       </c>
       <c r="C1375" s="31" t="s">
-        <v>3006</v>
+        <v>3003</v>
       </c>
       <c r="D1375" s="29"/>
       <c r="E1375" s="29" t="s">
@@ -45275,7 +45275,7 @@
         <v>1578</v>
       </c>
       <c r="C1376" s="31" t="s">
-        <v>3007</v>
+        <v>3004</v>
       </c>
       <c r="D1376" s="29" t="s">
         <v>2847</v>
@@ -45293,7 +45293,7 @@
         <v>20</v>
       </c>
       <c r="I1376" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1377" spans="1:9" ht="45">
@@ -45304,7 +45304,7 @@
         <v>1578</v>
       </c>
       <c r="C1377" s="31" t="s">
-        <v>3030</v>
+        <v>3027</v>
       </c>
       <c r="D1377" s="29" t="s">
         <v>2848</v>
@@ -45322,7 +45322,7 @@
         <v>21</v>
       </c>
       <c r="I1377" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1378" spans="1:9" ht="45">
@@ -45351,7 +45351,7 @@
         <v>21</v>
       </c>
       <c r="I1378" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1379" spans="1:9" ht="45">
@@ -45380,7 +45380,7 @@
         <v>21</v>
       </c>
       <c r="I1379" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1380" spans="1:9" ht="30">
@@ -45391,7 +45391,7 @@
         <v>1578</v>
       </c>
       <c r="C1380" s="31" t="s">
-        <v>3008</v>
+        <v>3005</v>
       </c>
       <c r="D1380" s="29"/>
       <c r="E1380" s="29" t="s">
@@ -45416,7 +45416,7 @@
         <v>1578</v>
       </c>
       <c r="C1381" s="31" t="s">
-        <v>3009</v>
+        <v>3006</v>
       </c>
       <c r="D1381" s="29"/>
       <c r="E1381" s="29" t="s">
@@ -45441,7 +45441,7 @@
         <v>1578</v>
       </c>
       <c r="C1382" s="31" t="s">
-        <v>3011</v>
+        <v>3008</v>
       </c>
       <c r="D1382" s="29" t="s">
         <v>2850</v>
@@ -45459,7 +45459,7 @@
         <v>21</v>
       </c>
       <c r="I1382" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1383" spans="1:9" ht="45">
@@ -45470,7 +45470,7 @@
         <v>1578</v>
       </c>
       <c r="C1383" s="31" t="s">
-        <v>3010</v>
+        <v>3007</v>
       </c>
       <c r="D1383" s="29" t="s">
         <v>2850</v>
@@ -45488,7 +45488,7 @@
         <v>21</v>
       </c>
       <c r="I1383" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1384" spans="1:9" ht="60">
@@ -45499,7 +45499,7 @@
         <v>1578</v>
       </c>
       <c r="C1384" s="31" t="s">
-        <v>3012</v>
+        <v>3009</v>
       </c>
       <c r="D1384" s="29" t="s">
         <v>2851</v>
@@ -45517,18 +45517,18 @@
         <v>20</v>
       </c>
       <c r="I1384" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1385" spans="1:9" ht="75">
       <c r="A1385" s="29" t="s">
-        <v>3013</v>
+        <v>3010</v>
       </c>
       <c r="B1385" s="33">
         <v>7</v>
       </c>
       <c r="C1385" s="31" t="s">
-        <v>3014</v>
+        <v>3011</v>
       </c>
       <c r="D1385" s="29" t="s">
         <v>2851</v>
@@ -45546,7 +45546,7 @@
         <v>20</v>
       </c>
       <c r="I1385" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1386" spans="1:9" ht="60">
@@ -45557,7 +45557,7 @@
         <v>1578</v>
       </c>
       <c r="C1386" s="31" t="s">
-        <v>3088</v>
+        <v>3085</v>
       </c>
       <c r="D1386" s="29" t="s">
         <v>2851</v>
@@ -45575,7 +45575,7 @@
         <v>20</v>
       </c>
       <c r="I1386" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1387" spans="1:9" ht="60">
@@ -45586,7 +45586,7 @@
         <v>1578</v>
       </c>
       <c r="C1387" s="31" t="s">
-        <v>3015</v>
+        <v>3012</v>
       </c>
       <c r="D1387" s="29" t="s">
         <v>2852</v>
@@ -45604,7 +45604,7 @@
         <v>20</v>
       </c>
       <c r="I1387" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1388" spans="1:9" ht="45">
@@ -45615,7 +45615,7 @@
         <v>1578</v>
       </c>
       <c r="C1388" s="31" t="s">
-        <v>2937</v>
+        <v>2934</v>
       </c>
       <c r="D1388" s="29" t="s">
         <v>2852</v>
@@ -45633,7 +45633,7 @@
         <v>20</v>
       </c>
       <c r="I1388" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1389" spans="1:9" ht="45">
@@ -45644,7 +45644,7 @@
         <v>1578</v>
       </c>
       <c r="C1389" s="31" t="s">
-        <v>3016</v>
+        <v>3013</v>
       </c>
       <c r="D1389" s="29" t="s">
         <v>2852</v>
@@ -45671,7 +45671,7 @@
         <v>1578</v>
       </c>
       <c r="C1390" s="31" t="s">
-        <v>3087</v>
+        <v>3084</v>
       </c>
       <c r="D1390" s="29" t="s">
         <v>2853</v>
@@ -45689,7 +45689,7 @@
         <v>20</v>
       </c>
       <c r="I1390" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1391" spans="1:9" ht="45">
@@ -45718,18 +45718,18 @@
         <v>20</v>
       </c>
       <c r="I1391" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1392" spans="1:9" ht="45">
       <c r="A1392" s="29" t="s">
-        <v>3031</v>
+        <v>3028</v>
       </c>
       <c r="B1392" s="33">
         <v>7</v>
       </c>
       <c r="C1392" s="31" t="s">
-        <v>3032</v>
+        <v>3029</v>
       </c>
       <c r="D1392" s="29" t="s">
         <v>2853</v>
@@ -45747,7 +45747,7 @@
         <v>20</v>
       </c>
       <c r="I1392" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1393" spans="1:9" ht="45">
@@ -45758,7 +45758,7 @@
         <v>1578</v>
       </c>
       <c r="C1393" s="31" t="s">
-        <v>3033</v>
+        <v>3030</v>
       </c>
       <c r="D1393" s="29" t="s">
         <v>2854</v>
@@ -45773,10 +45773,10 @@
         <v>15</v>
       </c>
       <c r="H1393" s="29" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I1393" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1394" spans="1:9" ht="45">
@@ -45787,7 +45787,7 @@
         <v>1578</v>
       </c>
       <c r="C1394" s="31" t="s">
-        <v>3034</v>
+        <v>3031</v>
       </c>
       <c r="D1394" s="29" t="s">
         <v>2854</v>
@@ -45805,7 +45805,7 @@
         <v>20</v>
       </c>
       <c r="I1394" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1395" spans="1:9" ht="45">
@@ -45816,7 +45816,7 @@
         <v>1578</v>
       </c>
       <c r="C1395" s="31" t="s">
-        <v>3035</v>
+        <v>3032</v>
       </c>
       <c r="D1395" s="29" t="s">
         <v>2854</v>
@@ -45834,7 +45834,7 @@
         <v>20</v>
       </c>
       <c r="I1395" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1396" spans="1:9" ht="45">
@@ -45845,7 +45845,7 @@
         <v>1578</v>
       </c>
       <c r="C1396" s="31" t="s">
-        <v>3036</v>
+        <v>3033</v>
       </c>
       <c r="D1396" s="29" t="s">
         <v>2855</v>
@@ -45863,7 +45863,7 @@
         <v>21</v>
       </c>
       <c r="I1396" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1397" spans="1:9" ht="45">
@@ -45874,7 +45874,7 @@
         <v>1578</v>
       </c>
       <c r="C1397" s="31" t="s">
-        <v>3037</v>
+        <v>3034</v>
       </c>
       <c r="D1397" s="29" t="s">
         <v>2855</v>
@@ -45892,7 +45892,7 @@
         <v>21</v>
       </c>
       <c r="I1397" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1398" spans="1:9" ht="45">
@@ -45921,7 +45921,7 @@
         <v>20</v>
       </c>
       <c r="I1398" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1399" spans="1:9" ht="45">
@@ -45932,7 +45932,7 @@
         <v>1578</v>
       </c>
       <c r="C1399" s="31" t="s">
-        <v>3038</v>
+        <v>3035</v>
       </c>
       <c r="D1399" s="29" t="s">
         <v>2856</v>
@@ -45950,7 +45950,7 @@
         <v>20</v>
       </c>
       <c r="I1399" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1400" spans="1:9" ht="60">
@@ -45961,7 +45961,7 @@
         <v>1578</v>
       </c>
       <c r="C1400" s="31" t="s">
-        <v>3039</v>
+        <v>3036</v>
       </c>
       <c r="D1400" s="29" t="s">
         <v>2857</v>
@@ -45979,7 +45979,7 @@
         <v>20</v>
       </c>
       <c r="I1400" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1401" spans="1:9" ht="45">
@@ -46008,7 +46008,7 @@
         <v>20</v>
       </c>
       <c r="I1401" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1402" spans="1:9" ht="45">
@@ -46019,7 +46019,7 @@
         <v>1578</v>
       </c>
       <c r="C1402" s="31" t="s">
-        <v>3040</v>
+        <v>3037</v>
       </c>
       <c r="D1402" s="29" t="s">
         <v>2858</v>
@@ -46037,7 +46037,7 @@
         <v>17</v>
       </c>
       <c r="I1402" s="31" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1403" spans="1:9" ht="45">
@@ -46048,7 +46048,7 @@
         <v>1578</v>
       </c>
       <c r="C1403" s="31" t="s">
-        <v>3041</v>
+        <v>3038</v>
       </c>
       <c r="D1403" s="29" t="s">
         <v>2858</v>
@@ -46075,7 +46075,7 @@
         <v>1578</v>
       </c>
       <c r="C1404" s="31" t="s">
-        <v>3042</v>
+        <v>3039</v>
       </c>
       <c r="D1404" s="29" t="s">
         <v>2858</v>
@@ -46092,9 +46092,7 @@
       <c r="H1404" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I1404" s="31" t="s">
-        <v>2932</v>
-      </c>
+      <c r="I1404" s="31"/>
     </row>
     <row r="1405" spans="1:9" ht="60">
       <c r="A1405" s="29" t="s">
@@ -46104,7 +46102,7 @@
         <v>1578</v>
       </c>
       <c r="C1405" s="31" t="s">
-        <v>3043</v>
+        <v>3040</v>
       </c>
       <c r="D1405" s="29" t="s">
         <v>2858</v>
@@ -46122,7 +46120,7 @@
         <v>20</v>
       </c>
       <c r="I1405" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1406" spans="1:9" ht="45">
@@ -46133,7 +46131,7 @@
         <v>1578</v>
       </c>
       <c r="C1406" s="31" t="s">
-        <v>3044</v>
+        <v>3041</v>
       </c>
       <c r="D1406" s="29"/>
       <c r="E1406" s="29" t="s">
@@ -46158,7 +46156,7 @@
         <v>1578</v>
       </c>
       <c r="C1407" s="31" t="s">
-        <v>3045</v>
+        <v>3042</v>
       </c>
       <c r="D1407" s="29"/>
       <c r="E1407" s="29" t="s">
@@ -46183,7 +46181,7 @@
         <v>1578</v>
       </c>
       <c r="C1408" s="31" t="s">
-        <v>3046</v>
+        <v>3043</v>
       </c>
       <c r="D1408" s="29"/>
       <c r="E1408" s="29" t="s">
@@ -46208,7 +46206,7 @@
         <v>1578</v>
       </c>
       <c r="C1409" s="31" t="s">
-        <v>3047</v>
+        <v>3044</v>
       </c>
       <c r="D1409" s="29"/>
       <c r="E1409" s="29" t="s">
@@ -46233,7 +46231,7 @@
         <v>1578</v>
       </c>
       <c r="C1410" s="31" t="s">
-        <v>3048</v>
+        <v>3045</v>
       </c>
       <c r="D1410" s="29"/>
       <c r="E1410" s="29" t="s">
@@ -46258,7 +46256,7 @@
         <v>1578</v>
       </c>
       <c r="C1411" s="31" t="s">
-        <v>3049</v>
+        <v>3046</v>
       </c>
       <c r="D1411" s="29"/>
       <c r="E1411" s="29" t="s">
@@ -46283,7 +46281,7 @@
         <v>1578</v>
       </c>
       <c r="C1412" s="31" t="s">
-        <v>3050</v>
+        <v>3047</v>
       </c>
       <c r="D1412" s="29"/>
       <c r="E1412" s="29" t="s">
@@ -46308,7 +46306,7 @@
         <v>1578</v>
       </c>
       <c r="C1413" s="31" t="s">
-        <v>3051</v>
+        <v>3048</v>
       </c>
       <c r="D1413" s="29"/>
       <c r="E1413" s="29" t="s">
@@ -46333,7 +46331,7 @@
         <v>1578</v>
       </c>
       <c r="C1414" s="31" t="s">
-        <v>3052</v>
+        <v>3049</v>
       </c>
       <c r="D1414" s="29"/>
       <c r="E1414" s="29" t="s">
@@ -46358,7 +46356,7 @@
         <v>1578</v>
       </c>
       <c r="C1415" s="31" t="s">
-        <v>3053</v>
+        <v>3050</v>
       </c>
       <c r="D1415" s="29"/>
       <c r="E1415" s="29" t="s">
@@ -46383,7 +46381,7 @@
         <v>1578</v>
       </c>
       <c r="C1416" s="31" t="s">
-        <v>3054</v>
+        <v>3051</v>
       </c>
       <c r="D1416" s="29"/>
       <c r="E1416" s="29" t="s">
@@ -46408,7 +46406,7 @@
         <v>1578</v>
       </c>
       <c r="C1417" s="31" t="s">
-        <v>3055</v>
+        <v>3052</v>
       </c>
       <c r="D1417" s="29"/>
       <c r="E1417" s="29" t="s">
@@ -46433,7 +46431,7 @@
         <v>1578</v>
       </c>
       <c r="C1418" s="31" t="s">
-        <v>3056</v>
+        <v>3053</v>
       </c>
       <c r="D1418" s="29"/>
       <c r="E1418" s="29" t="s">
@@ -46458,7 +46456,7 @@
         <v>1578</v>
       </c>
       <c r="C1419" s="31" t="s">
-        <v>3059</v>
+        <v>3056</v>
       </c>
       <c r="D1419" s="29"/>
       <c r="E1419" s="29" t="s">
@@ -46483,7 +46481,7 @@
         <v>1578</v>
       </c>
       <c r="C1420" s="31" t="s">
-        <v>3057</v>
+        <v>3054</v>
       </c>
       <c r="D1420" s="29"/>
       <c r="E1420" s="29" t="s">
@@ -46508,7 +46506,7 @@
         <v>1578</v>
       </c>
       <c r="C1421" s="31" t="s">
-        <v>3058</v>
+        <v>3055</v>
       </c>
       <c r="D1421" s="29"/>
       <c r="E1421" s="29" t="s">
@@ -46533,7 +46531,7 @@
         <v>1578</v>
       </c>
       <c r="C1422" s="31" t="s">
-        <v>3060</v>
+        <v>3057</v>
       </c>
       <c r="D1422" s="29"/>
       <c r="E1422" s="29" t="s">
@@ -46558,7 +46556,7 @@
         <v>1578</v>
       </c>
       <c r="C1423" s="31" t="s">
-        <v>3061</v>
+        <v>3058</v>
       </c>
       <c r="D1423" s="29"/>
       <c r="E1423" s="29" t="s">
@@ -46583,7 +46581,7 @@
         <v>1578</v>
       </c>
       <c r="C1424" s="31" t="s">
-        <v>3062</v>
+        <v>3059</v>
       </c>
       <c r="D1424" s="29"/>
       <c r="E1424" s="29" t="s">
@@ -46608,7 +46606,7 @@
         <v>1578</v>
       </c>
       <c r="C1425" s="31" t="s">
-        <v>3063</v>
+        <v>3060</v>
       </c>
       <c r="D1425" s="29"/>
       <c r="E1425" s="29" t="s">
@@ -46633,7 +46631,7 @@
         <v>1578</v>
       </c>
       <c r="C1426" s="31" t="s">
-        <v>3064</v>
+        <v>3061</v>
       </c>
       <c r="D1426" s="29"/>
       <c r="E1426" s="29" t="s">
@@ -46658,7 +46656,7 @@
         <v>1578</v>
       </c>
       <c r="C1427" s="31" t="s">
-        <v>3065</v>
+        <v>3062</v>
       </c>
       <c r="D1427" s="29"/>
       <c r="E1427" s="29" t="s">
@@ -46683,7 +46681,7 @@
         <v>1578</v>
       </c>
       <c r="C1428" s="31" t="s">
-        <v>3066</v>
+        <v>3063</v>
       </c>
       <c r="D1428" s="29"/>
       <c r="E1428" s="29" t="s">
@@ -46708,7 +46706,7 @@
         <v>1578</v>
       </c>
       <c r="C1429" s="31" t="s">
-        <v>3067</v>
+        <v>3064</v>
       </c>
       <c r="D1429" s="29"/>
       <c r="E1429" s="29" t="s">
@@ -46733,7 +46731,7 @@
         <v>1578</v>
       </c>
       <c r="C1430" s="31" t="s">
-        <v>3068</v>
+        <v>3065</v>
       </c>
       <c r="D1430" s="29"/>
       <c r="E1430" s="29" t="s">
@@ -46758,7 +46756,7 @@
         <v>1578</v>
       </c>
       <c r="C1431" s="31" t="s">
-        <v>3069</v>
+        <v>3066</v>
       </c>
       <c r="D1431" s="29"/>
       <c r="E1431" s="29" t="s">
@@ -46783,7 +46781,7 @@
         <v>1578</v>
       </c>
       <c r="C1432" s="31" t="s">
-        <v>3070</v>
+        <v>3067</v>
       </c>
       <c r="D1432" s="29"/>
       <c r="E1432" s="29" t="s">
@@ -46808,7 +46806,7 @@
         <v>1578</v>
       </c>
       <c r="C1433" s="31" t="s">
-        <v>3071</v>
+        <v>3068</v>
       </c>
       <c r="D1433" s="29"/>
       <c r="E1433" s="29" t="s">
@@ -46833,7 +46831,7 @@
         <v>1578</v>
       </c>
       <c r="C1434" s="31" t="s">
-        <v>3072</v>
+        <v>3069</v>
       </c>
       <c r="D1434" s="29"/>
       <c r="E1434" s="29" t="s">
@@ -46858,7 +46856,7 @@
         <v>1578</v>
       </c>
       <c r="C1435" s="31" t="s">
-        <v>3073</v>
+        <v>3070</v>
       </c>
       <c r="D1435" s="29"/>
       <c r="E1435" s="29" t="s">
@@ -46883,7 +46881,7 @@
         <v>1578</v>
       </c>
       <c r="C1436" s="31" t="s">
-        <v>3074</v>
+        <v>3071</v>
       </c>
       <c r="D1436" s="29"/>
       <c r="E1436" s="29" t="s">
@@ -46908,7 +46906,7 @@
         <v>1578</v>
       </c>
       <c r="C1437" s="31" t="s">
-        <v>3075</v>
+        <v>3072</v>
       </c>
       <c r="D1437" s="29"/>
       <c r="E1437" s="29" t="s">
@@ -46933,7 +46931,7 @@
         <v>1578</v>
       </c>
       <c r="C1438" s="31" t="s">
-        <v>3076</v>
+        <v>3073</v>
       </c>
       <c r="D1438" s="29"/>
       <c r="E1438" s="29" t="s">
@@ -46958,7 +46956,7 @@
         <v>1578</v>
       </c>
       <c r="C1439" s="31" t="s">
-        <v>3077</v>
+        <v>3074</v>
       </c>
       <c r="D1439" s="29"/>
       <c r="E1439" s="29" t="s">
@@ -46983,7 +46981,7 @@
         <v>1578</v>
       </c>
       <c r="C1440" s="31" t="s">
-        <v>3078</v>
+        <v>3075</v>
       </c>
       <c r="D1440" s="29"/>
       <c r="E1440" s="29" t="s">
@@ -47008,7 +47006,7 @@
         <v>1578</v>
       </c>
       <c r="C1441" s="31" t="s">
-        <v>3079</v>
+        <v>3076</v>
       </c>
       <c r="D1441" s="29" t="s">
         <v>2859</v>
@@ -47026,7 +47024,7 @@
         <v>20</v>
       </c>
       <c r="I1441" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1442" spans="1:9" ht="60">
@@ -47037,7 +47035,7 @@
         <v>1578</v>
       </c>
       <c r="C1442" s="31" t="s">
-        <v>3084</v>
+        <v>3081</v>
       </c>
       <c r="D1442" s="29" t="s">
         <v>2860</v>
@@ -47055,7 +47053,7 @@
         <v>20</v>
       </c>
       <c r="I1442" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1443" spans="1:9" ht="60">
@@ -47066,7 +47064,7 @@
         <v>1578</v>
       </c>
       <c r="C1443" s="31" t="s">
-        <v>3080</v>
+        <v>3077</v>
       </c>
       <c r="D1443" s="29" t="s">
         <v>2860</v>
@@ -47084,7 +47082,7 @@
         <v>20</v>
       </c>
       <c r="I1443" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1444" spans="1:9" ht="45">
@@ -47095,7 +47093,7 @@
         <v>1578</v>
       </c>
       <c r="C1444" s="31" t="s">
-        <v>3081</v>
+        <v>3078</v>
       </c>
       <c r="D1444" s="29"/>
       <c r="E1444" s="29" t="s">
@@ -47111,7 +47109,7 @@
         <v>20</v>
       </c>
       <c r="I1444" s="31" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1445" spans="1:9" ht="30">
@@ -47122,7 +47120,7 @@
         <v>1578</v>
       </c>
       <c r="C1445" s="31" t="s">
-        <v>3082</v>
+        <v>3079</v>
       </c>
       <c r="D1445" s="29"/>
       <c r="E1445" s="29" t="s">
@@ -47147,7 +47145,7 @@
         <v>1578</v>
       </c>
       <c r="C1446" s="31" t="s">
-        <v>3083</v>
+        <v>3080</v>
       </c>
       <c r="D1446" s="29"/>
       <c r="E1446" s="29" t="s">
@@ -47174,11 +47172,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -47186,6 +47179,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:I1446">
@@ -47252,21 +47250,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -47315,10 +47298,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -47338,16 +47343,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MS-OXCRPC]: Fix watchman issue.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCRPC/MS-OXCRPC_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCRPC/MS-OXCRPC_RequirementSpecification.xlsx
@@ -9536,7 +9536,7 @@
     <t>MS-OXCRPC_R1690:i</t>
   </si>
   <si>
-    <t>Verified by derived requirement: MS-OXCRPC_R4886.</t>
+    <t>Verified by derived requirements: MS-OXCRPC_R4885, MS-OXCRPC_R4886.</t>
   </si>
 </sst>
 </file>
@@ -9591,6 +9591,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -9811,6 +9812,21 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -9834,21 +9850,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10756,127 +10757,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -10889,12 +10890,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -10907,12 +10908,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -10925,12 +10926,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -10943,60 +10944,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -40017,7 +40018,7 @@
       <c r="H1170" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="I1170" s="31" t="s">
+      <c r="I1170" s="20" t="s">
         <v>3090</v>
       </c>
     </row>
@@ -47173,11 +47174,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -47185,6 +47181,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:I1446">
@@ -47251,18 +47252,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -47315,14 +47316,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -47332,6 +47325,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
[MS-OXCRPC] Add new test cases for AUX_SERVER_CAPABILITIES.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCRPC/MS-OXCRPC_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCRPC/MS-OXCRPC_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10467" uniqueCount="3152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10468" uniqueCount="3153">
   <si>
     <t>Req ID</t>
   </si>
@@ -9721,11 +9721,14 @@
   <si>
     <t>[In AUX_HEADER Structure] [Type (1 byte)] When the Version field is AUX_VERSION_1 and the type value is "AUX_PROTOCOL_DEVICE_IDENTIFICATION 0x4E", means "AUX_PROTOCOL_DEVICE_IDENTIFICATION " structure will follow the AUX_HEADER.</t>
   </si>
+  <si>
+    <t>Verified by requirement: MS-OXCRPC_R1649011, MS-OXCRPC_R1649012 and MS-OXCRPC_R1649013</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -10049,7 +10052,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="33">
     <dxf>
       <font>
         <b val="0"/>
@@ -10389,6 +10392,36 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.59996337778862885"/>
@@ -10651,7 +10684,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10684,9 +10717,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10719,6 +10769,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -31809,7 +31876,7 @@
         <v>15</v>
       </c>
       <c r="H837" s="34" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I837" s="35"/>
     </row>
@@ -34058,7 +34125,7 @@
       </c>
       <c r="I926" s="35"/>
     </row>
-    <row r="927" spans="1:9" ht="45">
+    <row r="927" spans="1:9" ht="60">
       <c r="A927" s="22" t="s">
         <v>3133</v>
       </c>
@@ -34079,9 +34146,11 @@
         <v>15</v>
       </c>
       <c r="H927" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="I927" s="35"/>
+        <v>17</v>
+      </c>
+      <c r="I927" s="24" t="s">
+        <v>3152</v>
+      </c>
     </row>
     <row r="928" spans="1:9" ht="60">
       <c r="A928" s="22" t="s">
@@ -48109,34 +48178,56 @@
     <mergeCell ref="B17:I17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A20:I1475">
-    <cfRule type="expression" dxfId="26" priority="53">
+  <conditionalFormatting sqref="A20:I926 A928:I1475 A927:H927">
+    <cfRule type="expression" dxfId="32" priority="59">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="54">
+    <cfRule type="expression" dxfId="31" priority="60">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="61">
+    <cfRule type="expression" dxfId="30" priority="67">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:I1475">
-    <cfRule type="expression" dxfId="23" priority="7">
+  <conditionalFormatting sqref="A20:I926 A928:I1475 A927:H927">
+    <cfRule type="expression" dxfId="29" priority="13">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="8">
+    <cfRule type="expression" dxfId="28" priority="14">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="9">
+    <cfRule type="expression" dxfId="27" priority="15">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F1475">
-    <cfRule type="expression" dxfId="20" priority="13">
+    <cfRule type="expression" dxfId="26" priority="19">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="14">
+    <cfRule type="expression" dxfId="25" priority="20">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I927">
+    <cfRule type="expression" dxfId="24" priority="4">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="5">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="6">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I927">
+    <cfRule type="expression" dxfId="21" priority="1">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="2">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="3">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">

</xml_diff>